<commit_message>
#15 two arrow tower and a king tower
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,17 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要经验</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -44,6 +40,22 @@
   </si>
   <si>
     <t>CardExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家升级需要经验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TowerLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家等级对应塔等级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -740,12 +752,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C102" totalsRowShown="0">
-  <autoFilter ref="A1:C102"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:D102" totalsRowShown="0">
+  <autoFilter ref="A1:D102"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Exp"/>
     <tableColumn id="3" name="CardExp"/>
+    <tableColumn id="4" name="TowerLevel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1038,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C102"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1049,18 +1062,21 @@
     <col min="3" max="3" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,19 +1086,25 @@
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1092,8 +1114,11 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1103,8 +1128,11 @@
       <c r="C5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1114,8 +1142,11 @@
       <c r="C6" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1125,8 +1156,11 @@
       <c r="C7" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1136,8 +1170,11 @@
       <c r="C8" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1147,8 +1184,11 @@
       <c r="C9" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1158,8 +1198,11 @@
       <c r="C10" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1170,8 +1213,11 @@
         <f>C10+500</f>
         <v>700</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1179,11 +1225,14 @@
         <v>145</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:C75" si="0">C11+500</f>
+        <f t="shared" ref="C12" si="0">C11+500</f>
         <v>1200</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1193,8 +1242,11 @@
       <c r="C13">
         <v>999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1204,8 +1256,11 @@
       <c r="C14">
         <v>999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1215,8 +1270,11 @@
       <c r="C15">
         <v>999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1226,8 +1284,11 @@
       <c r="C16">
         <v>999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1237,8 +1298,11 @@
       <c r="C17">
         <v>999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1248,8 +1312,11 @@
       <c r="C18">
         <v>999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1259,8 +1326,11 @@
       <c r="C19">
         <v>999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1270,8 +1340,11 @@
       <c r="C20">
         <v>999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1281,8 +1354,11 @@
       <c r="C21">
         <v>999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1292,8 +1368,11 @@
       <c r="C22">
         <v>999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1303,8 +1382,11 @@
       <c r="C23">
         <v>999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1314,8 +1396,11 @@
       <c r="C24">
         <v>999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1325,8 +1410,11 @@
       <c r="C25">
         <v>999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1336,8 +1424,11 @@
       <c r="C26">
         <v>999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1347,8 +1438,11 @@
       <c r="C27">
         <v>999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1358,8 +1452,11 @@
       <c r="C28">
         <v>999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1369,8 +1466,11 @@
       <c r="C29">
         <v>999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1380,8 +1480,11 @@
       <c r="C30">
         <v>999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1391,8 +1494,11 @@
       <c r="C31">
         <v>999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1402,8 +1508,11 @@
       <c r="C32">
         <v>999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1413,8 +1522,11 @@
       <c r="C33">
         <v>999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1424,8 +1536,11 @@
       <c r="C34">
         <v>999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1435,8 +1550,11 @@
       <c r="C35">
         <v>999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1446,8 +1564,11 @@
       <c r="C36">
         <v>999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1457,8 +1578,11 @@
       <c r="C37">
         <v>999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1468,8 +1592,11 @@
       <c r="C38">
         <v>999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1479,8 +1606,11 @@
       <c r="C39">
         <v>999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1490,8 +1620,11 @@
       <c r="C40">
         <v>999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1501,8 +1634,11 @@
       <c r="C41">
         <v>999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1512,8 +1648,11 @@
       <c r="C42">
         <v>999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1523,8 +1662,11 @@
       <c r="C43">
         <v>999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>41</v>
       </c>
@@ -1534,8 +1676,11 @@
       <c r="C44">
         <v>999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>42</v>
       </c>
@@ -1545,8 +1690,11 @@
       <c r="C45">
         <v>999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43</v>
       </c>
@@ -1556,8 +1704,11 @@
       <c r="C46">
         <v>999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>44</v>
       </c>
@@ -1567,8 +1718,11 @@
       <c r="C47">
         <v>999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>45</v>
       </c>
@@ -1578,8 +1732,11 @@
       <c r="C48">
         <v>999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1589,8 +1746,11 @@
       <c r="C49">
         <v>999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1600,8 +1760,11 @@
       <c r="C50">
         <v>999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>48</v>
       </c>
@@ -1611,8 +1774,11 @@
       <c r="C51">
         <v>999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>49</v>
       </c>
@@ -1622,8 +1788,11 @@
       <c r="C52">
         <v>999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1633,8 +1802,11 @@
       <c r="C53">
         <v>999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>51</v>
       </c>
@@ -1644,8 +1816,11 @@
       <c r="C54">
         <v>999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>52</v>
       </c>
@@ -1655,8 +1830,11 @@
       <c r="C55">
         <v>999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>53</v>
       </c>
@@ -1666,8 +1844,11 @@
       <c r="C56">
         <v>999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>54</v>
       </c>
@@ -1677,8 +1858,11 @@
       <c r="C57">
         <v>999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>55</v>
       </c>
@@ -1688,8 +1872,11 @@
       <c r="C58">
         <v>999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>56</v>
       </c>
@@ -1699,8 +1886,11 @@
       <c r="C59">
         <v>999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>57</v>
       </c>
@@ -1710,8 +1900,11 @@
       <c r="C60">
         <v>999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>58</v>
       </c>
@@ -1721,8 +1914,11 @@
       <c r="C61">
         <v>999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>59</v>
       </c>
@@ -1732,8 +1928,11 @@
       <c r="C62">
         <v>999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>60</v>
       </c>
@@ -1743,8 +1942,11 @@
       <c r="C63">
         <v>999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>61</v>
       </c>
@@ -1754,8 +1956,11 @@
       <c r="C64">
         <v>999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>62</v>
       </c>
@@ -1765,8 +1970,11 @@
       <c r="C65">
         <v>999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>63</v>
       </c>
@@ -1776,8 +1984,11 @@
       <c r="C66">
         <v>999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>64</v>
       </c>
@@ -1787,8 +1998,11 @@
       <c r="C67">
         <v>999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>65</v>
       </c>
@@ -1798,8 +2012,11 @@
       <c r="C68">
         <v>999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>66</v>
       </c>
@@ -1809,8 +2026,11 @@
       <c r="C69">
         <v>999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>67</v>
       </c>
@@ -1820,8 +2040,11 @@
       <c r="C70">
         <v>999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>68</v>
       </c>
@@ -1831,8 +2054,11 @@
       <c r="C71">
         <v>999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>69</v>
       </c>
@@ -1842,8 +2068,11 @@
       <c r="C72">
         <v>999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>70</v>
       </c>
@@ -1853,8 +2082,11 @@
       <c r="C73">
         <v>999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>71</v>
       </c>
@@ -1864,8 +2096,11 @@
       <c r="C74">
         <v>999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>72</v>
       </c>
@@ -1875,8 +2110,11 @@
       <c r="C75">
         <v>999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>73</v>
       </c>
@@ -1886,8 +2124,11 @@
       <c r="C76">
         <v>999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>74</v>
       </c>
@@ -1897,8 +2138,11 @@
       <c r="C77">
         <v>999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>75</v>
       </c>
@@ -1908,8 +2152,11 @@
       <c r="C78">
         <v>999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>76</v>
       </c>
@@ -1919,8 +2166,11 @@
       <c r="C79">
         <v>999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>77</v>
       </c>
@@ -1930,8 +2180,11 @@
       <c r="C80">
         <v>999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>78</v>
       </c>
@@ -1941,8 +2194,11 @@
       <c r="C81">
         <v>999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>79</v>
       </c>
@@ -1952,8 +2208,11 @@
       <c r="C82">
         <v>999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>80</v>
       </c>
@@ -1963,8 +2222,11 @@
       <c r="C83">
         <v>999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>81</v>
       </c>
@@ -1974,8 +2236,11 @@
       <c r="C84">
         <v>999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>82</v>
       </c>
@@ -1985,8 +2250,11 @@
       <c r="C85">
         <v>999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>83</v>
       </c>
@@ -1996,8 +2264,11 @@
       <c r="C86">
         <v>999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>84</v>
       </c>
@@ -2007,8 +2278,11 @@
       <c r="C87">
         <v>999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>85</v>
       </c>
@@ -2018,8 +2292,11 @@
       <c r="C88">
         <v>999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>86</v>
       </c>
@@ -2029,8 +2306,11 @@
       <c r="C89">
         <v>999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>87</v>
       </c>
@@ -2040,8 +2320,11 @@
       <c r="C90">
         <v>999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>88</v>
       </c>
@@ -2051,8 +2334,11 @@
       <c r="C91">
         <v>999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>89</v>
       </c>
@@ -2062,8 +2348,11 @@
       <c r="C92">
         <v>999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>90</v>
       </c>
@@ -2073,8 +2362,11 @@
       <c r="C93">
         <v>999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>91</v>
       </c>
@@ -2084,8 +2376,11 @@
       <c r="C94">
         <v>999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>92</v>
       </c>
@@ -2095,8 +2390,11 @@
       <c r="C95">
         <v>999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>93</v>
       </c>
@@ -2106,8 +2404,11 @@
       <c r="C96">
         <v>999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>94</v>
       </c>
@@ -2117,8 +2418,11 @@
       <c r="C97">
         <v>999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>95</v>
       </c>
@@ -2128,8 +2432,11 @@
       <c r="C98">
         <v>999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>96</v>
       </c>
@@ -2139,8 +2446,11 @@
       <c r="C99">
         <v>999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>97</v>
       </c>
@@ -2150,8 +2460,11 @@
       <c r="C100">
         <v>999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>98</v>
       </c>
@@ -2161,8 +2474,11 @@
       <c r="C101">
         <v>999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>99</v>
       </c>
@@ -2171,6 +2487,9 @@
       </c>
       <c r="C102">
         <v>999999</v>
+      </c>
+      <c r="D102">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust the equip addon on levels
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Exp" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -64,6 +64,14 @@
   </si>
   <si>
     <t>英雄技能等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipAddon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备加成</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -760,14 +768,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E102" totalsRowShown="0">
-  <autoFilter ref="A1:E102"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:F102" totalsRowShown="0">
+  <autoFilter ref="A1:F102"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Exp"/>
     <tableColumn id="3" name="CardExp"/>
     <tableColumn id="4" name="TowerLevel"/>
     <tableColumn id="5" name="HeroSkillLevel"/>
+    <tableColumn id="6" name="EquipAddon"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1060,18 +1069,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1087,8 +1096,11 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,8 +1116,11 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1121,8 +1136,11 @@
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1138,8 +1156,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1155,8 +1176,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1172,8 +1196,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1189,8 +1216,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1206,8 +1236,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1223,8 +1256,11 @@
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1240,8 +1276,11 @@
       <c r="E10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1258,8 +1297,11 @@
       <c r="E11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1276,8 +1318,11 @@
       <c r="E12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1293,8 +1338,11 @@
       <c r="E13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F13">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1310,8 +1358,11 @@
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1327,8 +1378,11 @@
       <c r="E15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1344,8 +1398,11 @@
       <c r="E16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1361,8 +1418,11 @@
       <c r="E17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F17">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1378,8 +1438,11 @@
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1395,8 +1458,11 @@
       <c r="E19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F19">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1412,8 +1478,11 @@
       <c r="E20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F20">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1429,8 +1498,11 @@
       <c r="E21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1446,8 +1518,11 @@
       <c r="E22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F22">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1463,8 +1538,11 @@
       <c r="E23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F23">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1480,8 +1558,11 @@
       <c r="E24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F24">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1497,8 +1578,11 @@
       <c r="E25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1514,8 +1598,11 @@
       <c r="E26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F26">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1531,8 +1618,11 @@
       <c r="E27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F27">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1548,8 +1638,11 @@
       <c r="E28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1565,8 +1658,11 @@
       <c r="E29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F29">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1582,8 +1678,11 @@
       <c r="E30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F30">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1599,8 +1698,11 @@
       <c r="E31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F31">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1616,8 +1718,11 @@
       <c r="E32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F32">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1633,8 +1738,11 @@
       <c r="E33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F33">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1650,8 +1758,11 @@
       <c r="E34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F34">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1667,8 +1778,11 @@
       <c r="E35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1684,8 +1798,11 @@
       <c r="E36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F36">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1701,8 +1818,11 @@
       <c r="E37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F37">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1718,8 +1838,11 @@
       <c r="E38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F38">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1735,8 +1858,11 @@
       <c r="E39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F39">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1752,8 +1878,11 @@
       <c r="E40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F40">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1769,8 +1898,11 @@
       <c r="E41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F41">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1786,8 +1918,11 @@
       <c r="E42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F42">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1803,8 +1938,11 @@
       <c r="E43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F43">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -1820,8 +1958,11 @@
       <c r="E44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F44">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -1837,8 +1978,11 @@
       <c r="E45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F45">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -1854,8 +1998,11 @@
       <c r="E46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F46">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -1871,8 +2018,11 @@
       <c r="E47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F47">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -1888,8 +2038,11 @@
       <c r="E48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F48">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1905,8 +2058,11 @@
       <c r="E49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F49">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1922,8 +2078,11 @@
       <c r="E50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F50">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -1939,8 +2098,11 @@
       <c r="E51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F51">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -1956,8 +2118,11 @@
       <c r="E52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F52">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1973,8 +2138,11 @@
       <c r="E53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F53">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -1990,8 +2158,11 @@
       <c r="E54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F54">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -2007,8 +2178,11 @@
       <c r="E55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F55">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -2024,8 +2198,11 @@
       <c r="E56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F56">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -2041,8 +2218,11 @@
       <c r="E57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F57">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -2058,8 +2238,11 @@
       <c r="E58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F58">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -2075,8 +2258,11 @@
       <c r="E59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F59">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -2092,8 +2278,11 @@
       <c r="E60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F60">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -2109,8 +2298,11 @@
       <c r="E61">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F61">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -2126,8 +2318,11 @@
       <c r="E62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F62">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -2143,8 +2338,11 @@
       <c r="E63">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F63">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -2160,8 +2358,11 @@
       <c r="E64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F64">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -2177,8 +2378,11 @@
       <c r="E65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F65">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
@@ -2194,8 +2398,11 @@
       <c r="E66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F66">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
@@ -2211,8 +2418,11 @@
       <c r="E67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F67">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
@@ -2228,8 +2438,11 @@
       <c r="E68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F68">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
@@ -2245,8 +2458,11 @@
       <c r="E69">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F69">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
@@ -2262,8 +2478,11 @@
       <c r="E70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F70">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -2279,8 +2498,11 @@
       <c r="E71">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F71">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
@@ -2296,8 +2518,11 @@
       <c r="E72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F72">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
@@ -2313,8 +2538,11 @@
       <c r="E73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F73">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
@@ -2330,8 +2558,11 @@
       <c r="E74">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F74">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -2347,8 +2578,11 @@
       <c r="E75">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F75">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
@@ -2364,8 +2598,11 @@
       <c r="E76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F76">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
@@ -2381,8 +2618,11 @@
       <c r="E77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F77">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
@@ -2398,8 +2638,11 @@
       <c r="E78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F78">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
@@ -2415,8 +2658,11 @@
       <c r="E79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F79">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
@@ -2432,8 +2678,11 @@
       <c r="E80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F80">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -2449,8 +2698,11 @@
       <c r="E81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F81">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
@@ -2466,8 +2718,11 @@
       <c r="E82">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F82">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>80</v>
       </c>
@@ -2483,8 +2738,11 @@
       <c r="E83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F83">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>81</v>
       </c>
@@ -2500,8 +2758,11 @@
       <c r="E84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F84">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>82</v>
       </c>
@@ -2517,8 +2778,11 @@
       <c r="E85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F85">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>83</v>
       </c>
@@ -2534,8 +2798,11 @@
       <c r="E86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F86">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>84</v>
       </c>
@@ -2551,8 +2818,11 @@
       <c r="E87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F87">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>85</v>
       </c>
@@ -2568,8 +2838,11 @@
       <c r="E88">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F88">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>86</v>
       </c>
@@ -2585,8 +2858,11 @@
       <c r="E89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F89">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>87</v>
       </c>
@@ -2602,8 +2878,11 @@
       <c r="E90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F90">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>88</v>
       </c>
@@ -2619,8 +2898,11 @@
       <c r="E91">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F91">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>89</v>
       </c>
@@ -2636,8 +2918,11 @@
       <c r="E92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F92">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
@@ -2653,8 +2938,11 @@
       <c r="E93">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F93">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>91</v>
       </c>
@@ -2670,8 +2958,11 @@
       <c r="E94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F94">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>92</v>
       </c>
@@ -2687,8 +2978,11 @@
       <c r="E95">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F95">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>93</v>
       </c>
@@ -2704,8 +2998,11 @@
       <c r="E96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F96">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>94</v>
       </c>
@@ -2721,8 +3018,11 @@
       <c r="E97">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F97">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>95</v>
       </c>
@@ -2738,8 +3038,11 @@
       <c r="E98">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F98">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>96</v>
       </c>
@@ -2755,8 +3058,11 @@
       <c r="E99">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F99">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>97</v>
       </c>
@@ -2772,8 +3078,11 @@
       <c r="E100">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F100">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>98</v>
       </c>
@@ -2789,8 +3098,11 @@
       <c r="E101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F101">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>99</v>
       </c>
@@ -2805,6 +3117,9 @@
       </c>
       <c r="E102">
         <v>5</v>
+      </c>
+      <c r="F102">
+        <v>493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
balance the tower attack the attack speed. and equip addon to tower
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1157,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1319,7 +1319,7 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>3</v>
       </c>
       <c r="F20">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="F21">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1519,7 +1519,7 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="F28">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
         <v>4</v>
       </c>
       <c r="F29">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="F30">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1699,7 +1699,7 @@
         <v>4</v>
       </c>
       <c r="F31">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>5</v>
       </c>
       <c r="F32">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1739,7 +1739,7 @@
         <v>5</v>
       </c>
       <c r="F33">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>5</v>
       </c>
       <c r="F34">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="F35">
-        <v>158</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="F36">
-        <v>163</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,7 +1819,7 @@
         <v>5</v>
       </c>
       <c r="F37">
-        <v>168</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>5</v>
       </c>
       <c r="F38">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1859,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="F39">
-        <v>178</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="F40">
-        <v>183</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1899,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="F41">
-        <v>188</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>5</v>
       </c>
       <c r="F42">
-        <v>193</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1939,7 +1939,7 @@
         <v>5</v>
       </c>
       <c r="F43">
-        <v>198</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1959,7 +1959,7 @@
         <v>5</v>
       </c>
       <c r="F44">
-        <v>203</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1979,7 +1979,7 @@
         <v>5</v>
       </c>
       <c r="F45">
-        <v>208</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
         <v>5</v>
       </c>
       <c r="F46">
-        <v>213</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2019,7 @@
         <v>5</v>
       </c>
       <c r="F47">
-        <v>218</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
         <v>5</v>
       </c>
       <c r="F48">
-        <v>223</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="F49">
-        <v>228</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2079,7 +2079,7 @@
         <v>5</v>
       </c>
       <c r="F50">
-        <v>233</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>5</v>
       </c>
       <c r="F51">
-        <v>238</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>5</v>
       </c>
       <c r="F52">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>5</v>
       </c>
       <c r="F53">
-        <v>248</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2159,7 +2159,7 @@
         <v>5</v>
       </c>
       <c r="F54">
-        <v>253</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>5</v>
       </c>
       <c r="F55">
-        <v>258</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
         <v>5</v>
       </c>
       <c r="F56">
-        <v>263</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2219,7 +2219,7 @@
         <v>5</v>
       </c>
       <c r="F57">
-        <v>268</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2239,7 +2239,7 @@
         <v>5</v>
       </c>
       <c r="F58">
-        <v>273</v>
+        <v>307</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,7 +2259,7 @@
         <v>5</v>
       </c>
       <c r="F59">
-        <v>278</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>5</v>
       </c>
       <c r="F60">
-        <v>283</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
         <v>5</v>
       </c>
       <c r="F61">
-        <v>288</v>
+        <v>325</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="F62">
-        <v>293</v>
+        <v>331</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
         <v>5</v>
       </c>
       <c r="F63">
-        <v>298</v>
+        <v>337</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>5</v>
       </c>
       <c r="F64">
-        <v>303</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
         <v>5</v>
       </c>
       <c r="F65">
-        <v>308</v>
+        <v>349</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2399,7 +2399,7 @@
         <v>5</v>
       </c>
       <c r="F66">
-        <v>313</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2419,7 +2419,7 @@
         <v>5</v>
       </c>
       <c r="F67">
-        <v>318</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>5</v>
       </c>
       <c r="F68">
-        <v>323</v>
+        <v>367</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2459,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="F69">
-        <v>328</v>
+        <v>373</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2479,7 +2479,7 @@
         <v>5</v>
       </c>
       <c r="F70">
-        <v>333</v>
+        <v>379</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2499,7 +2499,7 @@
         <v>5</v>
       </c>
       <c r="F71">
-        <v>338</v>
+        <v>385</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>5</v>
       </c>
       <c r="F72">
-        <v>343</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
         <v>5</v>
       </c>
       <c r="F73">
-        <v>348</v>
+        <v>397</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>5</v>
       </c>
       <c r="F74">
-        <v>353</v>
+        <v>403</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2579,7 +2579,7 @@
         <v>5</v>
       </c>
       <c r="F75">
-        <v>358</v>
+        <v>409</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="F76">
-        <v>363</v>
+        <v>415</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2619,7 +2619,7 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>368</v>
+        <v>421</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>5</v>
       </c>
       <c r="F78">
-        <v>373</v>
+        <v>427</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2659,7 +2659,7 @@
         <v>5</v>
       </c>
       <c r="F79">
-        <v>378</v>
+        <v>433</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>5</v>
       </c>
       <c r="F80">
-        <v>383</v>
+        <v>439</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
         <v>5</v>
       </c>
       <c r="F81">
-        <v>388</v>
+        <v>445</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>5</v>
       </c>
       <c r="F82">
-        <v>393</v>
+        <v>451</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2739,7 +2739,7 @@
         <v>5</v>
       </c>
       <c r="F83">
-        <v>398</v>
+        <v>457</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>5</v>
       </c>
       <c r="F84">
-        <v>403</v>
+        <v>463</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>5</v>
       </c>
       <c r="F85">
-        <v>408</v>
+        <v>469</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2799,7 +2799,7 @@
         <v>5</v>
       </c>
       <c r="F86">
-        <v>413</v>
+        <v>475</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>5</v>
       </c>
       <c r="F87">
-        <v>418</v>
+        <v>481</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>5</v>
       </c>
       <c r="F88">
-        <v>423</v>
+        <v>487</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2859,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="F89">
-        <v>428</v>
+        <v>493</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>5</v>
       </c>
       <c r="F90">
-        <v>433</v>
+        <v>499</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2899,7 +2899,7 @@
         <v>5</v>
       </c>
       <c r="F91">
-        <v>438</v>
+        <v>505</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2919,7 +2919,7 @@
         <v>5</v>
       </c>
       <c r="F92">
-        <v>443</v>
+        <v>511</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2939,7 +2939,7 @@
         <v>5</v>
       </c>
       <c r="F93">
-        <v>448</v>
+        <v>517</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>5</v>
       </c>
       <c r="F94">
-        <v>453</v>
+        <v>523</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2979,7 +2979,7 @@
         <v>5</v>
       </c>
       <c r="F95">
-        <v>458</v>
+        <v>529</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
         <v>5</v>
       </c>
       <c r="F96">
-        <v>463</v>
+        <v>535</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
         <v>5</v>
       </c>
       <c r="F97">
-        <v>468</v>
+        <v>541</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
         <v>5</v>
       </c>
       <c r="F98">
-        <v>473</v>
+        <v>547</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
         <v>5</v>
       </c>
       <c r="F99">
-        <v>478</v>
+        <v>553</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3079,7 +3079,7 @@
         <v>5</v>
       </c>
       <c r="F100">
-        <v>483</v>
+        <v>559</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>5</v>
       </c>
       <c r="F101">
-        <v>488</v>
+        <v>565</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3119,7 +3119,7 @@
         <v>5</v>
       </c>
       <c r="F102">
-        <v>493</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support res drop on scenequests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Exp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -71,19 +71,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ResouceFactor</t>
+    <t>double</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>double</t>
+    <t>GoldFactor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResFactor</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +270,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -746,7 +758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,15 +771,6 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -779,6 +782,18 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -825,7 +840,34 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1126,31 +1168,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:F102" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:F102"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="Exp" dataDxfId="4"/>
-    <tableColumn id="3" name="CardExp" dataDxfId="3"/>
-    <tableColumn id="4" name="TowerLevel" dataDxfId="2"/>
-    <tableColumn id="5" name="HeroSkillLevel" dataDxfId="1"/>
-    <tableColumn id="6" name="ResouceFactor" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G102" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A3:G102"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" name="Exp" dataDxfId="5"/>
+    <tableColumn id="3" name="CardExp" dataDxfId="4"/>
+    <tableColumn id="4" name="TowerLevel" dataDxfId="3"/>
+    <tableColumn id="5" name="HeroSkillLevel" dataDxfId="2"/>
+    <tableColumn id="6" name="GoldFactor" dataDxfId="1">
       <calculatedColumnFormula>POWER(A4+3,0.6)+3</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="7" name="ResFactor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1218,6 +1261,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1253,6 +1313,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1429,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1441,27 +1518,30 @@
     <col min="4" max="5" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1478,2108 +1558,2411 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
+      <c r="G3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
-        <v>20</v>
-      </c>
-      <c r="C4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
       <c r="F4">
         <f>POWER(A4+3,0.6)+3</f>
         <v>5.2973967099940698</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
+      <c r="G4" s="8">
+        <v>1.059479341998814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>30</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F68" si="0">POWER(A5+3,0.6)+3</f>
         <v>5.626527804403767</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="G5" s="8">
+        <v>1.1253055608807534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
         <v>40</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>5.9301560515835217</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
+      <c r="G6" s="8">
+        <v>1.1860312103167043</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="4">
         <v>50</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>20</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>6.2140958497160383</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="G7" s="8">
+        <v>1.2428191699432076</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
         <v>85</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>6.4822022531844965</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
+      <c r="G8" s="8">
+        <v>1.2964404506368994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="4">
         <v>100</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="4">
         <v>80</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="5">
         <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>6.7371928188465517</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
+      <c r="G9" s="8">
+        <v>1.3474385637693103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="4">
         <v>115</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>200</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="5">
         <v>2</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>6.9810717055349727</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
+      <c r="G10" s="8">
+        <v>1.3962143411069945</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="4">
         <v>130</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <f>C10+500</f>
         <v>700</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="5">
         <v>2</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>7.2153691330919001</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
+      <c r="G11" s="8">
+        <v>1.44307382661838</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="4">
         <v>145</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <f t="shared" ref="C12" si="1">C11+500</f>
         <v>1200</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="5">
         <v>2</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="5">
         <v>2</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>7.4412860698458401</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="8">
+      <c r="G12" s="8">
+        <v>1.4882572139691681</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="5">
         <v>200</v>
       </c>
-      <c r="C13" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D13" s="8">
+      <c r="C13" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D13" s="5">
         <v>2</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="5">
         <v>2</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>7.6597864200360659</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="8">
+      <c r="G13" s="8">
+        <v>1.5319572840072131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>220</v>
       </c>
-      <c r="C14" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D14" s="8">
+      <c r="C14" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="5">
         <v>2</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>7.8716583257669139</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="8">
+      <c r="G14" s="8">
+        <v>1.5743316651533827</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="5">
         <v>240</v>
       </c>
-      <c r="C15" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D15" s="8">
-        <v>3</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="C15" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5">
         <v>2</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>8.0775563919874074</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="8">
+      <c r="G15" s="8">
+        <v>1.6155112783974814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <v>260</v>
       </c>
-      <c r="C16" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D16" s="8">
-        <v>3</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="C16" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5">
         <v>2</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>8.2780316430915768</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="8">
+      <c r="G16" s="8">
+        <v>1.6556063286183154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="5">
         <v>280</v>
       </c>
-      <c r="C17" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D17" s="8">
-        <v>3</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="C17" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
         <v>3</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>8.4735533169184887</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="8">
+      <c r="G17" s="8">
+        <v>1.6947106633836977</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="5">
         <v>375</v>
       </c>
-      <c r="C18" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D18" s="8">
-        <v>3</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="C18" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
         <v>3</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>8.6645250677694108</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="8">
+      <c r="G18" s="8">
+        <v>1.7329050135538822</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="5">
         <v>400</v>
       </c>
-      <c r="C19" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D19" s="8">
-        <v>3</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="C19" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5">
         <v>3</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>8.8512972424092151</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="8">
+      <c r="G19" s="8">
+        <v>1.770259448481843</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="5">
         <v>425</v>
       </c>
-      <c r="C20" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D20" s="8">
-        <v>3</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C20" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D20" s="5">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5">
         <v>3</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>9.0341763365451619</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="8">
+      <c r="G20" s="8">
+        <v>1.8068352673090324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="5">
         <v>450</v>
       </c>
-      <c r="C21" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D21" s="8">
-        <v>3</v>
-      </c>
-      <c r="E21" s="8">
+      <c r="C21" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5">
         <v>3</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
         <v>9.2134323873607435</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="8">
+      <c r="G21" s="8">
+        <v>1.8426864774721488</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="5">
         <v>475</v>
       </c>
-      <c r="C22" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D22" s="8">
-        <v>3</v>
-      </c>
-      <c r="E22" s="8">
+      <c r="C22" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5">
         <v>3</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
         <v>9.3893048289839669</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="8">
+      <c r="G22" s="8">
+        <v>1.8778609657967933</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="5">
         <v>600</v>
       </c>
-      <c r="C23" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D23" s="8">
-        <v>3</v>
-      </c>
-      <c r="E23" s="8">
+      <c r="C23" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5">
         <v>4</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
         <v>9.5620071855158546</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="8">
+      <c r="G23" s="8">
+        <v>1.912401437103171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="5">
         <v>21</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="5">
         <v>630</v>
       </c>
-      <c r="C24" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D24" s="8">
-        <v>3</v>
-      </c>
-      <c r="E24" s="8">
+      <c r="C24" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5">
         <v>4</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>9.7317308726771969</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="8">
+      <c r="G24" s="8">
+        <v>1.9463461745354393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="5">
         <v>22</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="5">
         <v>660</v>
       </c>
-      <c r="C25" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D25" s="8">
-        <v>3</v>
-      </c>
-      <c r="E25" s="8">
+      <c r="C25" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D25" s="5">
+        <v>3</v>
+      </c>
+      <c r="E25" s="5">
         <v>4</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
         <v>9.8986483073060718</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="8">
+      <c r="G25" s="8">
+        <v>1.9797296614612143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="5">
         <v>23</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="5">
         <v>690</v>
       </c>
-      <c r="C26" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D26" s="8">
-        <v>3</v>
-      </c>
-      <c r="E26" s="8">
+      <c r="C26" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3</v>
+      </c>
+      <c r="E26" s="5">
         <v>4</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>10.062915473248847</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="8">
+      <c r="G26" s="8">
+        <v>2.0125830946497691</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="5">
         <v>24</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="5">
         <v>720</v>
       </c>
-      <c r="C27" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D27" s="8">
-        <v>3</v>
-      </c>
-      <c r="E27" s="8">
+      <c r="C27" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3</v>
+      </c>
+      <c r="E27" s="5">
         <v>4</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
         <v>10.224674055842076</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="8">
+      <c r="G27" s="8">
+        <v>2.0449348111684151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="5">
         <v>25</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="5">
         <v>875</v>
       </c>
-      <c r="C28" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D28" s="8">
-        <v>3</v>
-      </c>
-      <c r="E28" s="8">
+      <c r="C28" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5">
         <v>4</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
         <v>10.38405323074322</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="8">
+      <c r="G28" s="8">
+        <v>2.076810646148644</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="5">
         <v>26</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="5">
         <v>910</v>
       </c>
-      <c r="C29" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D29" s="8">
-        <v>3</v>
-      </c>
-      <c r="E29" s="8">
+      <c r="C29" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5">
         <v>4</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>10.541171173377641</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="8">
+      <c r="G29" s="8">
+        <v>2.1082342346755283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="5">
         <v>27</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="5">
         <v>945</v>
       </c>
-      <c r="C30" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D30" s="8">
-        <v>3</v>
-      </c>
-      <c r="E30" s="8">
+      <c r="C30" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D30" s="5">
+        <v>3</v>
+      </c>
+      <c r="E30" s="5">
         <v>4</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
         <v>10.696136340726078</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="8">
+      <c r="G30" s="8">
+        <v>2.1392272681452154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="5">
         <v>28</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="5">
         <v>980</v>
       </c>
-      <c r="C31" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D31" s="8">
-        <v>3</v>
-      </c>
-      <c r="E31" s="8">
+      <c r="C31" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D31" s="5">
+        <v>3</v>
+      </c>
+      <c r="E31" s="5">
         <v>4</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
         <v>10.849048566202034</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="8">
+      <c r="G31" s="8">
+        <v>2.1698097132404071</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="5">
         <v>29</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="5">
         <v>1015</v>
       </c>
-      <c r="C32" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D32" s="8">
-        <v>3</v>
-      </c>
-      <c r="E32" s="8">
+      <c r="C32" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D32" s="5">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5">
         <v>5</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
         <v>10.999999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="8">
+      <c r="G32" s="8">
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="5">
         <v>30</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="5">
         <v>1200</v>
       </c>
-      <c r="C33" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D33" s="8">
-        <v>3</v>
-      </c>
-      <c r="E33" s="8">
+      <c r="C33" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D33" s="5">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5">
         <v>5</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
         <v>11.149075920852829</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="8">
+      <c r="G33" s="8">
+        <v>2.2298151841705658</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="5">
         <v>31</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="5">
         <v>1240</v>
       </c>
-      <c r="C34" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D34" s="8">
-        <v>3</v>
-      </c>
-      <c r="E34" s="8">
+      <c r="C34" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D34" s="5">
+        <v>3</v>
+      </c>
+      <c r="E34" s="5">
         <v>5</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
         <v>11.296355440131292</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="8">
+      <c r="G34" s="8">
+        <v>2.2592710880262583</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="5">
         <v>32</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="5">
         <v>1280</v>
       </c>
-      <c r="C35" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D35" s="8">
-        <v>3</v>
-      </c>
-      <c r="E35" s="8">
+      <c r="C35" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D35" s="5">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5">
         <v>5</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
         <v>11.441912115297924</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="8">
+      <c r="G35" s="8">
+        <v>2.2883824230595851</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="5">
         <v>33</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="5">
         <v>1320</v>
       </c>
-      <c r="C36" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D36" s="8">
-        <v>3</v>
-      </c>
-      <c r="E36" s="8">
+      <c r="C36" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D36" s="5">
+        <v>3</v>
+      </c>
+      <c r="E36" s="5">
         <v>5</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
         <v>11.585814486631531</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="8">
+      <c r="G36" s="8">
+        <v>2.3171628973263063</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="5">
         <v>34</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="5">
         <v>1360</v>
       </c>
-      <c r="C37" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D37" s="8">
-        <v>3</v>
-      </c>
-      <c r="E37" s="8">
+      <c r="C37" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3</v>
+      </c>
+      <c r="E37" s="5">
         <v>5</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
         <v>11.72812654867613</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="8">
+      <c r="G37" s="8">
+        <v>2.345625309735226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="5">
         <v>35</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="5">
         <v>1575</v>
       </c>
-      <c r="C38" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D38" s="8">
-        <v>3</v>
-      </c>
-      <c r="E38" s="8">
+      <c r="C38" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D38" s="5">
+        <v>3</v>
+      </c>
+      <c r="E38" s="5">
         <v>5</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
         <v>11.868908165896258</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="8">
+      <c r="G38" s="8">
+        <v>2.3737816331792514</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="5">
         <v>36</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="5">
         <v>1620</v>
       </c>
-      <c r="C39" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D39" s="8">
-        <v>3</v>
-      </c>
-      <c r="E39" s="8">
+      <c r="C39" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D39" s="5">
+        <v>3</v>
+      </c>
+      <c r="E39" s="5">
         <v>5</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
         <v>12.008215440430581</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="8">
+      <c r="G39" s="8">
+        <v>2.4016430880861162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="5">
         <v>37</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="5">
         <v>1665</v>
       </c>
-      <c r="C40" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D40" s="8">
-        <v>3</v>
-      </c>
-      <c r="E40" s="8">
+      <c r="C40" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D40" s="5">
+        <v>3</v>
+      </c>
+      <c r="E40" s="5">
         <v>5</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
         <v>12.146101038546524</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="8">
+      <c r="G40" s="8">
+        <v>2.4292202077093048</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="5">
         <v>38</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="5">
         <v>1710</v>
       </c>
-      <c r="C41" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D41" s="8">
-        <v>3</v>
-      </c>
-      <c r="E41" s="8">
+      <c r="C41" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D41" s="5">
+        <v>3</v>
+      </c>
+      <c r="E41" s="5">
         <v>5</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
         <v>12.282614481346684</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="8">
+      <c r="G41" s="8">
+        <v>2.4565228962693366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="5">
         <v>39</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="5">
         <v>1755</v>
       </c>
-      <c r="C42" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D42" s="8">
-        <v>3</v>
-      </c>
-      <c r="E42" s="8">
+      <c r="C42" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D42" s="5">
+        <v>3</v>
+      </c>
+      <c r="E42" s="5">
         <v>5</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
         <v>12.41780240441493</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="8">
+      <c r="G42" s="8">
+        <v>2.4835604808829861</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="5">
         <v>40</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="5">
         <v>2000</v>
       </c>
-      <c r="C43" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D43" s="8">
-        <v>3</v>
-      </c>
-      <c r="E43" s="8">
+      <c r="C43" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D43" s="5">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5">
         <v>5</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
         <v>12.551708790378902</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="8">
+      <c r="G43" s="8">
+        <v>2.5103417580757803</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" s="5">
         <v>41</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="5">
         <v>2050</v>
       </c>
-      <c r="C44" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D44" s="8">
-        <v>3</v>
-      </c>
-      <c r="E44" s="8">
+      <c r="C44" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D44" s="5">
+        <v>3</v>
+      </c>
+      <c r="E44" s="5">
         <v>5</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
         <v>12.684375177775884</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="8">
+      <c r="G44" s="8">
+        <v>2.5368750355551768</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45" s="5">
         <v>42</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="5">
         <v>2100</v>
       </c>
-      <c r="C45" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D45" s="8">
-        <v>3</v>
-      </c>
-      <c r="E45" s="8">
+      <c r="C45" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D45" s="5">
+        <v>3</v>
+      </c>
+      <c r="E45" s="5">
         <v>5</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
         <v>12.81584084911856</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="8">
+      <c r="G45" s="8">
+        <v>2.5631681698237121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46" s="5">
         <v>43</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="5">
         <v>2150</v>
       </c>
-      <c r="C46" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D46" s="8">
-        <v>3</v>
-      </c>
-      <c r="E46" s="8">
+      <c r="C46" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D46" s="5">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
         <v>5</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
         <v>12.946143000646654</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="8">
+      <c r="G46" s="8">
+        <v>2.5892286001293305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="5">
         <v>44</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="5">
         <v>2200</v>
       </c>
-      <c r="C47" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D47" s="8">
-        <v>3</v>
-      </c>
-      <c r="E47" s="8">
+      <c r="C47" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D47" s="5">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5">
         <v>5</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
         <v>13.075316895906047</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="8">
+      <c r="G47" s="8">
+        <v>2.6150633791812092</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48" s="5">
         <v>45</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="5">
         <v>2475</v>
       </c>
-      <c r="C48" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D48" s="8">
-        <v>3</v>
-      </c>
-      <c r="E48" s="8">
+      <c r="C48" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D48" s="5">
+        <v>3</v>
+      </c>
+      <c r="E48" s="5">
         <v>5</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
         <v>13.203396005006329</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="8">
+      <c r="G48" s="8">
+        <v>2.6406792010012659</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A49" s="5">
         <v>46</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="5">
         <v>2530</v>
       </c>
-      <c r="C49" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D49" s="8">
-        <v>3</v>
-      </c>
-      <c r="E49" s="8">
+      <c r="C49" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D49" s="5">
+        <v>3</v>
+      </c>
+      <c r="E49" s="5">
         <v>5</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
         <v>13.330412131161864</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="8">
+      <c r="G49" s="8">
+        <v>2.6660824262323728</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A50" s="5">
         <v>47</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="5">
         <v>2585</v>
       </c>
-      <c r="C50" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D50" s="8">
-        <v>3</v>
-      </c>
-      <c r="E50" s="8">
+      <c r="C50" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D50" s="5">
+        <v>3</v>
+      </c>
+      <c r="E50" s="5">
         <v>5</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
         <v>13.456395525912733</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="8">
+      <c r="G50" s="8">
+        <v>2.6912791051825464</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A51" s="5">
         <v>48</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="5">
         <v>2640</v>
       </c>
-      <c r="C51" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D51" s="8">
-        <v>3</v>
-      </c>
-      <c r="E51" s="8">
+      <c r="C51" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D51" s="5">
+        <v>3</v>
+      </c>
+      <c r="E51" s="5">
         <v>5</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
         <v>13.581374994243514</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="8">
+      <c r="G51" s="8">
+        <v>2.7162749988487027</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A52" s="5">
         <v>49</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="5">
         <v>2695</v>
       </c>
-      <c r="C52" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D52" s="8">
-        <v>3</v>
-      </c>
-      <c r="E52" s="8">
+      <c r="C52" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D52" s="5">
+        <v>3</v>
+      </c>
+      <c r="E52" s="5">
         <v>5</v>
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
         <v>13.705377990665905</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="8">
+      <c r="G52" s="8">
+        <v>2.7410755981331811</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A53" s="5">
         <v>50</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="5">
         <v>3000</v>
       </c>
-      <c r="C53" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D53" s="8">
-        <v>3</v>
-      </c>
-      <c r="E53" s="8">
+      <c r="C53" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D53" s="5">
+        <v>3</v>
+      </c>
+      <c r="E53" s="5">
         <v>5</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
         <v>13.828430707200107</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="8">
+      <c r="G53" s="8">
+        <v>2.7656861414400216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A54" s="5">
         <v>51</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="5">
         <v>3060</v>
       </c>
-      <c r="C54" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D54" s="8">
-        <v>3</v>
-      </c>
-      <c r="E54" s="8">
+      <c r="C54" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D54" s="5">
+        <v>3</v>
+      </c>
+      <c r="E54" s="5">
         <v>5</v>
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
         <v>13.950558154077704</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="8">
+      <c r="G54" s="8">
+        <v>2.7901116308155407</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A55" s="5">
         <v>52</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="5">
         <v>3120</v>
       </c>
-      <c r="C55" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D55" s="8">
-        <v>3</v>
-      </c>
-      <c r="E55" s="8">
+      <c r="C55" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D55" s="5">
+        <v>3</v>
+      </c>
+      <c r="E55" s="5">
         <v>5</v>
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
         <v>14.071784233891282</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="8">
+      <c r="G55" s="8">
+        <v>2.8143568467782565</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A56" s="5">
         <v>53</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="5">
         <v>3180</v>
       </c>
-      <c r="C56" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D56" s="8">
-        <v>3</v>
-      </c>
-      <c r="E56" s="8">
+      <c r="C56" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D56" s="5">
+        <v>3</v>
+      </c>
+      <c r="E56" s="5">
         <v>5</v>
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
         <v>14.192131809832132</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="8">
+      <c r="G56" s="8">
+        <v>2.8384263619664263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A57" s="5">
         <v>54</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57" s="5">
         <v>3240</v>
       </c>
-      <c r="C57" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D57" s="8">
-        <v>3</v>
-      </c>
-      <c r="E57" s="8">
+      <c r="C57" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D57" s="5">
+        <v>3</v>
+      </c>
+      <c r="E57" s="5">
         <v>5</v>
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
         <v>14.311622768584231</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="8">
+      <c r="G57" s="8">
+        <v>2.8623245537168462</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A58" s="5">
         <v>55</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58" s="5">
         <v>3575</v>
       </c>
-      <c r="C58" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D58" s="8">
-        <v>3</v>
-      </c>
-      <c r="E58" s="8">
+      <c r="C58" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D58" s="5">
+        <v>3</v>
+      </c>
+      <c r="E58" s="5">
         <v>5</v>
       </c>
       <c r="F58">
         <f t="shared" si="0"/>
         <v>14.430278078379143</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="8">
+      <c r="G58" s="8">
+        <v>2.8860556156758284</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A59" s="5">
         <v>56</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="5">
         <v>3640</v>
       </c>
-      <c r="C59" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D59" s="8">
-        <v>3</v>
-      </c>
-      <c r="E59" s="8">
+      <c r="C59" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D59" s="5">
+        <v>3</v>
+      </c>
+      <c r="E59" s="5">
         <v>5</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
         <v>14.548117842660861</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="8">
+      <c r="G59" s="8">
+        <v>2.9096235685321723</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A60" s="5">
         <v>57</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="5">
         <v>3705</v>
       </c>
-      <c r="C60" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D60" s="8">
-        <v>3</v>
-      </c>
-      <c r="E60" s="8">
+      <c r="C60" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D60" s="5">
+        <v>3</v>
+      </c>
+      <c r="E60" s="5">
         <v>5</v>
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
         <v>14.665161349761227</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="8">
+      <c r="G60" s="8">
+        <v>2.9330322699522453</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A61" s="5">
         <v>58</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61" s="5">
         <v>3770</v>
       </c>
-      <c r="C61" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D61" s="8">
-        <v>3</v>
-      </c>
-      <c r="E61" s="8">
+      <c r="C61" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D61" s="5">
+        <v>3</v>
+      </c>
+      <c r="E61" s="5">
         <v>5</v>
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
         <v>14.781427118943885</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="8">
+      <c r="G61" s="8">
+        <v>2.9562854237887768</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A62" s="5">
         <v>59</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="5">
         <v>3835</v>
       </c>
-      <c r="C62" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D62" s="8">
-        <v>3</v>
-      </c>
-      <c r="E62" s="8">
+      <c r="C62" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D62" s="5">
+        <v>3</v>
+      </c>
+      <c r="E62" s="5">
         <v>5</v>
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
         <v>14.896932943137111</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="8">
+      <c r="G62" s="8">
+        <v>2.9793865886274222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A63" s="5">
         <v>60</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63" s="5">
         <v>4200</v>
       </c>
-      <c r="C63" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D63" s="8">
-        <v>3</v>
-      </c>
-      <c r="E63" s="8">
+      <c r="C63" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D63" s="5">
+        <v>3</v>
+      </c>
+      <c r="E63" s="5">
         <v>5</v>
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
         <v>15.011695928643283</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="8">
+      <c r="G63" s="8">
+        <v>3.0023391857286565</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A64" s="5">
         <v>61</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="5">
         <v>4270</v>
       </c>
-      <c r="C64" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D64" s="8">
-        <v>3</v>
-      </c>
-      <c r="E64" s="8">
+      <c r="C64" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D64" s="5">
+        <v>3</v>
+      </c>
+      <c r="E64" s="5">
         <v>5</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
         <v>15.125732532083184</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" s="8">
+      <c r="G64" s="8">
+        <v>3.025146506416637</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A65" s="5">
         <v>62</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="5">
         <v>4340</v>
       </c>
-      <c r="C65" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D65" s="8">
-        <v>3</v>
-      </c>
-      <c r="E65" s="8">
+      <c r="C65" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D65" s="5">
+        <v>3</v>
+      </c>
+      <c r="E65" s="5">
         <v>5</v>
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
         <v>15.239058594807814</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="8">
+      <c r="G65" s="8">
+        <v>3.0478117189615626</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A66" s="5">
         <v>63</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="5">
         <v>4410</v>
       </c>
-      <c r="C66" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D66" s="8">
-        <v>3</v>
-      </c>
-      <c r="E66" s="8">
+      <c r="C66" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D66" s="5">
+        <v>3</v>
+      </c>
+      <c r="E66" s="5">
         <v>5</v>
       </c>
       <c r="F66">
         <f t="shared" si="0"/>
         <v>15.351689374987611</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="8">
+      <c r="G66" s="8">
+        <v>3.0703378749975223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A67" s="5">
         <v>64</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="5">
         <v>4480</v>
       </c>
-      <c r="C67" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D67" s="8">
-        <v>3</v>
-      </c>
-      <c r="E67" s="8">
+      <c r="C67" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D67" s="5">
+        <v>3</v>
+      </c>
+      <c r="E67" s="5">
         <v>5</v>
       </c>
       <c r="F67">
         <f t="shared" si="0"/>
         <v>15.463639577568394</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A68" s="8">
+      <c r="G67" s="8">
+        <v>3.0927279155136786</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A68" s="5">
         <v>65</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="5">
         <v>4875</v>
       </c>
-      <c r="C68" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D68" s="8">
-        <v>3</v>
-      </c>
-      <c r="E68" s="8">
+      <c r="C68" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D68" s="5">
+        <v>3</v>
+      </c>
+      <c r="E68" s="5">
         <v>5</v>
       </c>
       <c r="F68">
         <f t="shared" si="0"/>
         <v>15.574923382265665</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A69" s="8">
+      <c r="G68" s="8">
+        <v>3.1149846764531328</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A69" s="5">
         <v>66</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="5">
         <v>4950</v>
       </c>
-      <c r="C69" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D69" s="8">
-        <v>3</v>
-      </c>
-      <c r="E69" s="8">
+      <c r="C69" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D69" s="5">
+        <v>3</v>
+      </c>
+      <c r="E69" s="5">
         <v>5</v>
       </c>
       <c r="F69">
         <f t="shared" ref="F69:F102" si="2">POWER(A69+3,0.6)+3</f>
         <v>15.685554469752462</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A70" s="8">
+      <c r="G69" s="8">
+        <v>3.1371108939504926</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A70" s="5">
         <v>67</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="5">
         <v>5025</v>
       </c>
-      <c r="C70" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D70" s="8">
-        <v>3</v>
-      </c>
-      <c r="E70" s="8">
+      <c r="C70" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D70" s="5">
+        <v>3</v>
+      </c>
+      <c r="E70" s="5">
         <v>5</v>
       </c>
       <c r="F70">
         <f t="shared" si="2"/>
         <v>15.79554604618191</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A71" s="8">
+      <c r="G70" s="8">
+        <v>3.1591092092363819</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A71" s="5">
         <v>68</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B71" s="5">
         <v>5100</v>
       </c>
-      <c r="C71" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D71" s="8">
-        <v>3</v>
-      </c>
-      <c r="E71" s="8">
+      <c r="C71" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D71" s="5">
+        <v>3</v>
+      </c>
+      <c r="E71" s="5">
         <v>5</v>
       </c>
       <c r="F71">
         <f t="shared" si="2"/>
         <v>15.904910866172429</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A72" s="8">
+      <c r="G71" s="8">
+        <v>3.1809821732344856</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A72" s="5">
         <v>69</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B72" s="5">
         <v>5175</v>
       </c>
-      <c r="C72" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D72" s="8">
-        <v>3</v>
-      </c>
-      <c r="E72" s="8">
+      <c r="C72" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D72" s="5">
+        <v>3</v>
+      </c>
+      <c r="E72" s="5">
         <v>5</v>
       </c>
       <c r="F72">
         <f t="shared" si="2"/>
         <v>16.01366125437238</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A73" s="8">
+      <c r="G72" s="8">
+        <v>3.202732250874476</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A73" s="5">
         <v>70</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="5">
         <v>5600</v>
       </c>
-      <c r="C73" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D73" s="8">
-        <v>3</v>
-      </c>
-      <c r="E73" s="8">
+      <c r="C73" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D73" s="5">
+        <v>3</v>
+      </c>
+      <c r="E73" s="5">
         <v>5</v>
       </c>
       <c r="F73">
         <f t="shared" si="2"/>
         <v>16.121809125710286</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A74" s="8">
+      <c r="G73" s="8">
+        <v>3.2243618251420569</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A74" s="5">
         <v>71</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B74" s="5">
         <v>5680</v>
       </c>
-      <c r="C74" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D74" s="8">
-        <v>3</v>
-      </c>
-      <c r="E74" s="8">
+      <c r="C74" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D74" s="5">
+        <v>3</v>
+      </c>
+      <c r="E74" s="5">
         <v>5</v>
       </c>
       <c r="F74">
         <f t="shared" si="2"/>
         <v>16.229366004427643</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A75" s="8">
+      <c r="G74" s="8">
+        <v>3.2458732008855287</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A75" s="5">
         <v>72</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="5">
         <v>5760</v>
       </c>
-      <c r="C75" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D75" s="8">
-        <v>3</v>
-      </c>
-      <c r="E75" s="8">
+      <c r="C75" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D75" s="5">
+        <v>3</v>
+      </c>
+      <c r="E75" s="5">
         <v>5</v>
       </c>
       <c r="F75">
         <f t="shared" si="2"/>
         <v>16.336343041982992</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A76" s="8">
+      <c r="G75" s="8">
+        <v>3.2672686083965985</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A76" s="5">
         <v>73</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B76" s="5">
         <v>5840</v>
       </c>
-      <c r="C76" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D76" s="8">
-        <v>3</v>
-      </c>
-      <c r="E76" s="8">
+      <c r="C76" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D76" s="5">
+        <v>3</v>
+      </c>
+      <c r="E76" s="5">
         <v>5</v>
       </c>
       <c r="F76">
         <f t="shared" si="2"/>
         <v>16.442751033908309</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A77" s="8">
+      <c r="G76" s="8">
+        <v>3.2885502067816619</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A77" s="5">
         <v>74</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="5">
         <v>5920</v>
       </c>
-      <c r="C77" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D77" s="8">
-        <v>3</v>
-      </c>
-      <c r="E77" s="8">
+      <c r="C77" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D77" s="5">
+        <v>3</v>
+      </c>
+      <c r="E77" s="5">
         <v>5</v>
       </c>
       <c r="F77">
         <f t="shared" si="2"/>
         <v>16.548600435691771</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A78" s="8">
+      <c r="G77" s="8">
+        <v>3.3097200871383543</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A78" s="5">
         <v>75</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="5">
         <v>6375</v>
       </c>
-      <c r="C78" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D78" s="8">
-        <v>3</v>
-      </c>
-      <c r="E78" s="8">
+      <c r="C78" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D78" s="5">
+        <v>3</v>
+      </c>
+      <c r="E78" s="5">
         <v>5</v>
       </c>
       <c r="F78">
         <f t="shared" si="2"/>
         <v>16.653901377755393</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A79" s="8">
+      <c r="G78" s="8">
+        <v>3.3307802755510787</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A79" s="5">
         <v>76</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="5">
         <v>6460</v>
       </c>
-      <c r="C79" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D79" s="8">
-        <v>3</v>
-      </c>
-      <c r="E79" s="8">
+      <c r="C79" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D79" s="5">
+        <v>3</v>
+      </c>
+      <c r="E79" s="5">
         <v>5</v>
       </c>
       <c r="F79">
         <f t="shared" si="2"/>
         <v>16.75866367958966</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A80" s="8">
+      <c r="G79" s="8">
+        <v>3.3517327359179321</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A80" s="5">
         <v>77</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B80" s="5">
         <v>6545</v>
       </c>
-      <c r="C80" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D80" s="8">
-        <v>3</v>
-      </c>
-      <c r="E80" s="8">
+      <c r="C80" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D80" s="5">
+        <v>3</v>
+      </c>
+      <c r="E80" s="5">
         <v>5</v>
       </c>
       <c r="F80">
         <f t="shared" si="2"/>
         <v>16.862896863102925</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A81" s="8">
+      <c r="G80" s="8">
+        <v>3.372579372620585</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A81" s="5">
         <v>78</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B81" s="5">
         <v>6630</v>
       </c>
-      <c r="C81" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D81" s="8">
-        <v>3</v>
-      </c>
-      <c r="E81" s="8">
+      <c r="C81" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D81" s="5">
+        <v>3</v>
+      </c>
+      <c r="E81" s="5">
         <v>5</v>
       </c>
       <c r="F81">
         <f t="shared" si="2"/>
         <v>16.966610165238237</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A82" s="8">
+      <c r="G81" s="8">
+        <v>3.3933220330476472</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A82" s="5">
         <v>79</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B82" s="5">
         <v>6715</v>
       </c>
-      <c r="C82" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D82" s="8">
-        <v>3</v>
-      </c>
-      <c r="E82" s="8">
+      <c r="C82" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D82" s="5">
+        <v>3</v>
+      </c>
+      <c r="E82" s="5">
         <v>5</v>
       </c>
       <c r="F82">
         <f t="shared" si="2"/>
         <v>17.069812549906494</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="8">
+      <c r="G82" s="8">
+        <v>3.4139625099812987</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A83" s="5">
         <v>80</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="5">
         <v>7200</v>
       </c>
-      <c r="C83" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D83" s="8">
-        <v>3</v>
-      </c>
-      <c r="E83" s="8">
+      <c r="C83" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D83" s="5">
+        <v>3</v>
+      </c>
+      <c r="E83" s="5">
         <v>5</v>
       </c>
       <c r="F83">
         <f t="shared" si="2"/>
         <v>17.172512719280761</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A84" s="8">
+      <c r="G83" s="8">
+        <v>3.4345025438561523</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A84" s="5">
         <v>81</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B84" s="5">
         <v>7290</v>
       </c>
-      <c r="C84" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D84" s="8">
-        <v>3</v>
-      </c>
-      <c r="E84" s="8">
+      <c r="C84" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D84" s="5">
+        <v>3</v>
+      </c>
+      <c r="E84" s="5">
         <v>5</v>
       </c>
       <c r="F84">
         <f t="shared" si="2"/>
         <v>17.274719124493167</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A85" s="8">
+      <c r="G84" s="8">
+        <v>3.4549438248986335</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A85" s="5">
         <v>82</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="5">
         <v>7380</v>
       </c>
-      <c r="C85" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D85" s="8">
-        <v>3</v>
-      </c>
-      <c r="E85" s="8">
+      <c r="C85" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D85" s="5">
+        <v>3</v>
+      </c>
+      <c r="E85" s="5">
         <v>5</v>
       </c>
       <c r="F85">
         <f t="shared" si="2"/>
         <v>17.376439975772879</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A86" s="8">
+      <c r="G85" s="8">
+        <v>3.4752879951545759</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A86" s="5">
         <v>83</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="5">
         <v>7470</v>
       </c>
-      <c r="C86" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D86" s="8">
-        <v>3</v>
-      </c>
-      <c r="E86" s="8">
+      <c r="C86" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D86" s="5">
+        <v>3</v>
+      </c>
+      <c r="E86" s="5">
         <v>5</v>
       </c>
       <c r="F86">
         <f t="shared" si="2"/>
         <v>17.477683252060292</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A87" s="8">
+      <c r="G86" s="8">
+        <v>3.4955366504120584</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A87" s="5">
         <v>84</v>
       </c>
-      <c r="B87" s="8">
+      <c r="B87" s="5">
         <v>7560</v>
       </c>
-      <c r="C87" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D87" s="8">
-        <v>3</v>
-      </c>
-      <c r="E87" s="8">
+      <c r="C87" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D87" s="5">
+        <v>3</v>
+      </c>
+      <c r="E87" s="5">
         <v>5</v>
       </c>
       <c r="F87">
         <f t="shared" si="2"/>
         <v>17.578456710130649</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A88" s="8">
+      <c r="G87" s="8">
+        <v>3.5156913420261295</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A88" s="5">
         <v>85</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B88" s="5">
         <v>8075</v>
       </c>
-      <c r="C88" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D88" s="8">
-        <v>3</v>
-      </c>
-      <c r="E88" s="8">
+      <c r="C88" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D88" s="5">
+        <v>3</v>
+      </c>
+      <c r="E88" s="5">
         <v>5</v>
       </c>
       <c r="F88">
         <f t="shared" si="2"/>
         <v>17.678767893256996</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89" s="8">
+      <c r="G88" s="8">
+        <v>3.5357535786513994</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A89" s="5">
         <v>86</v>
       </c>
-      <c r="B89" s="8">
+      <c r="B89" s="5">
         <v>8170</v>
       </c>
-      <c r="C89" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D89" s="8">
-        <v>3</v>
-      </c>
-      <c r="E89" s="8">
+      <c r="C89" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D89" s="5">
+        <v>3</v>
+      </c>
+      <c r="E89" s="5">
         <v>5</v>
       </c>
       <c r="F89">
         <f t="shared" si="2"/>
         <v>17.778624139441146</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A90" s="8">
+      <c r="G89" s="8">
+        <v>3.5557248278882292</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A90" s="5">
         <v>87</v>
       </c>
-      <c r="B90" s="8">
+      <c r="B90" s="5">
         <v>8265</v>
       </c>
-      <c r="C90" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D90" s="8">
-        <v>3</v>
-      </c>
-      <c r="E90" s="8">
+      <c r="C90" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D90" s="5">
+        <v>3</v>
+      </c>
+      <c r="E90" s="5">
         <v>5</v>
       </c>
       <c r="F90">
         <f t="shared" si="2"/>
         <v>17.878032589238494</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A91" s="8">
+      <c r="G90" s="8">
+        <v>3.5756065178476986</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A91" s="5">
         <v>88</v>
       </c>
-      <c r="B91" s="8">
+      <c r="B91" s="5">
         <v>8360</v>
       </c>
-      <c r="C91" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D91" s="8">
-        <v>3</v>
-      </c>
-      <c r="E91" s="8">
+      <c r="C91" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D91" s="5">
+        <v>3</v>
+      </c>
+      <c r="E91" s="5">
         <v>5</v>
       </c>
       <c r="F91">
         <f t="shared" si="2"/>
         <v>17.977000193201071</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A92" s="8">
+      <c r="G91" s="8">
+        <v>3.5954000386402143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A92" s="5">
         <v>89</v>
       </c>
-      <c r="B92" s="8">
+      <c r="B92" s="5">
         <v>8455</v>
       </c>
-      <c r="C92" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D92" s="8">
-        <v>3</v>
-      </c>
-      <c r="E92" s="8">
+      <c r="C92" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D92" s="5">
+        <v>3</v>
+      </c>
+      <c r="E92" s="5">
         <v>5</v>
       </c>
       <c r="F92">
         <f t="shared" si="2"/>
         <v>18.075533718961573</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A93" s="8">
+      <c r="G92" s="8">
+        <v>3.6151067437923148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A93" s="5">
         <v>90</v>
       </c>
-      <c r="B93" s="8">
+      <c r="B93" s="5">
         <v>9000</v>
       </c>
-      <c r="C93" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D93" s="8">
-        <v>3</v>
-      </c>
-      <c r="E93" s="8">
+      <c r="C93" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D93" s="5">
+        <v>3</v>
+      </c>
+      <c r="E93" s="5">
         <v>5</v>
       </c>
       <c r="F93">
         <f t="shared" si="2"/>
         <v>18.173639757979167</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A94" s="8">
+      <c r="G93" s="8">
+        <v>3.6347279515958335</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A94" s="5">
         <v>91</v>
       </c>
-      <c r="B94" s="8">
+      <c r="B94" s="5">
         <v>9100</v>
       </c>
-      <c r="C94" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D94" s="8">
-        <v>3</v>
-      </c>
-      <c r="E94" s="8">
+      <c r="C94" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D94" s="5">
+        <v>3</v>
+      </c>
+      <c r="E94" s="5">
         <v>5</v>
       </c>
       <c r="F94">
         <f t="shared" si="2"/>
         <v>18.271324731966914</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A95" s="8">
+      <c r="G94" s="8">
+        <v>3.6542649463933827</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A95" s="5">
         <v>92</v>
       </c>
-      <c r="B95" s="8">
+      <c r="B95" s="5">
         <v>9200</v>
       </c>
-      <c r="C95" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D95" s="8">
-        <v>3</v>
-      </c>
-      <c r="E95" s="8">
+      <c r="C95" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D95" s="5">
+        <v>3</v>
+      </c>
+      <c r="E95" s="5">
         <v>5</v>
       </c>
       <c r="F95">
         <f t="shared" si="2"/>
         <v>18.368594899018895</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A96" s="8">
+      <c r="G95" s="8">
+        <v>3.673718979803779</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A96" s="5">
         <v>93</v>
       </c>
-      <c r="B96" s="8">
+      <c r="B96" s="5">
         <v>9300</v>
       </c>
-      <c r="C96" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D96" s="8">
-        <v>3</v>
-      </c>
-      <c r="E96" s="8">
+      <c r="C96" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D96" s="5">
+        <v>3</v>
+      </c>
+      <c r="E96" s="5">
         <v>5</v>
       </c>
       <c r="F96">
         <f t="shared" si="2"/>
         <v>18.465456359454102</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A97" s="8">
+      <c r="G96" s="8">
+        <v>3.6930912718908204</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A97" s="5">
         <v>94</v>
       </c>
-      <c r="B97" s="8">
+      <c r="B97" s="5">
         <v>9400</v>
       </c>
-      <c r="C97" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D97" s="8">
-        <v>3</v>
-      </c>
-      <c r="E97" s="8">
+      <c r="C97" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D97" s="5">
+        <v>3</v>
+      </c>
+      <c r="E97" s="5">
         <v>5</v>
       </c>
       <c r="F97">
         <f t="shared" si="2"/>
         <v>18.561915061393066</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A98" s="8">
+      <c r="G97" s="8">
+        <v>3.7123830122786132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A98" s="5">
         <v>95</v>
       </c>
-      <c r="B98" s="8">
+      <c r="B98" s="5">
         <v>9975</v>
       </c>
-      <c r="C98" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D98" s="8">
-        <v>3</v>
-      </c>
-      <c r="E98" s="8">
+      <c r="C98" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D98" s="5">
+        <v>3</v>
+      </c>
+      <c r="E98" s="5">
         <v>5</v>
       </c>
       <c r="F98">
         <f t="shared" si="2"/>
         <v>18.657976806082026</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A99" s="8">
+      <c r="G98" s="8">
+        <v>3.7315953612164052</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A99" s="5">
         <v>96</v>
       </c>
-      <c r="B99" s="8">
+      <c r="B99" s="5">
         <v>10080</v>
       </c>
-      <c r="C99" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D99" s="8">
-        <v>3</v>
-      </c>
-      <c r="E99" s="8">
+      <c r="C99" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D99" s="5">
+        <v>3</v>
+      </c>
+      <c r="E99" s="5">
         <v>5</v>
       </c>
       <c r="F99">
         <f t="shared" si="2"/>
         <v>18.75364725297846</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A100" s="8">
+      <c r="G99" s="8">
+        <v>3.7507294505956921</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A100" s="5">
         <v>97</v>
       </c>
-      <c r="B100" s="8">
+      <c r="B100" s="5">
         <v>10185</v>
       </c>
-      <c r="C100" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D100" s="8">
-        <v>3</v>
-      </c>
-      <c r="E100" s="8">
+      <c r="C100" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D100" s="5">
+        <v>3</v>
+      </c>
+      <c r="E100" s="5">
         <v>5</v>
       </c>
       <c r="F100">
         <f t="shared" si="2"/>
         <v>18.848931924611136</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A101" s="8">
+      <c r="G100" s="8">
+        <v>3.7697863849222273</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A101" s="5">
         <v>98</v>
       </c>
-      <c r="B101" s="8">
+      <c r="B101" s="5">
         <v>10290</v>
       </c>
-      <c r="C101" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D101" s="8">
-        <v>3</v>
-      </c>
-      <c r="E101" s="8">
+      <c r="C101" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D101" s="5">
+        <v>3</v>
+      </c>
+      <c r="E101" s="5">
         <v>5</v>
       </c>
       <c r="F101">
         <f t="shared" si="2"/>
         <v>18.9438362112266</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A102" s="8">
+      <c r="G101" s="8">
+        <v>3.7887672422453198</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A102" s="5">
         <v>99</v>
       </c>
-      <c r="B102" s="8">
+      <c r="B102" s="5">
         <v>10395</v>
       </c>
-      <c r="C102" s="8">
-        <v>999999</v>
-      </c>
-      <c r="D102" s="8">
-        <v>3</v>
-      </c>
-      <c r="E102" s="8">
+      <c r="C102" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D102" s="5">
+        <v>3</v>
+      </c>
+      <c r="E102" s="5">
         <v>5</v>
       </c>
       <c r="F102">
         <f t="shared" si="2"/>
         <v>19.038365375233763</v>
+      </c>
+      <c r="G102" s="8">
+        <v>3.8076730750467527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a deckview show bug on card level up
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1088,74 +1088,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1193,7 +1125,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1508,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2008,7 +1940,7 @@
         <v>999999</v>
       </c>
       <c r="D21" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="5">
         <v>3</v>
@@ -2032,7 +1964,7 @@
         <v>999999</v>
       </c>
       <c r="D22" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="5">
         <v>3</v>
@@ -2056,7 +1988,7 @@
         <v>999999</v>
       </c>
       <c r="D23" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23" s="5">
         <v>4</v>
@@ -2080,7 +2012,7 @@
         <v>999999</v>
       </c>
       <c r="D24" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" s="5">
         <v>4</v>
@@ -2104,7 +2036,7 @@
         <v>999999</v>
       </c>
       <c r="D25" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" s="5">
         <v>4</v>
@@ -2128,7 +2060,7 @@
         <v>999999</v>
       </c>
       <c r="D26" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26" s="5">
         <v>4</v>
@@ -2152,7 +2084,7 @@
         <v>999999</v>
       </c>
       <c r="D27" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E27" s="5">
         <v>4</v>
@@ -2176,7 +2108,7 @@
         <v>999999</v>
       </c>
       <c r="D28" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28" s="5">
         <v>4</v>
@@ -2200,7 +2132,7 @@
         <v>999999</v>
       </c>
       <c r="D29" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E29" s="5">
         <v>4</v>
@@ -2224,7 +2156,7 @@
         <v>999999</v>
       </c>
       <c r="D30" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E30" s="5">
         <v>4</v>
@@ -2248,7 +2180,7 @@
         <v>999999</v>
       </c>
       <c r="D31" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E31" s="5">
         <v>4</v>
@@ -2272,7 +2204,7 @@
         <v>999999</v>
       </c>
       <c r="D32" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E32" s="5">
         <v>5</v>
@@ -2296,7 +2228,7 @@
         <v>999999</v>
       </c>
       <c r="D33" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E33" s="5">
         <v>5</v>
@@ -2320,7 +2252,7 @@
         <v>999999</v>
       </c>
       <c r="D34" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E34" s="5">
         <v>5</v>
@@ -2344,7 +2276,7 @@
         <v>999999</v>
       </c>
       <c r="D35" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E35" s="5">
         <v>5</v>
@@ -2368,7 +2300,7 @@
         <v>999999</v>
       </c>
       <c r="D36" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E36" s="5">
         <v>5</v>
@@ -2392,7 +2324,7 @@
         <v>999999</v>
       </c>
       <c r="D37" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E37" s="5">
         <v>5</v>
@@ -2416,7 +2348,7 @@
         <v>999999</v>
       </c>
       <c r="D38" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E38" s="5">
         <v>5</v>
@@ -2440,7 +2372,7 @@
         <v>999999</v>
       </c>
       <c r="D39" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E39" s="5">
         <v>5</v>
@@ -2464,7 +2396,7 @@
         <v>999999</v>
       </c>
       <c r="D40" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E40" s="5">
         <v>5</v>
@@ -2488,7 +2420,7 @@
         <v>999999</v>
       </c>
       <c r="D41" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E41" s="5">
         <v>5</v>
@@ -2512,7 +2444,7 @@
         <v>999999</v>
       </c>
       <c r="D42" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E42" s="5">
         <v>5</v>
@@ -2536,7 +2468,7 @@
         <v>999999</v>
       </c>
       <c r="D43" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E43" s="5">
         <v>5</v>
@@ -2560,7 +2492,7 @@
         <v>999999</v>
       </c>
       <c r="D44" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E44" s="5">
         <v>5</v>
@@ -2584,7 +2516,7 @@
         <v>999999</v>
       </c>
       <c r="D45" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E45" s="5">
         <v>5</v>
@@ -2608,7 +2540,7 @@
         <v>999999</v>
       </c>
       <c r="D46" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E46" s="5">
         <v>5</v>
@@ -2632,7 +2564,7 @@
         <v>999999</v>
       </c>
       <c r="D47" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E47" s="5">
         <v>5</v>
@@ -2656,7 +2588,7 @@
         <v>999999</v>
       </c>
       <c r="D48" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E48" s="5">
         <v>5</v>
@@ -2680,7 +2612,7 @@
         <v>999999</v>
       </c>
       <c r="D49" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E49" s="5">
         <v>5</v>
@@ -2704,7 +2636,7 @@
         <v>999999</v>
       </c>
       <c r="D50" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E50" s="5">
         <v>5</v>
@@ -2728,7 +2660,7 @@
         <v>999999</v>
       </c>
       <c r="D51" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E51" s="5">
         <v>5</v>
@@ -2752,7 +2684,7 @@
         <v>999999</v>
       </c>
       <c r="D52" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E52" s="5">
         <v>5</v>
@@ -2776,7 +2708,7 @@
         <v>999999</v>
       </c>
       <c r="D53" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E53" s="5">
         <v>5</v>
@@ -2800,7 +2732,7 @@
         <v>999999</v>
       </c>
       <c r="D54" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E54" s="5">
         <v>5</v>
@@ -2824,7 +2756,7 @@
         <v>999999</v>
       </c>
       <c r="D55" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E55" s="5">
         <v>5</v>
@@ -2848,7 +2780,7 @@
         <v>999999</v>
       </c>
       <c r="D56" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E56" s="5">
         <v>5</v>
@@ -2872,7 +2804,7 @@
         <v>999999</v>
       </c>
       <c r="D57" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E57" s="5">
         <v>5</v>
@@ -2896,7 +2828,7 @@
         <v>999999</v>
       </c>
       <c r="D58" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E58" s="5">
         <v>5</v>
@@ -2920,7 +2852,7 @@
         <v>999999</v>
       </c>
       <c r="D59" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E59" s="5">
         <v>5</v>
@@ -2944,7 +2876,7 @@
         <v>999999</v>
       </c>
       <c r="D60" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E60" s="5">
         <v>5</v>
@@ -2968,7 +2900,7 @@
         <v>999999</v>
       </c>
       <c r="D61" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E61" s="5">
         <v>5</v>
@@ -2992,7 +2924,7 @@
         <v>999999</v>
       </c>
       <c r="D62" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E62" s="5">
         <v>5</v>
@@ -3016,7 +2948,7 @@
         <v>999999</v>
       </c>
       <c r="D63" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E63" s="5">
         <v>5</v>
@@ -3040,7 +2972,7 @@
         <v>999999</v>
       </c>
       <c r="D64" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E64" s="5">
         <v>5</v>
@@ -3064,7 +2996,7 @@
         <v>999999</v>
       </c>
       <c r="D65" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E65" s="5">
         <v>5</v>
@@ -3088,7 +3020,7 @@
         <v>999999</v>
       </c>
       <c r="D66" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E66" s="5">
         <v>5</v>
@@ -3112,7 +3044,7 @@
         <v>999999</v>
       </c>
       <c r="D67" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E67" s="5">
         <v>5</v>
@@ -3136,7 +3068,7 @@
         <v>999999</v>
       </c>
       <c r="D68" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E68" s="5">
         <v>5</v>
@@ -3160,7 +3092,7 @@
         <v>999999</v>
       </c>
       <c r="D69" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E69" s="5">
         <v>5</v>
@@ -3184,7 +3116,7 @@
         <v>999999</v>
       </c>
       <c r="D70" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E70" s="5">
         <v>5</v>
@@ -3208,7 +3140,7 @@
         <v>999999</v>
       </c>
       <c r="D71" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E71" s="5">
         <v>5</v>
@@ -3232,7 +3164,7 @@
         <v>999999</v>
       </c>
       <c r="D72" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E72" s="5">
         <v>5</v>
@@ -3256,7 +3188,7 @@
         <v>999999</v>
       </c>
       <c r="D73" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E73" s="5">
         <v>5</v>
@@ -3280,7 +3212,7 @@
         <v>999999</v>
       </c>
       <c r="D74" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E74" s="5">
         <v>5</v>
@@ -3304,7 +3236,7 @@
         <v>999999</v>
       </c>
       <c r="D75" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E75" s="5">
         <v>5</v>
@@ -3328,7 +3260,7 @@
         <v>999999</v>
       </c>
       <c r="D76" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E76" s="5">
         <v>5</v>
@@ -3352,7 +3284,7 @@
         <v>999999</v>
       </c>
       <c r="D77" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E77" s="5">
         <v>5</v>
@@ -3376,7 +3308,7 @@
         <v>999999</v>
       </c>
       <c r="D78" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E78" s="5">
         <v>5</v>
@@ -3400,7 +3332,7 @@
         <v>999999</v>
       </c>
       <c r="D79" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E79" s="5">
         <v>5</v>
@@ -3424,7 +3356,7 @@
         <v>999999</v>
       </c>
       <c r="D80" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E80" s="5">
         <v>5</v>
@@ -3448,7 +3380,7 @@
         <v>999999</v>
       </c>
       <c r="D81" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E81" s="5">
         <v>5</v>
@@ -3472,7 +3404,7 @@
         <v>999999</v>
       </c>
       <c r="D82" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E82" s="5">
         <v>5</v>
@@ -3496,7 +3428,7 @@
         <v>999999</v>
       </c>
       <c r="D83" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E83" s="5">
         <v>5</v>
@@ -3520,7 +3452,7 @@
         <v>999999</v>
       </c>
       <c r="D84" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E84" s="5">
         <v>5</v>
@@ -3544,7 +3476,7 @@
         <v>999999</v>
       </c>
       <c r="D85" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E85" s="5">
         <v>5</v>
@@ -3568,7 +3500,7 @@
         <v>999999</v>
       </c>
       <c r="D86" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E86" s="5">
         <v>5</v>
@@ -3592,7 +3524,7 @@
         <v>999999</v>
       </c>
       <c r="D87" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E87" s="5">
         <v>5</v>
@@ -3616,7 +3548,7 @@
         <v>999999</v>
       </c>
       <c r="D88" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E88" s="5">
         <v>5</v>
@@ -3640,7 +3572,7 @@
         <v>999999</v>
       </c>
       <c r="D89" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E89" s="5">
         <v>5</v>
@@ -3664,7 +3596,7 @@
         <v>999999</v>
       </c>
       <c r="D90" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E90" s="5">
         <v>5</v>
@@ -3688,7 +3620,7 @@
         <v>999999</v>
       </c>
       <c r="D91" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E91" s="5">
         <v>5</v>
@@ -3712,7 +3644,7 @@
         <v>999999</v>
       </c>
       <c r="D92" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E92" s="5">
         <v>5</v>
@@ -3736,7 +3668,7 @@
         <v>999999</v>
       </c>
       <c r="D93" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E93" s="5">
         <v>5</v>
@@ -3760,7 +3692,7 @@
         <v>999999</v>
       </c>
       <c r="D94" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E94" s="5">
         <v>5</v>
@@ -3784,7 +3716,7 @@
         <v>999999</v>
       </c>
       <c r="D95" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E95" s="5">
         <v>5</v>
@@ -3808,7 +3740,7 @@
         <v>999999</v>
       </c>
       <c r="D96" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E96" s="5">
         <v>5</v>
@@ -3832,7 +3764,7 @@
         <v>999999</v>
       </c>
       <c r="D97" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E97" s="5">
         <v>5</v>
@@ -3856,7 +3788,7 @@
         <v>999999</v>
       </c>
       <c r="D98" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E98" s="5">
         <v>5</v>
@@ -3880,7 +3812,7 @@
         <v>999999</v>
       </c>
       <c r="D99" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E99" s="5">
         <v>5</v>
@@ -3904,7 +3836,7 @@
         <v>999999</v>
       </c>
       <c r="D100" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E100" s="5">
         <v>5</v>
@@ -3928,7 +3860,7 @@
         <v>999999</v>
       </c>
       <c r="D101" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E101" s="5">
         <v>5</v>
@@ -3952,7 +3884,7 @@
         <v>999999</v>
       </c>
       <c r="D102" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E102" s="5">
         <v>5</v>

</xml_diff>

<commit_message>
optimise the levelup exp cost, and card level of ai
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -59,14 +59,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>HeroSkillLevel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>英雄技能等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>资源曲线</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -84,6 +76,14 @@
   </si>
   <si>
     <t>金币曲线</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物卡等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardLevel</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1110,8 +1110,10 @@
     <tableColumn id="1" name="Id" dataDxfId="6"/>
     <tableColumn id="2" name="Exp" dataDxfId="5"/>
     <tableColumn id="3" name="CardExp" dataDxfId="4"/>
-    <tableColumn id="4" name="TowerLevel" dataDxfId="3"/>
-    <tableColumn id="5" name="HeroSkillLevel" dataDxfId="2"/>
+    <tableColumn id="4" name="TowerLevel" dataDxfId="3">
+      <calculatedColumnFormula>INT(E4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="CardLevel" dataDxfId="2"/>
     <tableColumn id="6" name="GoldFactor" dataDxfId="1">
       <calculatedColumnFormula>POWER(A4+3,0.6)+3</calculatedColumnFormula>
     </tableColumn>
@@ -1445,13 +1447,14 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B7" sqref="B7:B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="5" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1468,13 +1471,13 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -1491,13 +1494,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1514,13 +1517,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1534,6 +1537,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="5">
+        <f>INT(E4)</f>
         <v>1</v>
       </c>
       <c r="E4" s="5">
@@ -1558,13 +1562,14 @@
         <v>4</v>
       </c>
       <c r="D5" s="5">
+        <f t="shared" ref="D5:D68" si="0">INT(E5)</f>
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F68" si="0">POWER(A5+3,0.6)+3</f>
+        <f t="shared" ref="F5:F68" si="1">POWER(A5+3,0.6)+3</f>
         <v>5.626527804403767</v>
       </c>
       <c r="G5" s="8">
@@ -1576,19 +1581,20 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4">
         <v>10</v>
       </c>
       <c r="D6" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E6" s="5">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.9301560515835217</v>
       </c>
       <c r="G6" s="8">
@@ -1600,19 +1606,21 @@
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>50</v>
+        <f>INT(B6*0.7+A7*10+A7*A7*3-30)</f>
+        <v>93</v>
       </c>
       <c r="C7" s="4">
         <v>20</v>
       </c>
       <c r="D7" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E7" s="5">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2140958497160383</v>
       </c>
       <c r="G7" s="8">
@@ -1624,19 +1632,21 @@
         <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>85</v>
+        <f t="shared" ref="B8:B71" si="2">INT(B7*0.7+A8*10+A8*A8*3-30)</f>
+        <v>160</v>
       </c>
       <c r="C8" s="4">
         <v>40</v>
       </c>
       <c r="D8" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4822022531844965</v>
       </c>
       <c r="G8" s="8">
@@ -1648,19 +1658,21 @@
         <v>6</v>
       </c>
       <c r="B9" s="4">
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>250</v>
       </c>
       <c r="C9" s="4">
         <v>80</v>
       </c>
       <c r="D9" s="5">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.7371928188465517</v>
       </c>
       <c r="G9" s="8">
@@ -1672,19 +1684,21 @@
         <v>7</v>
       </c>
       <c r="B10" s="4">
-        <v>115</v>
+        <f t="shared" si="2"/>
+        <v>362</v>
       </c>
       <c r="C10" s="4">
         <v>200</v>
       </c>
       <c r="D10" s="5">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E10" s="5">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9810717055349727</v>
       </c>
       <c r="G10" s="8">
@@ -1696,20 +1710,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="4">
-        <v>130</v>
+        <f t="shared" si="2"/>
+        <v>495</v>
       </c>
       <c r="C11" s="4">
         <f>C10+500</f>
         <v>700</v>
       </c>
       <c r="D11" s="5">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E11" s="5">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.2153691330919001</v>
       </c>
       <c r="G11" s="8">
@@ -1721,20 +1737,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="4">
-        <v>145</v>
+        <f t="shared" si="2"/>
+        <v>649</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" ref="C12" si="1">C11+500</f>
+        <f t="shared" ref="C12" si="3">C11+500</f>
         <v>1200</v>
       </c>
       <c r="D12" s="5">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E12" s="5">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4412860698458401</v>
       </c>
       <c r="G12" s="8">
@@ -1745,20 +1763,22 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="5">
-        <v>200</v>
+      <c r="B13" s="4">
+        <f t="shared" si="2"/>
+        <v>824</v>
       </c>
       <c r="C13" s="5">
         <v>999999</v>
       </c>
       <c r="D13" s="5">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E13" s="5">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6597864200360659</v>
       </c>
       <c r="G13" s="8">
@@ -1769,20 +1789,22 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="5">
-        <v>220</v>
+      <c r="B14" s="4">
+        <f t="shared" si="2"/>
+        <v>1019</v>
       </c>
       <c r="C14" s="5">
         <v>999999</v>
       </c>
       <c r="D14" s="5">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E14" s="5">
         <v>2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8716583257669139</v>
       </c>
       <c r="G14" s="8">
@@ -1793,20 +1815,22 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="5">
-        <v>240</v>
+      <c r="B15" s="4">
+        <f t="shared" si="2"/>
+        <v>1235</v>
       </c>
       <c r="C15" s="5">
         <v>999999</v>
       </c>
       <c r="D15" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E15" s="5">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0775563919874074</v>
       </c>
       <c r="G15" s="8">
@@ -1817,20 +1841,22 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="5">
-        <v>260</v>
+      <c r="B16" s="4">
+        <f t="shared" si="2"/>
+        <v>1471</v>
       </c>
       <c r="C16" s="5">
         <v>999999</v>
       </c>
       <c r="D16" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E16" s="5">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.2780316430915768</v>
       </c>
       <c r="G16" s="8">
@@ -1841,20 +1867,22 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="5">
-        <v>280</v>
+      <c r="B17" s="4">
+        <f t="shared" si="2"/>
+        <v>1727</v>
       </c>
       <c r="C17" s="5">
         <v>999999</v>
       </c>
       <c r="D17" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E17" s="5">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.4735533169184887</v>
       </c>
       <c r="G17" s="8">
@@ -1865,20 +1893,22 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="5">
-        <v>375</v>
+      <c r="B18" s="4">
+        <f t="shared" si="2"/>
+        <v>2003</v>
       </c>
       <c r="C18" s="5">
         <v>999999</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E18" s="5">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6645250677694108</v>
       </c>
       <c r="G18" s="8">
@@ -1889,20 +1919,22 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="5">
-        <v>400</v>
+      <c r="B19" s="4">
+        <f t="shared" si="2"/>
+        <v>2300</v>
       </c>
       <c r="C19" s="5">
         <v>999999</v>
       </c>
       <c r="D19" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E19" s="5">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.8512972424092151</v>
       </c>
       <c r="G19" s="8">
@@ -1913,20 +1945,22 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="5">
-        <v>425</v>
+      <c r="B20" s="4">
+        <f t="shared" si="2"/>
+        <v>2617</v>
       </c>
       <c r="C20" s="5">
         <v>999999</v>
       </c>
       <c r="D20" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E20" s="5">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0341763365451619</v>
       </c>
       <c r="G20" s="8">
@@ -1937,20 +1971,22 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="B21" s="5">
-        <v>450</v>
+      <c r="B21" s="4">
+        <f t="shared" si="2"/>
+        <v>2953</v>
       </c>
       <c r="C21" s="5">
         <v>999999</v>
       </c>
       <c r="D21" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E21" s="5">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2134323873607435</v>
       </c>
       <c r="G21" s="8">
@@ -1961,20 +1997,22 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="B22" s="5">
-        <v>475</v>
+      <c r="B22" s="4">
+        <f t="shared" si="2"/>
+        <v>3310</v>
       </c>
       <c r="C22" s="5">
         <v>999999</v>
       </c>
       <c r="D22" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E22" s="5">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.3893048289839669</v>
       </c>
       <c r="G22" s="8">
@@ -1985,20 +2023,22 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="B23" s="5">
-        <v>600</v>
+      <c r="B23" s="4">
+        <f t="shared" si="2"/>
+        <v>3687</v>
       </c>
       <c r="C23" s="5">
         <v>999999</v>
       </c>
       <c r="D23" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E23" s="5">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.5620071855158546</v>
       </c>
       <c r="G23" s="8">
@@ -2009,20 +2049,23 @@
       <c r="A24" s="5">
         <v>21</v>
       </c>
-      <c r="B24" s="5">
-        <v>630</v>
+      <c r="B24" s="4">
+        <f t="shared" si="2"/>
+        <v>4083</v>
       </c>
       <c r="C24" s="5">
         <v>999999</v>
       </c>
       <c r="D24" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E24" s="5">
-        <v>4</v>
+        <f>3.3+(A24-21)*0.1-E23*0.12</f>
+        <v>2.952</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.7317308726771969</v>
       </c>
       <c r="G24" s="8">
@@ -2033,20 +2076,23 @@
       <c r="A25" s="5">
         <v>22</v>
       </c>
-      <c r="B25" s="5">
-        <v>660</v>
+      <c r="B25" s="4">
+        <f t="shared" si="2"/>
+        <v>4500</v>
       </c>
       <c r="C25" s="5">
         <v>999999</v>
       </c>
       <c r="D25" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E25" s="5">
-        <v>4</v>
+        <f t="shared" ref="E25:E88" si="4">3.3+(A25-21)*0.1-E24*0.12</f>
+        <v>3.04576</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8986483073060718</v>
       </c>
       <c r="G25" s="8">
@@ -2057,20 +2103,23 @@
       <c r="A26" s="5">
         <v>23</v>
       </c>
-      <c r="B26" s="5">
-        <v>690</v>
+      <c r="B26" s="4">
+        <f t="shared" si="2"/>
+        <v>4937</v>
       </c>
       <c r="C26" s="5">
         <v>999999</v>
       </c>
       <c r="D26" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E26" s="5">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.1345087999999999</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.062915473248847</v>
       </c>
       <c r="G26" s="8">
@@ -2081,20 +2130,23 @@
       <c r="A27" s="5">
         <v>24</v>
       </c>
-      <c r="B27" s="5">
-        <v>720</v>
+      <c r="B27" s="4">
+        <f t="shared" si="2"/>
+        <v>5393</v>
       </c>
       <c r="C27" s="5">
         <v>999999</v>
       </c>
       <c r="D27" s="5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E27" s="5">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.2238589439999998</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.224674055842076</v>
       </c>
       <c r="G27" s="8">
@@ -2105,20 +2157,23 @@
       <c r="A28" s="5">
         <v>25</v>
       </c>
-      <c r="B28" s="5">
-        <v>875</v>
+      <c r="B28" s="4">
+        <f t="shared" si="2"/>
+        <v>5870</v>
       </c>
       <c r="C28" s="5">
         <v>999999</v>
       </c>
       <c r="D28" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E28" s="5">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.3131369267199999</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.38405323074322</v>
       </c>
       <c r="G28" s="8">
@@ -2129,20 +2184,23 @@
       <c r="A29" s="5">
         <v>26</v>
       </c>
-      <c r="B29" s="5">
-        <v>910</v>
+      <c r="B29" s="4">
+        <f t="shared" si="2"/>
+        <v>6367</v>
       </c>
       <c r="C29" s="5">
         <v>999999</v>
       </c>
       <c r="D29" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E29" s="5">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.4024235687936</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.541171173377641</v>
       </c>
       <c r="G29" s="8">
@@ -2153,20 +2211,23 @@
       <c r="A30" s="5">
         <v>27</v>
       </c>
-      <c r="B30" s="5">
-        <v>945</v>
+      <c r="B30" s="4">
+        <f t="shared" si="2"/>
+        <v>6883</v>
       </c>
       <c r="C30" s="5">
         <v>999999</v>
       </c>
       <c r="D30" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E30" s="5">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.4917091717447679</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.696136340726078</v>
       </c>
       <c r="G30" s="8">
@@ -2177,20 +2238,23 @@
       <c r="A31" s="5">
         <v>28</v>
       </c>
-      <c r="B31" s="5">
-        <v>980</v>
+      <c r="B31" s="4">
+        <f t="shared" si="2"/>
+        <v>7420</v>
       </c>
       <c r="C31" s="5">
         <v>999999</v>
       </c>
       <c r="D31" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E31" s="5">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.5809948993906278</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.849048566202034</v>
       </c>
       <c r="G31" s="8">
@@ -2201,20 +2265,23 @@
       <c r="A32" s="5">
         <v>29</v>
       </c>
-      <c r="B32" s="5">
-        <v>1015</v>
+      <c r="B32" s="4">
+        <f t="shared" si="2"/>
+        <v>7977</v>
       </c>
       <c r="C32" s="5">
         <v>999999</v>
       </c>
       <c r="D32" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E32" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>3.6702806120731242</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.999999999999998</v>
       </c>
       <c r="G32" s="8">
@@ -2225,20 +2292,23 @@
       <c r="A33" s="5">
         <v>30</v>
       </c>
-      <c r="B33" s="5">
-        <v>1200</v>
+      <c r="B33" s="4">
+        <f t="shared" si="2"/>
+        <v>8553</v>
       </c>
       <c r="C33" s="5">
         <v>999999</v>
       </c>
       <c r="D33" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E33" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>3.7595663265512251</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.149075920852829</v>
       </c>
       <c r="G33" s="8">
@@ -2249,20 +2319,23 @@
       <c r="A34" s="5">
         <v>31</v>
       </c>
-      <c r="B34" s="5">
-        <v>1240</v>
+      <c r="B34" s="4">
+        <f t="shared" si="2"/>
+        <v>9150</v>
       </c>
       <c r="C34" s="5">
         <v>999999</v>
       </c>
       <c r="D34" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E34" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>3.8488520408138527</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.296355440131292</v>
       </c>
       <c r="G34" s="8">
@@ -2273,20 +2346,23 @@
       <c r="A35" s="5">
         <v>32</v>
       </c>
-      <c r="B35" s="5">
-        <v>1280</v>
+      <c r="B35" s="4">
+        <f t="shared" si="2"/>
+        <v>9767</v>
       </c>
       <c r="C35" s="5">
         <v>999999</v>
       </c>
       <c r="D35" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E35" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>3.9381377551023382</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.441912115297924</v>
       </c>
       <c r="G35" s="8">
@@ -2297,20 +2373,23 @@
       <c r="A36" s="5">
         <v>33</v>
       </c>
-      <c r="B36" s="5">
-        <v>1320</v>
+      <c r="B36" s="4">
+        <f t="shared" si="2"/>
+        <v>10403</v>
       </c>
       <c r="C36" s="5">
         <v>999999</v>
       </c>
       <c r="D36" s="5">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E36" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.0274234693877196</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.585814486631531</v>
       </c>
       <c r="G36" s="8">
@@ -2321,20 +2400,23 @@
       <c r="A37" s="5">
         <v>34</v>
       </c>
-      <c r="B37" s="5">
-        <v>1360</v>
+      <c r="B37" s="4">
+        <f t="shared" si="2"/>
+        <v>11060</v>
       </c>
       <c r="C37" s="5">
         <v>999999</v>
       </c>
       <c r="D37" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E37" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.116709183673473</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.72812654867613</v>
       </c>
       <c r="G37" s="8">
@@ -2345,20 +2427,23 @@
       <c r="A38" s="5">
         <v>35</v>
       </c>
-      <c r="B38" s="5">
-        <v>1575</v>
+      <c r="B38" s="4">
+        <f t="shared" si="2"/>
+        <v>11737</v>
       </c>
       <c r="C38" s="5">
         <v>999999</v>
       </c>
       <c r="D38" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E38" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.205994897959183</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.868908165896258</v>
       </c>
       <c r="G38" s="8">
@@ -2369,20 +2454,23 @@
       <c r="A39" s="5">
         <v>36</v>
       </c>
-      <c r="B39" s="5">
-        <v>1620</v>
+      <c r="B39" s="4">
+        <f t="shared" si="2"/>
+        <v>12433</v>
       </c>
       <c r="C39" s="5">
         <v>999999</v>
       </c>
       <c r="D39" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E39" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.2952806122448983</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.008215440430581</v>
       </c>
       <c r="G39" s="8">
@@ -2393,20 +2481,23 @@
       <c r="A40" s="5">
         <v>37</v>
       </c>
-      <c r="B40" s="5">
-        <v>1665</v>
+      <c r="B40" s="4">
+        <f t="shared" si="2"/>
+        <v>13150</v>
       </c>
       <c r="C40" s="5">
         <v>999999</v>
       </c>
       <c r="D40" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E40" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.3845663265306127</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.146101038546524</v>
       </c>
       <c r="G40" s="8">
@@ -2417,20 +2508,23 @@
       <c r="A41" s="5">
         <v>38</v>
       </c>
-      <c r="B41" s="5">
-        <v>1710</v>
+      <c r="B41" s="4">
+        <f t="shared" si="2"/>
+        <v>13887</v>
       </c>
       <c r="C41" s="5">
         <v>999999</v>
       </c>
       <c r="D41" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E41" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.4738520408163263</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.282614481346684</v>
       </c>
       <c r="G41" s="8">
@@ -2441,20 +2535,23 @@
       <c r="A42" s="5">
         <v>39</v>
       </c>
-      <c r="B42" s="5">
-        <v>1755</v>
+      <c r="B42" s="4">
+        <f t="shared" si="2"/>
+        <v>14643</v>
       </c>
       <c r="C42" s="5">
         <v>999999</v>
       </c>
       <c r="D42" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E42" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.5631377551020407</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.41780240441493</v>
       </c>
       <c r="G42" s="8">
@@ -2465,20 +2562,23 @@
       <c r="A43" s="5">
         <v>40</v>
       </c>
-      <c r="B43" s="5">
-        <v>2000</v>
+      <c r="B43" s="4">
+        <f t="shared" si="2"/>
+        <v>15420</v>
       </c>
       <c r="C43" s="5">
         <v>999999</v>
       </c>
       <c r="D43" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E43" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.6524234693877551</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.551708790378902</v>
       </c>
       <c r="G43" s="8">
@@ -2489,20 +2589,23 @@
       <c r="A44" s="5">
         <v>41</v>
       </c>
-      <c r="B44" s="5">
-        <v>2050</v>
+      <c r="B44" s="4">
+        <f t="shared" si="2"/>
+        <v>16217</v>
       </c>
       <c r="C44" s="5">
         <v>999999</v>
       </c>
       <c r="D44" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E44" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.7417091836734695</v>
       </c>
       <c r="F44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.684375177775884</v>
       </c>
       <c r="G44" s="8">
@@ -2513,20 +2616,23 @@
       <c r="A45" s="5">
         <v>42</v>
       </c>
-      <c r="B45" s="5">
-        <v>2100</v>
+      <c r="B45" s="4">
+        <f t="shared" si="2"/>
+        <v>17033</v>
       </c>
       <c r="C45" s="5">
         <v>999999</v>
       </c>
       <c r="D45" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E45" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.8309948979591839</v>
       </c>
       <c r="F45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.81584084911856</v>
       </c>
       <c r="G45" s="8">
@@ -2537,20 +2643,23 @@
       <c r="A46" s="5">
         <v>43</v>
       </c>
-      <c r="B46" s="5">
-        <v>2150</v>
+      <c r="B46" s="4">
+        <f t="shared" si="2"/>
+        <v>17870</v>
       </c>
       <c r="C46" s="5">
         <v>999999</v>
       </c>
       <c r="D46" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E46" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4.9202806122448983</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.946143000646654</v>
       </c>
       <c r="G46" s="8">
@@ -2561,20 +2670,23 @@
       <c r="A47" s="5">
         <v>44</v>
       </c>
-      <c r="B47" s="5">
-        <v>2200</v>
+      <c r="B47" s="4">
+        <f t="shared" si="2"/>
+        <v>18727</v>
       </c>
       <c r="C47" s="5">
         <v>999999</v>
       </c>
       <c r="D47" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E47" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.0095663265306118</v>
       </c>
       <c r="F47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.075316895906047</v>
       </c>
       <c r="G47" s="8">
@@ -2585,20 +2697,23 @@
       <c r="A48" s="5">
         <v>45</v>
       </c>
-      <c r="B48" s="5">
-        <v>2475</v>
+      <c r="B48" s="4">
+        <f t="shared" si="2"/>
+        <v>19603</v>
       </c>
       <c r="C48" s="5">
         <v>999999</v>
       </c>
       <c r="D48" s="5">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E48" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.0988520408163271</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.203396005006329</v>
       </c>
       <c r="G48" s="8">
@@ -2609,20 +2724,23 @@
       <c r="A49" s="5">
         <v>46</v>
       </c>
-      <c r="B49" s="5">
-        <v>2530</v>
+      <c r="B49" s="4">
+        <f t="shared" si="2"/>
+        <v>20500</v>
       </c>
       <c r="C49" s="5">
         <v>999999</v>
       </c>
       <c r="D49" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E49" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.1881377551020407</v>
       </c>
       <c r="F49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.330412131161864</v>
       </c>
       <c r="G49" s="8">
@@ -2633,20 +2751,23 @@
       <c r="A50" s="5">
         <v>47</v>
       </c>
-      <c r="B50" s="5">
-        <v>2585</v>
+      <c r="B50" s="4">
+        <f t="shared" si="2"/>
+        <v>21417</v>
       </c>
       <c r="C50" s="5">
         <v>999999</v>
       </c>
       <c r="D50" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E50" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.277423469387756</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.456395525912733</v>
       </c>
       <c r="G50" s="8">
@@ -2657,20 +2778,23 @@
       <c r="A51" s="5">
         <v>48</v>
       </c>
-      <c r="B51" s="5">
-        <v>2640</v>
+      <c r="B51" s="4">
+        <f t="shared" si="2"/>
+        <v>22353</v>
       </c>
       <c r="C51" s="5">
         <v>999999</v>
       </c>
       <c r="D51" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E51" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.3667091836734695</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.581374994243514</v>
       </c>
       <c r="G51" s="8">
@@ -2681,20 +2805,23 @@
       <c r="A52" s="5">
         <v>49</v>
       </c>
-      <c r="B52" s="5">
-        <v>2695</v>
+      <c r="B52" s="4">
+        <f t="shared" si="2"/>
+        <v>23310</v>
       </c>
       <c r="C52" s="5">
         <v>999999</v>
       </c>
       <c r="D52" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E52" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.455994897959183</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.705377990665905</v>
       </c>
       <c r="G52" s="8">
@@ -2705,20 +2832,23 @@
       <c r="A53" s="5">
         <v>50</v>
       </c>
-      <c r="B53" s="5">
-        <v>3000</v>
+      <c r="B53" s="4">
+        <f t="shared" si="2"/>
+        <v>24287</v>
       </c>
       <c r="C53" s="5">
         <v>999999</v>
       </c>
       <c r="D53" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E53" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.5452806122448983</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.828430707200107</v>
       </c>
       <c r="G53" s="8">
@@ -2729,20 +2859,23 @@
       <c r="A54" s="5">
         <v>51</v>
       </c>
-      <c r="B54" s="5">
-        <v>3060</v>
+      <c r="B54" s="4">
+        <f t="shared" si="2"/>
+        <v>25283</v>
       </c>
       <c r="C54" s="5">
         <v>999999</v>
       </c>
       <c r="D54" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E54" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.6345663265306118</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.950558154077704</v>
       </c>
       <c r="G54" s="8">
@@ -2753,20 +2886,23 @@
       <c r="A55" s="5">
         <v>52</v>
       </c>
-      <c r="B55" s="5">
-        <v>3120</v>
+      <c r="B55" s="4">
+        <f t="shared" si="2"/>
+        <v>26300</v>
       </c>
       <c r="C55" s="5">
         <v>999999</v>
       </c>
       <c r="D55" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E55" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.7238520408163271</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.071784233891282</v>
       </c>
       <c r="G55" s="8">
@@ -2777,20 +2913,23 @@
       <c r="A56" s="5">
         <v>53</v>
       </c>
-      <c r="B56" s="5">
-        <v>3180</v>
+      <c r="B56" s="4">
+        <f t="shared" si="2"/>
+        <v>27337</v>
       </c>
       <c r="C56" s="5">
         <v>999999</v>
       </c>
       <c r="D56" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E56" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.8131377551020407</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.192131809832132</v>
       </c>
       <c r="G56" s="8">
@@ -2801,20 +2940,23 @@
       <c r="A57" s="5">
         <v>54</v>
       </c>
-      <c r="B57" s="5">
-        <v>3240</v>
+      <c r="B57" s="4">
+        <f t="shared" si="2"/>
+        <v>28393</v>
       </c>
       <c r="C57" s="5">
         <v>999999</v>
       </c>
       <c r="D57" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E57" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.9024234693877551</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.311622768584231</v>
       </c>
       <c r="G57" s="8">
@@ -2825,20 +2967,23 @@
       <c r="A58" s="5">
         <v>55</v>
       </c>
-      <c r="B58" s="5">
-        <v>3575</v>
+      <c r="B58" s="4">
+        <f t="shared" si="2"/>
+        <v>29470</v>
       </c>
       <c r="C58" s="5">
         <v>999999</v>
       </c>
       <c r="D58" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E58" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>5.9917091836734695</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.430278078379143</v>
       </c>
       <c r="G58" s="8">
@@ -2849,20 +2994,23 @@
       <c r="A59" s="5">
         <v>56</v>
       </c>
-      <c r="B59" s="5">
-        <v>3640</v>
+      <c r="B59" s="4">
+        <f t="shared" si="2"/>
+        <v>30567</v>
       </c>
       <c r="C59" s="5">
         <v>999999</v>
       </c>
       <c r="D59" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E59" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.080994897959183</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.548117842660861</v>
       </c>
       <c r="G59" s="8">
@@ -2873,20 +3021,23 @@
       <c r="A60" s="5">
         <v>57</v>
       </c>
-      <c r="B60" s="5">
-        <v>3705</v>
+      <c r="B60" s="4">
+        <f t="shared" si="2"/>
+        <v>31683</v>
       </c>
       <c r="C60" s="5">
         <v>999999</v>
       </c>
       <c r="D60" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E60" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.1702806122448983</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.665161349761227</v>
       </c>
       <c r="G60" s="8">
@@ -2897,20 +3048,23 @@
       <c r="A61" s="5">
         <v>58</v>
       </c>
-      <c r="B61" s="5">
-        <v>3770</v>
+      <c r="B61" s="4">
+        <f t="shared" si="2"/>
+        <v>32820</v>
       </c>
       <c r="C61" s="5">
         <v>999999</v>
       </c>
       <c r="D61" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E61" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.2595663265306118</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.781427118943885</v>
       </c>
       <c r="G61" s="8">
@@ -2921,20 +3075,23 @@
       <c r="A62" s="5">
         <v>59</v>
       </c>
-      <c r="B62" s="5">
-        <v>3835</v>
+      <c r="B62" s="4">
+        <f t="shared" si="2"/>
+        <v>33977</v>
       </c>
       <c r="C62" s="5">
         <v>999999</v>
       </c>
       <c r="D62" s="5">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E62" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.3488520408163263</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.896932943137111</v>
       </c>
       <c r="G62" s="8">
@@ -2945,20 +3102,23 @@
       <c r="A63" s="5">
         <v>60</v>
       </c>
-      <c r="B63" s="5">
-        <v>4200</v>
+      <c r="B63" s="4">
+        <f t="shared" si="2"/>
+        <v>35153</v>
       </c>
       <c r="C63" s="5">
         <v>999999</v>
       </c>
       <c r="D63" s="5">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E63" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.4381377551020407</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.011695928643283</v>
       </c>
       <c r="G63" s="8">
@@ -2969,20 +3129,23 @@
       <c r="A64" s="5">
         <v>61</v>
       </c>
-      <c r="B64" s="5">
-        <v>4270</v>
+      <c r="B64" s="4">
+        <f t="shared" si="2"/>
+        <v>36350</v>
       </c>
       <c r="C64" s="5">
         <v>999999</v>
       </c>
       <c r="D64" s="5">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E64" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.5274234693877551</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.125732532083184</v>
       </c>
       <c r="G64" s="8">
@@ -2993,20 +3156,23 @@
       <c r="A65" s="5">
         <v>62</v>
       </c>
-      <c r="B65" s="5">
-        <v>4340</v>
+      <c r="B65" s="4">
+        <f t="shared" si="2"/>
+        <v>37567</v>
       </c>
       <c r="C65" s="5">
         <v>999999</v>
       </c>
       <c r="D65" s="5">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E65" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.6167091836734695</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.239058594807814</v>
       </c>
       <c r="G65" s="8">
@@ -3017,20 +3183,23 @@
       <c r="A66" s="5">
         <v>63</v>
       </c>
-      <c r="B66" s="5">
-        <v>4410</v>
+      <c r="B66" s="4">
+        <f t="shared" si="2"/>
+        <v>38803</v>
       </c>
       <c r="C66" s="5">
         <v>999999</v>
       </c>
       <c r="D66" s="5">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E66" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.7059948979591839</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.351689374987611</v>
       </c>
       <c r="G66" s="8">
@@ -3041,20 +3210,23 @@
       <c r="A67" s="5">
         <v>64</v>
       </c>
-      <c r="B67" s="5">
-        <v>4480</v>
+      <c r="B67" s="4">
+        <f t="shared" si="2"/>
+        <v>40060</v>
       </c>
       <c r="C67" s="5">
         <v>999999</v>
       </c>
       <c r="D67" s="5">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E67" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.7952806122448974</v>
       </c>
       <c r="F67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.463639577568394</v>
       </c>
       <c r="G67" s="8">
@@ -3065,20 +3237,23 @@
       <c r="A68" s="5">
         <v>65</v>
       </c>
-      <c r="B68" s="5">
-        <v>4875</v>
+      <c r="B68" s="4">
+        <f t="shared" si="2"/>
+        <v>41337</v>
       </c>
       <c r="C68" s="5">
         <v>999999</v>
       </c>
       <c r="D68" s="5">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E68" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.8845663265306127</v>
       </c>
       <c r="F68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.574923382265665</v>
       </c>
       <c r="G68" s="8">
@@ -3089,20 +3264,23 @@
       <c r="A69" s="5">
         <v>66</v>
       </c>
-      <c r="B69" s="5">
-        <v>4950</v>
+      <c r="B69" s="4">
+        <f t="shared" si="2"/>
+        <v>42633</v>
       </c>
       <c r="C69" s="5">
         <v>999999</v>
       </c>
       <c r="D69" s="5">
-        <v>8</v>
+        <f t="shared" ref="D69:D102" si="5">INT(E69)</f>
+        <v>6</v>
       </c>
       <c r="E69" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6.9738520408163263</v>
       </c>
       <c r="F69">
-        <f t="shared" ref="F69:F102" si="2">POWER(A69+3,0.6)+3</f>
+        <f t="shared" ref="F69:F102" si="6">POWER(A69+3,0.6)+3</f>
         <v>15.685554469752462</v>
       </c>
       <c r="G69" s="8">
@@ -3113,20 +3291,23 @@
       <c r="A70" s="5">
         <v>67</v>
       </c>
-      <c r="B70" s="5">
-        <v>5025</v>
+      <c r="B70" s="4">
+        <f t="shared" si="2"/>
+        <v>43950</v>
       </c>
       <c r="C70" s="5">
         <v>999999</v>
       </c>
       <c r="D70" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E70" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.0631377551020416</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>15.79554604618191</v>
       </c>
       <c r="G70" s="8">
@@ -3137,20 +3318,23 @@
       <c r="A71" s="5">
         <v>68</v>
       </c>
-      <c r="B71" s="5">
-        <v>5100</v>
+      <c r="B71" s="4">
+        <f t="shared" si="2"/>
+        <v>45287</v>
       </c>
       <c r="C71" s="5">
         <v>999999</v>
       </c>
       <c r="D71" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E71" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.1524234693877551</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>15.904910866172429</v>
       </c>
       <c r="G71" s="8">
@@ -3161,20 +3345,23 @@
       <c r="A72" s="5">
         <v>69</v>
       </c>
-      <c r="B72" s="5">
-        <v>5175</v>
+      <c r="B72" s="4">
+        <f t="shared" ref="B72:B102" si="7">INT(B71*0.7+A72*10+A72*A72*3-30)</f>
+        <v>46643</v>
       </c>
       <c r="C72" s="5">
         <v>999999</v>
       </c>
       <c r="D72" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E72" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.2417091836734713</v>
       </c>
       <c r="F72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.01366125437238</v>
       </c>
       <c r="G72" s="8">
@@ -3185,20 +3372,23 @@
       <c r="A73" s="5">
         <v>70</v>
       </c>
-      <c r="B73" s="5">
-        <v>5600</v>
+      <c r="B73" s="4">
+        <f t="shared" si="7"/>
+        <v>48020</v>
       </c>
       <c r="C73" s="5">
         <v>999999</v>
       </c>
       <c r="D73" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E73" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.330994897959183</v>
       </c>
       <c r="F73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.121809125710286</v>
       </c>
       <c r="G73" s="8">
@@ -3209,20 +3399,23 @@
       <c r="A74" s="5">
         <v>71</v>
       </c>
-      <c r="B74" s="5">
-        <v>5680</v>
+      <c r="B74" s="4">
+        <f t="shared" si="7"/>
+        <v>49417</v>
       </c>
       <c r="C74" s="5">
         <v>999999</v>
       </c>
       <c r="D74" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E74" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.4202806122448983</v>
       </c>
       <c r="F74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.229366004427643</v>
       </c>
       <c r="G74" s="8">
@@ -3233,20 +3426,23 @@
       <c r="A75" s="5">
         <v>72</v>
       </c>
-      <c r="B75" s="5">
-        <v>5760</v>
+      <c r="B75" s="4">
+        <f t="shared" si="7"/>
+        <v>50833</v>
       </c>
       <c r="C75" s="5">
         <v>999999</v>
       </c>
       <c r="D75" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E75" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.5095663265306127</v>
       </c>
       <c r="F75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.336343041982992</v>
       </c>
       <c r="G75" s="8">
@@ -3257,20 +3453,23 @@
       <c r="A76" s="5">
         <v>73</v>
       </c>
-      <c r="B76" s="5">
-        <v>5840</v>
+      <c r="B76" s="4">
+        <f t="shared" si="7"/>
+        <v>52270</v>
       </c>
       <c r="C76" s="5">
         <v>999999</v>
       </c>
       <c r="D76" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E76" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.5988520408163263</v>
       </c>
       <c r="F76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.442751033908309</v>
       </c>
       <c r="G76" s="8">
@@ -3281,20 +3480,23 @@
       <c r="A77" s="5">
         <v>74</v>
       </c>
-      <c r="B77" s="5">
-        <v>5920</v>
+      <c r="B77" s="4">
+        <f t="shared" si="7"/>
+        <v>53727</v>
       </c>
       <c r="C77" s="5">
         <v>999999</v>
       </c>
       <c r="D77" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E77" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.6881377551020424</v>
       </c>
       <c r="F77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.548600435691771</v>
       </c>
       <c r="G77" s="8">
@@ -3305,20 +3507,23 @@
       <c r="A78" s="5">
         <v>75</v>
       </c>
-      <c r="B78" s="5">
-        <v>6375</v>
+      <c r="B78" s="4">
+        <f t="shared" si="7"/>
+        <v>55203</v>
       </c>
       <c r="C78" s="5">
         <v>999999</v>
       </c>
       <c r="D78" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E78" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.7774234693877542</v>
       </c>
       <c r="F78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.653901377755393</v>
       </c>
       <c r="G78" s="8">
@@ -3329,20 +3534,23 @@
       <c r="A79" s="5">
         <v>76</v>
       </c>
-      <c r="B79" s="5">
-        <v>6460</v>
+      <c r="B79" s="4">
+        <f t="shared" si="7"/>
+        <v>56700</v>
       </c>
       <c r="C79" s="5">
         <v>999999</v>
       </c>
       <c r="D79" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E79" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.8667091836734704</v>
       </c>
       <c r="F79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.75866367958966</v>
       </c>
       <c r="G79" s="8">
@@ -3353,20 +3561,23 @@
       <c r="A80" s="5">
         <v>77</v>
       </c>
-      <c r="B80" s="5">
-        <v>6545</v>
+      <c r="B80" s="4">
+        <f t="shared" si="7"/>
+        <v>58217</v>
       </c>
       <c r="C80" s="5">
         <v>999999</v>
       </c>
       <c r="D80" s="5">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="E80" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7.9559948979591839</v>
       </c>
       <c r="F80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.862896863102925</v>
       </c>
       <c r="G80" s="8">
@@ -3377,20 +3588,23 @@
       <c r="A81" s="5">
         <v>78</v>
       </c>
-      <c r="B81" s="5">
-        <v>6630</v>
+      <c r="B81" s="4">
+        <f t="shared" si="7"/>
+        <v>59753</v>
       </c>
       <c r="C81" s="5">
         <v>999999</v>
       </c>
       <c r="D81" s="5">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E81" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.0452806122448983</v>
       </c>
       <c r="F81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16.966610165238237</v>
       </c>
       <c r="G81" s="8">
@@ -3401,20 +3615,23 @@
       <c r="A82" s="5">
         <v>79</v>
       </c>
-      <c r="B82" s="5">
-        <v>6715</v>
+      <c r="B82" s="4">
+        <f t="shared" si="7"/>
+        <v>61310</v>
       </c>
       <c r="C82" s="5">
         <v>999999</v>
       </c>
       <c r="D82" s="5">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E82" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.1345663265306136</v>
       </c>
       <c r="F82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.069812549906494</v>
       </c>
       <c r="G82" s="8">
@@ -3425,20 +3642,23 @@
       <c r="A83" s="5">
         <v>80</v>
       </c>
-      <c r="B83" s="5">
-        <v>7200</v>
+      <c r="B83" s="4">
+        <f t="shared" si="7"/>
+        <v>62887</v>
       </c>
       <c r="C83" s="5">
         <v>999999</v>
       </c>
       <c r="D83" s="5">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E83" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.2238520408163254</v>
       </c>
       <c r="F83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.172512719280761</v>
       </c>
       <c r="G83" s="8">
@@ -3449,20 +3669,23 @@
       <c r="A84" s="5">
         <v>81</v>
       </c>
-      <c r="B84" s="5">
-        <v>7290</v>
+      <c r="B84" s="4">
+        <f t="shared" si="7"/>
+        <v>64483</v>
       </c>
       <c r="C84" s="5">
         <v>999999</v>
       </c>
       <c r="D84" s="5">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E84" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.3131377551020424</v>
       </c>
       <c r="F84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.274719124493167</v>
       </c>
       <c r="G84" s="8">
@@ -3473,20 +3696,23 @@
       <c r="A85" s="5">
         <v>82</v>
       </c>
-      <c r="B85" s="5">
-        <v>7380</v>
+      <c r="B85" s="4">
+        <f t="shared" si="7"/>
+        <v>66100</v>
       </c>
       <c r="C85" s="5">
         <v>999999</v>
       </c>
       <c r="D85" s="5">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E85" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.402423469387756</v>
       </c>
       <c r="F85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.376439975772879</v>
       </c>
       <c r="G85" s="8">
@@ -3497,20 +3723,23 @@
       <c r="A86" s="5">
         <v>83</v>
       </c>
-      <c r="B86" s="5">
-        <v>7470</v>
+      <c r="B86" s="4">
+        <f t="shared" si="7"/>
+        <v>67737</v>
       </c>
       <c r="C86" s="5">
         <v>999999</v>
       </c>
       <c r="D86" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="E86" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.4917091836734695</v>
       </c>
       <c r="F86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.477683252060292</v>
       </c>
       <c r="G86" s="8">
@@ -3521,20 +3750,23 @@
       <c r="A87" s="5">
         <v>84</v>
       </c>
-      <c r="B87" s="5">
-        <v>7560</v>
+      <c r="B87" s="4">
+        <f t="shared" si="7"/>
+        <v>69393</v>
       </c>
       <c r="C87" s="5">
         <v>999999</v>
       </c>
       <c r="D87" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="E87" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.5809948979591848</v>
       </c>
       <c r="F87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.578456710130649</v>
       </c>
       <c r="G87" s="8">
@@ -3545,20 +3777,23 @@
       <c r="A88" s="5">
         <v>85</v>
       </c>
-      <c r="B88" s="5">
-        <v>8075</v>
+      <c r="B88" s="4">
+        <f t="shared" si="7"/>
+        <v>71070</v>
       </c>
       <c r="C88" s="5">
         <v>999999</v>
       </c>
       <c r="D88" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="E88" s="5">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>8.6702806122448965</v>
       </c>
       <c r="F88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.678767893256996</v>
       </c>
       <c r="G88" s="8">
@@ -3569,20 +3804,23 @@
       <c r="A89" s="5">
         <v>86</v>
       </c>
-      <c r="B89" s="5">
-        <v>8170</v>
+      <c r="B89" s="4">
+        <f t="shared" si="7"/>
+        <v>72767</v>
       </c>
       <c r="C89" s="5">
         <v>999999</v>
       </c>
       <c r="D89" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="E89" s="5">
-        <v>5</v>
+        <f t="shared" ref="E89:E102" si="8">3.3+(A89-21)*0.1-E88*0.12</f>
+        <v>8.7595663265306136</v>
       </c>
       <c r="F89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.778624139441146</v>
       </c>
       <c r="G89" s="8">
@@ -3593,20 +3831,23 @@
       <c r="A90" s="5">
         <v>87</v>
       </c>
-      <c r="B90" s="5">
-        <v>8265</v>
+      <c r="B90" s="4">
+        <f t="shared" si="7"/>
+        <v>74483</v>
       </c>
       <c r="C90" s="5">
         <v>999999</v>
       </c>
       <c r="D90" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="E90" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>8.8488520408163271</v>
       </c>
       <c r="F90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.878032589238494</v>
       </c>
       <c r="G90" s="8">
@@ -3617,20 +3858,23 @@
       <c r="A91" s="5">
         <v>88</v>
       </c>
-      <c r="B91" s="5">
-        <v>8360</v>
+      <c r="B91" s="4">
+        <f t="shared" si="7"/>
+        <v>76220</v>
       </c>
       <c r="C91" s="5">
         <v>999999</v>
       </c>
       <c r="D91" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="E91" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>8.9381377551020407</v>
       </c>
       <c r="F91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17.977000193201071</v>
       </c>
       <c r="G91" s="8">
@@ -3641,20 +3885,23 @@
       <c r="A92" s="5">
         <v>89</v>
       </c>
-      <c r="B92" s="5">
-        <v>8455</v>
+      <c r="B92" s="4">
+        <f t="shared" si="7"/>
+        <v>77977</v>
       </c>
       <c r="C92" s="5">
         <v>999999</v>
       </c>
       <c r="D92" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E92" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.027423469387756</v>
       </c>
       <c r="F92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.075533718961573</v>
       </c>
       <c r="G92" s="8">
@@ -3665,20 +3912,23 @@
       <c r="A93" s="5">
         <v>90</v>
       </c>
-      <c r="B93" s="5">
-        <v>9000</v>
+      <c r="B93" s="4">
+        <f t="shared" si="7"/>
+        <v>79753</v>
       </c>
       <c r="C93" s="5">
         <v>999999</v>
       </c>
       <c r="D93" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E93" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.1167091836734677</v>
       </c>
       <c r="F93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.173639757979167</v>
       </c>
       <c r="G93" s="8">
@@ -3689,20 +3939,23 @@
       <c r="A94" s="5">
         <v>91</v>
       </c>
-      <c r="B94" s="5">
-        <v>9100</v>
+      <c r="B94" s="4">
+        <f t="shared" si="7"/>
+        <v>81550</v>
       </c>
       <c r="C94" s="5">
         <v>999999</v>
       </c>
       <c r="D94" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E94" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.2059948979591848</v>
       </c>
       <c r="F94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.271324731966914</v>
       </c>
       <c r="G94" s="8">
@@ -3713,20 +3966,23 @@
       <c r="A95" s="5">
         <v>92</v>
       </c>
-      <c r="B95" s="5">
-        <v>9200</v>
+      <c r="B95" s="4">
+        <f t="shared" si="7"/>
+        <v>83367</v>
       </c>
       <c r="C95" s="5">
         <v>999999</v>
       </c>
       <c r="D95" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E95" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.2952806122448983</v>
       </c>
       <c r="F95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.368594899018895</v>
       </c>
       <c r="G95" s="8">
@@ -3737,20 +3993,23 @@
       <c r="A96" s="5">
         <v>93</v>
       </c>
-      <c r="B96" s="5">
-        <v>9300</v>
+      <c r="B96" s="4">
+        <f t="shared" si="7"/>
+        <v>85203</v>
       </c>
       <c r="C96" s="5">
         <v>999999</v>
       </c>
       <c r="D96" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E96" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.3845663265306118</v>
       </c>
       <c r="F96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.465456359454102</v>
       </c>
       <c r="G96" s="8">
@@ -3761,20 +4020,23 @@
       <c r="A97" s="5">
         <v>94</v>
       </c>
-      <c r="B97" s="5">
-        <v>9400</v>
+      <c r="B97" s="4">
+        <f t="shared" si="7"/>
+        <v>87060</v>
       </c>
       <c r="C97" s="5">
         <v>999999</v>
       </c>
       <c r="D97" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E97" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.4738520408163289</v>
       </c>
       <c r="F97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.561915061393066</v>
       </c>
       <c r="G97" s="8">
@@ -3785,20 +4047,23 @@
       <c r="A98" s="5">
         <v>95</v>
       </c>
-      <c r="B98" s="5">
-        <v>9975</v>
+      <c r="B98" s="4">
+        <f t="shared" si="7"/>
+        <v>88937</v>
       </c>
       <c r="C98" s="5">
         <v>999999</v>
       </c>
       <c r="D98" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E98" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.5631377551020407</v>
       </c>
       <c r="F98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.657976806082026</v>
       </c>
       <c r="G98" s="8">
@@ -3809,20 +4074,23 @@
       <c r="A99" s="5">
         <v>96</v>
       </c>
-      <c r="B99" s="5">
-        <v>10080</v>
+      <c r="B99" s="4">
+        <f t="shared" si="7"/>
+        <v>90833</v>
       </c>
       <c r="C99" s="5">
         <v>999999</v>
       </c>
       <c r="D99" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E99" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.652423469387756</v>
       </c>
       <c r="F99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.75364725297846</v>
       </c>
       <c r="G99" s="8">
@@ -3833,20 +4101,23 @@
       <c r="A100" s="5">
         <v>97</v>
       </c>
-      <c r="B100" s="5">
-        <v>10185</v>
+      <c r="B100" s="4">
+        <f t="shared" si="7"/>
+        <v>92750</v>
       </c>
       <c r="C100" s="5">
         <v>999999</v>
       </c>
       <c r="D100" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E100" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.7417091836734695</v>
       </c>
       <c r="F100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.848931924611136</v>
       </c>
       <c r="G100" s="8">
@@ -3857,20 +4128,23 @@
       <c r="A101" s="5">
         <v>98</v>
       </c>
-      <c r="B101" s="5">
-        <v>10290</v>
+      <c r="B101" s="4">
+        <f t="shared" si="7"/>
+        <v>94687</v>
       </c>
       <c r="C101" s="5">
         <v>999999</v>
       </c>
       <c r="D101" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E101" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.830994897959183</v>
       </c>
       <c r="F101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.9438362112266</v>
       </c>
       <c r="G101" s="8">
@@ -3881,20 +4155,23 @@
       <c r="A102" s="5">
         <v>99</v>
       </c>
-      <c r="B102" s="5">
-        <v>10395</v>
+      <c r="B102" s="4">
+        <f t="shared" si="7"/>
+        <v>96643</v>
       </c>
       <c r="C102" s="5">
         <v>999999</v>
       </c>
       <c r="D102" s="5">
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
       <c r="E102" s="5">
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>9.9202806122449001</v>
       </c>
       <c r="F102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>19.038365375233763</v>
       </c>
       <c r="G102" s="8">

</xml_diff>

<commit_message>
optimise the exp gain
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -91,7 +91,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,14 +277,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -787,9 +782,6 @@
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -798,6 +790,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -861,6 +856,7 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="176" formatCode="0.00_ "/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -888,6 +884,7 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="176" formatCode="0.00_ "/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -915,6 +912,7 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="176" formatCode="0.00_ "/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1446,37 +1444,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B102"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="3" width="7.5" customWidth="1"/>
     <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="5" max="7" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1531,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
@@ -1540,14 +1538,14 @@
         <f>INT(E4)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="11">
         <f>POWER(A4+3,0.6)+3</f>
         <v>5.2973967099940698</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="11">
         <v>1.059479341998814</v>
       </c>
     </row>
@@ -1556,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
@@ -1565,14 +1563,14 @@
         <f t="shared" ref="D5:D68" si="0">INT(E5)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="11">
         <f t="shared" ref="F5:F68" si="1">POWER(A5+3,0.6)+3</f>
         <v>5.626527804403767</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="11">
         <v>1.1253055608807534</v>
       </c>
     </row>
@@ -1581,7 +1579,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C6" s="4">
         <v>10</v>
@@ -1590,14 +1588,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="11">
         <v>1.2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="11">
         <f t="shared" si="1"/>
         <v>5.9301560515835217</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="11">
         <v>1.1860312103167043</v>
       </c>
     </row>
@@ -1607,7 +1605,7 @@
       </c>
       <c r="B7" s="4">
         <f>INT(B6*0.7+A7*10+A7*A7*3-30)</f>
-        <v>93</v>
+        <v>408</v>
       </c>
       <c r="C7" s="4">
         <v>20</v>
@@ -1616,14 +1614,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="11">
         <v>1.3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="11">
         <f t="shared" si="1"/>
         <v>6.2140958497160383</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="11">
         <v>1.2428191699432076</v>
       </c>
     </row>
@@ -1633,7 +1631,7 @@
       </c>
       <c r="B8" s="4">
         <f t="shared" ref="B8:B71" si="2">INT(B7*0.7+A8*10+A8*A8*3-30)</f>
-        <v>160</v>
+        <v>380</v>
       </c>
       <c r="C8" s="4">
         <v>40</v>
@@ -1642,14 +1640,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="11">
         <v>1.4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="11">
         <f t="shared" si="1"/>
         <v>6.4822022531844965</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="11">
         <v>1.2964404506368994</v>
       </c>
     </row>
@@ -1659,7 +1657,7 @@
       </c>
       <c r="B9" s="4">
         <f t="shared" si="2"/>
-        <v>250</v>
+        <v>404</v>
       </c>
       <c r="C9" s="4">
         <v>80</v>
@@ -1668,14 +1666,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="11">
         <v>1.5</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="11">
         <f t="shared" si="1"/>
         <v>6.7371928188465517</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="11">
         <v>1.3474385637693103</v>
       </c>
     </row>
@@ -1685,7 +1683,7 @@
       </c>
       <c r="B10" s="4">
         <f t="shared" si="2"/>
-        <v>362</v>
+        <v>469</v>
       </c>
       <c r="C10" s="4">
         <v>200</v>
@@ -1694,14 +1692,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="11">
         <v>1.6</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="11">
         <f t="shared" si="1"/>
         <v>6.9810717055349727</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="11">
         <v>1.3962143411069945</v>
       </c>
     </row>
@@ -1711,7 +1709,7 @@
       </c>
       <c r="B11" s="4">
         <f t="shared" si="2"/>
-        <v>495</v>
+        <v>570</v>
       </c>
       <c r="C11" s="4">
         <f>C10+500</f>
@@ -1721,14 +1719,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="11">
         <v>1.7</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="11">
         <f t="shared" si="1"/>
         <v>7.2153691330919001</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="11">
         <v>1.44307382661838</v>
       </c>
     </row>
@@ -1738,7 +1736,7 @@
       </c>
       <c r="B12" s="4">
         <f t="shared" si="2"/>
-        <v>649</v>
+        <v>702</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" ref="C12" si="3">C11+500</f>
@@ -1748,14 +1746,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="11">
         <v>1.8</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="11">
         <f t="shared" si="1"/>
         <v>7.4412860698458401</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="11">
         <v>1.4882572139691681</v>
       </c>
     </row>
@@ -1765,7 +1763,7 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" si="2"/>
-        <v>824</v>
+        <v>861</v>
       </c>
       <c r="C13" s="5">
         <v>999999</v>
@@ -1774,14 +1772,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="11">
         <v>1.9</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="11">
         <f t="shared" si="1"/>
         <v>7.6597864200360659</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="11">
         <v>1.5319572840072131</v>
       </c>
     </row>
@@ -1791,7 +1789,7 @@
       </c>
       <c r="B14" s="4">
         <f t="shared" si="2"/>
-        <v>1019</v>
+        <v>1045</v>
       </c>
       <c r="C14" s="5">
         <v>999999</v>
@@ -1800,14 +1798,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="11">
         <v>2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="11">
         <f t="shared" si="1"/>
         <v>7.8716583257669139</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="11">
         <v>1.5743316651533827</v>
       </c>
     </row>
@@ -1817,7 +1815,7 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" si="2"/>
-        <v>1235</v>
+        <v>1253</v>
       </c>
       <c r="C15" s="5">
         <v>999999</v>
@@ -1826,14 +1824,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="11">
         <v>2.1</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="11">
         <f t="shared" si="1"/>
         <v>8.0775563919874074</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="11">
         <v>1.6155112783974814</v>
       </c>
     </row>
@@ -1843,7 +1841,7 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" si="2"/>
-        <v>1471</v>
+        <v>1484</v>
       </c>
       <c r="C16" s="5">
         <v>999999</v>
@@ -1852,14 +1850,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="11">
         <f t="shared" si="1"/>
         <v>8.2780316430915768</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="11">
         <v>1.6556063286183154</v>
       </c>
     </row>
@@ -1869,7 +1867,7 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" si="2"/>
-        <v>1727</v>
+        <v>1736</v>
       </c>
       <c r="C17" s="5">
         <v>999999</v>
@@ -1878,14 +1876,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="11">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="11">
         <f t="shared" si="1"/>
         <v>8.4735533169184887</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="11">
         <v>1.6947106633836977</v>
       </c>
     </row>
@@ -1895,7 +1893,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="2"/>
-        <v>2003</v>
+        <v>2010</v>
       </c>
       <c r="C18" s="5">
         <v>999999</v>
@@ -1904,14 +1902,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="11">
         <v>2.4</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="11">
         <f t="shared" si="1"/>
         <v>8.6645250677694108</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="11">
         <v>1.7329050135538822</v>
       </c>
     </row>
@@ -1921,7 +1919,7 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" si="2"/>
-        <v>2300</v>
+        <v>2305</v>
       </c>
       <c r="C19" s="5">
         <v>999999</v>
@@ -1930,14 +1928,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="11">
         <v>2.5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="11">
         <f t="shared" si="1"/>
         <v>8.8512972424092151</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="11">
         <v>1.770259448481843</v>
       </c>
     </row>
@@ -1947,7 +1945,7 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" si="2"/>
-        <v>2617</v>
+        <v>2620</v>
       </c>
       <c r="C20" s="5">
         <v>999999</v>
@@ -1956,14 +1954,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="11">
         <v>2.6</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="11">
         <f t="shared" si="1"/>
         <v>9.0341763365451619</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="11">
         <v>1.8068352673090324</v>
       </c>
     </row>
@@ -1973,7 +1971,7 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" si="2"/>
-        <v>2953</v>
+        <v>2956</v>
       </c>
       <c r="C21" s="5">
         <v>999999</v>
@@ -1982,14 +1980,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="11">
         <v>2.7</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="11">
         <f t="shared" si="1"/>
         <v>9.2134323873607435</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="11">
         <v>1.8426864774721488</v>
       </c>
     </row>
@@ -1999,7 +1997,7 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" si="2"/>
-        <v>3310</v>
+        <v>3312</v>
       </c>
       <c r="C22" s="5">
         <v>999999</v>
@@ -2008,14 +2006,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="11">
         <v>2.8</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="11">
         <f t="shared" si="1"/>
         <v>9.3893048289839669</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="11">
         <v>1.8778609657967933</v>
       </c>
     </row>
@@ -2025,7 +2023,7 @@
       </c>
       <c r="B23" s="4">
         <f t="shared" si="2"/>
-        <v>3687</v>
+        <v>3688</v>
       </c>
       <c r="C23" s="5">
         <v>999999</v>
@@ -2034,14 +2032,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="11">
         <v>2.9</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="11">
         <f t="shared" si="1"/>
         <v>9.5620071855158546</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="11">
         <v>1.912401437103171</v>
       </c>
     </row>
@@ -2051,7 +2049,7 @@
       </c>
       <c r="B24" s="4">
         <f t="shared" si="2"/>
-        <v>4083</v>
+        <v>4084</v>
       </c>
       <c r="C24" s="5">
         <v>999999</v>
@@ -2060,15 +2058,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="11">
         <f>3.3+(A24-21)*0.1-E23*0.12</f>
         <v>2.952</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="11">
         <f t="shared" si="1"/>
         <v>9.7317308726771969</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="11">
         <v>1.9463461745354393</v>
       </c>
     </row>
@@ -2087,15 +2085,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="11">
         <f t="shared" ref="E25:E88" si="4">3.3+(A25-21)*0.1-E24*0.12</f>
         <v>3.04576</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="11">
         <f t="shared" si="1"/>
         <v>9.8986483073060718</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="11">
         <v>1.9797296614612143</v>
       </c>
     </row>
@@ -2114,15 +2112,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="11">
         <f t="shared" si="4"/>
         <v>3.1345087999999999</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="11">
         <f t="shared" si="1"/>
         <v>10.062915473248847</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="11">
         <v>2.0125830946497691</v>
       </c>
     </row>
@@ -2141,15 +2139,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="11">
         <f t="shared" si="4"/>
         <v>3.2238589439999998</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="11">
         <f t="shared" si="1"/>
         <v>10.224674055842076</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="11">
         <v>2.0449348111684151</v>
       </c>
     </row>
@@ -2168,15 +2166,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="11">
         <f t="shared" si="4"/>
         <v>3.3131369267199999</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="11">
         <f t="shared" si="1"/>
         <v>10.38405323074322</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="11">
         <v>2.076810646148644</v>
       </c>
     </row>
@@ -2195,15 +2193,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="11">
         <f t="shared" si="4"/>
         <v>3.4024235687936</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="11">
         <f t="shared" si="1"/>
         <v>10.541171173377641</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="11">
         <v>2.1082342346755283</v>
       </c>
     </row>
@@ -2222,15 +2220,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="11">
         <f t="shared" si="4"/>
         <v>3.4917091717447679</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="11">
         <f t="shared" si="1"/>
         <v>10.696136340726078</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="11">
         <v>2.1392272681452154</v>
       </c>
     </row>
@@ -2249,15 +2247,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="11">
         <f t="shared" si="4"/>
         <v>3.5809948993906278</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="11">
         <f t="shared" si="1"/>
         <v>10.849048566202034</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="11">
         <v>2.1698097132404071</v>
       </c>
     </row>
@@ -2276,15 +2274,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="11">
         <f t="shared" si="4"/>
         <v>3.6702806120731242</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="11">
         <f t="shared" si="1"/>
         <v>10.999999999999998</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="11">
         <v>2.1999999999999997</v>
       </c>
     </row>
@@ -2303,15 +2301,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="11">
         <f t="shared" si="4"/>
         <v>3.7595663265512251</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="11">
         <f t="shared" si="1"/>
         <v>11.149075920852829</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="11">
         <v>2.2298151841705658</v>
       </c>
     </row>
@@ -2330,15 +2328,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="11">
         <f t="shared" si="4"/>
         <v>3.8488520408138527</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="11">
         <f t="shared" si="1"/>
         <v>11.296355440131292</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="11">
         <v>2.2592710880262583</v>
       </c>
     </row>
@@ -2357,15 +2355,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="11">
         <f t="shared" si="4"/>
         <v>3.9381377551023382</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="11">
         <f t="shared" si="1"/>
         <v>11.441912115297924</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="11">
         <v>2.2883824230595851</v>
       </c>
     </row>
@@ -2384,15 +2382,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="11">
         <f t="shared" si="4"/>
         <v>4.0274234693877196</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="11">
         <f t="shared" si="1"/>
         <v>11.585814486631531</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="11">
         <v>2.3171628973263063</v>
       </c>
     </row>
@@ -2411,15 +2409,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="11">
         <f t="shared" si="4"/>
         <v>4.116709183673473</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="11">
         <f t="shared" si="1"/>
         <v>11.72812654867613</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="11">
         <v>2.345625309735226</v>
       </c>
     </row>
@@ -2438,15 +2436,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="11">
         <f t="shared" si="4"/>
         <v>4.205994897959183</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="11">
         <f t="shared" si="1"/>
         <v>11.868908165896258</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="11">
         <v>2.3737816331792514</v>
       </c>
     </row>
@@ -2465,15 +2463,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="11">
         <f t="shared" si="4"/>
         <v>4.2952806122448983</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="11">
         <f t="shared" si="1"/>
         <v>12.008215440430581</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="11">
         <v>2.4016430880861162</v>
       </c>
     </row>
@@ -2492,15 +2490,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="11">
         <f t="shared" si="4"/>
         <v>4.3845663265306127</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="11">
         <f t="shared" si="1"/>
         <v>12.146101038546524</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="11">
         <v>2.4292202077093048</v>
       </c>
     </row>
@@ -2519,15 +2517,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="11">
         <f t="shared" si="4"/>
         <v>4.4738520408163263</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="11">
         <f t="shared" si="1"/>
         <v>12.282614481346684</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="11">
         <v>2.4565228962693366</v>
       </c>
     </row>
@@ -2546,15 +2544,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="11">
         <f t="shared" si="4"/>
         <v>4.5631377551020407</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="11">
         <f t="shared" si="1"/>
         <v>12.41780240441493</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="11">
         <v>2.4835604808829861</v>
       </c>
     </row>
@@ -2573,15 +2571,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="11">
         <f t="shared" si="4"/>
         <v>4.6524234693877551</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="11">
         <f t="shared" si="1"/>
         <v>12.551708790378902</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="11">
         <v>2.5103417580757803</v>
       </c>
     </row>
@@ -2600,15 +2598,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="11">
         <f t="shared" si="4"/>
         <v>4.7417091836734695</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="11">
         <f t="shared" si="1"/>
         <v>12.684375177775884</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="11">
         <v>2.5368750355551768</v>
       </c>
     </row>
@@ -2627,15 +2625,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="11">
         <f t="shared" si="4"/>
         <v>4.8309948979591839</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="11">
         <f t="shared" si="1"/>
         <v>12.81584084911856</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="11">
         <v>2.5631681698237121</v>
       </c>
     </row>
@@ -2654,15 +2652,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="11">
         <f t="shared" si="4"/>
         <v>4.9202806122448983</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="11">
         <f t="shared" si="1"/>
         <v>12.946143000646654</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="11">
         <v>2.5892286001293305</v>
       </c>
     </row>
@@ -2681,15 +2679,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="11">
         <f t="shared" si="4"/>
         <v>5.0095663265306118</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="11">
         <f t="shared" si="1"/>
         <v>13.075316895906047</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="11">
         <v>2.6150633791812092</v>
       </c>
     </row>
@@ -2708,15 +2706,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="11">
         <f t="shared" si="4"/>
         <v>5.0988520408163271</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="11">
         <f t="shared" si="1"/>
         <v>13.203396005006329</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="11">
         <v>2.6406792010012659</v>
       </c>
     </row>
@@ -2735,15 +2733,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="11">
         <f t="shared" si="4"/>
         <v>5.1881377551020407</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="11">
         <f t="shared" si="1"/>
         <v>13.330412131161864</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="11">
         <v>2.6660824262323728</v>
       </c>
     </row>
@@ -2762,15 +2760,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="11">
         <f t="shared" si="4"/>
         <v>5.277423469387756</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="11">
         <f t="shared" si="1"/>
         <v>13.456395525912733</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="11">
         <v>2.6912791051825464</v>
       </c>
     </row>
@@ -2789,15 +2787,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="11">
         <f t="shared" si="4"/>
         <v>5.3667091836734695</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="11">
         <f t="shared" si="1"/>
         <v>13.581374994243514</v>
       </c>
-      <c r="G51" s="8">
+      <c r="G51" s="11">
         <v>2.7162749988487027</v>
       </c>
     </row>
@@ -2816,15 +2814,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="11">
         <f t="shared" si="4"/>
         <v>5.455994897959183</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="11">
         <f t="shared" si="1"/>
         <v>13.705377990665905</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="11">
         <v>2.7410755981331811</v>
       </c>
     </row>
@@ -2843,15 +2841,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="11">
         <f t="shared" si="4"/>
         <v>5.5452806122448983</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="11">
         <f t="shared" si="1"/>
         <v>13.828430707200107</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="11">
         <v>2.7656861414400216</v>
       </c>
     </row>
@@ -2870,15 +2868,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="11">
         <f t="shared" si="4"/>
         <v>5.6345663265306118</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="11">
         <f t="shared" si="1"/>
         <v>13.950558154077704</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="11">
         <v>2.7901116308155407</v>
       </c>
     </row>
@@ -2897,15 +2895,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="11">
         <f t="shared" si="4"/>
         <v>5.7238520408163271</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="11">
         <f t="shared" si="1"/>
         <v>14.071784233891282</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="11">
         <v>2.8143568467782565</v>
       </c>
     </row>
@@ -2924,15 +2922,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="11">
         <f t="shared" si="4"/>
         <v>5.8131377551020407</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="11">
         <f t="shared" si="1"/>
         <v>14.192131809832132</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="11">
         <v>2.8384263619664263</v>
       </c>
     </row>
@@ -2951,15 +2949,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="11">
         <f t="shared" si="4"/>
         <v>5.9024234693877551</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="11">
         <f t="shared" si="1"/>
         <v>14.311622768584231</v>
       </c>
-      <c r="G57" s="8">
+      <c r="G57" s="11">
         <v>2.8623245537168462</v>
       </c>
     </row>
@@ -2978,15 +2976,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="11">
         <f t="shared" si="4"/>
         <v>5.9917091836734695</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="11">
         <f t="shared" si="1"/>
         <v>14.430278078379143</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="11">
         <v>2.8860556156758284</v>
       </c>
     </row>
@@ -3005,15 +3003,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="11">
         <f t="shared" si="4"/>
         <v>6.080994897959183</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="11">
         <f t="shared" si="1"/>
         <v>14.548117842660861</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="11">
         <v>2.9096235685321723</v>
       </c>
     </row>
@@ -3032,15 +3030,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E60" s="11">
         <f t="shared" si="4"/>
         <v>6.1702806122448983</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="11">
         <f t="shared" si="1"/>
         <v>14.665161349761227</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="11">
         <v>2.9330322699522453</v>
       </c>
     </row>
@@ -3059,15 +3057,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E61" s="5">
+      <c r="E61" s="11">
         <f t="shared" si="4"/>
         <v>6.2595663265306118</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="11">
         <f t="shared" si="1"/>
         <v>14.781427118943885</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="11">
         <v>2.9562854237887768</v>
       </c>
     </row>
@@ -3086,15 +3084,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E62" s="5">
+      <c r="E62" s="11">
         <f t="shared" si="4"/>
         <v>6.3488520408163263</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="11">
         <f t="shared" si="1"/>
         <v>14.896932943137111</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="11">
         <v>2.9793865886274222</v>
       </c>
     </row>
@@ -3113,15 +3111,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E63" s="11">
         <f t="shared" si="4"/>
         <v>6.4381377551020407</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="11">
         <f t="shared" si="1"/>
         <v>15.011695928643283</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="11">
         <v>3.0023391857286565</v>
       </c>
     </row>
@@ -3140,15 +3138,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E64" s="5">
+      <c r="E64" s="11">
         <f t="shared" si="4"/>
         <v>6.5274234693877551</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="11">
         <f t="shared" si="1"/>
         <v>15.125732532083184</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="11">
         <v>3.025146506416637</v>
       </c>
     </row>
@@ -3167,15 +3165,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E65" s="5">
+      <c r="E65" s="11">
         <f t="shared" si="4"/>
         <v>6.6167091836734695</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="11">
         <f t="shared" si="1"/>
         <v>15.239058594807814</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G65" s="11">
         <v>3.0478117189615626</v>
       </c>
     </row>
@@ -3194,15 +3192,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E66" s="5">
+      <c r="E66" s="11">
         <f t="shared" si="4"/>
         <v>6.7059948979591839</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="11">
         <f t="shared" si="1"/>
         <v>15.351689374987611</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G66" s="11">
         <v>3.0703378749975223</v>
       </c>
     </row>
@@ -3221,15 +3219,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E67" s="5">
+      <c r="E67" s="11">
         <f t="shared" si="4"/>
         <v>6.7952806122448974</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="11">
         <f t="shared" si="1"/>
         <v>15.463639577568394</v>
       </c>
-      <c r="G67" s="8">
+      <c r="G67" s="11">
         <v>3.0927279155136786</v>
       </c>
     </row>
@@ -3248,15 +3246,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E68" s="5">
+      <c r="E68" s="11">
         <f t="shared" si="4"/>
         <v>6.8845663265306127</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="11">
         <f t="shared" si="1"/>
         <v>15.574923382265665</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G68" s="11">
         <v>3.1149846764531328</v>
       </c>
     </row>
@@ -3275,15 +3273,15 @@
         <f t="shared" ref="D69:D102" si="5">INT(E69)</f>
         <v>6</v>
       </c>
-      <c r="E69" s="5">
+      <c r="E69" s="11">
         <f t="shared" si="4"/>
         <v>6.9738520408163263</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="11">
         <f t="shared" ref="F69:F102" si="6">POWER(A69+3,0.6)+3</f>
         <v>15.685554469752462</v>
       </c>
-      <c r="G69" s="8">
+      <c r="G69" s="11">
         <v>3.1371108939504926</v>
       </c>
     </row>
@@ -3302,15 +3300,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E70" s="5">
+      <c r="E70" s="11">
         <f t="shared" si="4"/>
         <v>7.0631377551020416</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="11">
         <f t="shared" si="6"/>
         <v>15.79554604618191</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="11">
         <v>3.1591092092363819</v>
       </c>
     </row>
@@ -3329,15 +3327,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E71" s="5">
+      <c r="E71" s="11">
         <f t="shared" si="4"/>
         <v>7.1524234693877551</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="11">
         <f t="shared" si="6"/>
         <v>15.904910866172429</v>
       </c>
-      <c r="G71" s="8">
+      <c r="G71" s="11">
         <v>3.1809821732344856</v>
       </c>
     </row>
@@ -3356,15 +3354,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72" s="11">
         <f t="shared" si="4"/>
         <v>7.2417091836734713</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="11">
         <f t="shared" si="6"/>
         <v>16.01366125437238</v>
       </c>
-      <c r="G72" s="8">
+      <c r="G72" s="11">
         <v>3.202732250874476</v>
       </c>
     </row>
@@ -3383,15 +3381,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="11">
         <f t="shared" si="4"/>
         <v>7.330994897959183</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="11">
         <f t="shared" si="6"/>
         <v>16.121809125710286</v>
       </c>
-      <c r="G73" s="8">
+      <c r="G73" s="11">
         <v>3.2243618251420569</v>
       </c>
     </row>
@@ -3410,15 +3408,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="11">
         <f t="shared" si="4"/>
         <v>7.4202806122448983</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="11">
         <f t="shared" si="6"/>
         <v>16.229366004427643</v>
       </c>
-      <c r="G74" s="8">
+      <c r="G74" s="11">
         <v>3.2458732008855287</v>
       </c>
     </row>
@@ -3437,15 +3435,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="11">
         <f t="shared" si="4"/>
         <v>7.5095663265306127</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="11">
         <f t="shared" si="6"/>
         <v>16.336343041982992</v>
       </c>
-      <c r="G75" s="8">
+      <c r="G75" s="11">
         <v>3.2672686083965985</v>
       </c>
     </row>
@@ -3464,15 +3462,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="11">
         <f t="shared" si="4"/>
         <v>7.5988520408163263</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="11">
         <f t="shared" si="6"/>
         <v>16.442751033908309</v>
       </c>
-      <c r="G76" s="8">
+      <c r="G76" s="11">
         <v>3.2885502067816619</v>
       </c>
     </row>
@@ -3491,15 +3489,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77" s="11">
         <f t="shared" si="4"/>
         <v>7.6881377551020424</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="11">
         <f t="shared" si="6"/>
         <v>16.548600435691771</v>
       </c>
-      <c r="G77" s="8">
+      <c r="G77" s="11">
         <v>3.3097200871383543</v>
       </c>
     </row>
@@ -3518,15 +3516,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78" s="11">
         <f t="shared" si="4"/>
         <v>7.7774234693877542</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="11">
         <f t="shared" si="6"/>
         <v>16.653901377755393</v>
       </c>
-      <c r="G78" s="8">
+      <c r="G78" s="11">
         <v>3.3307802755510787</v>
       </c>
     </row>
@@ -3545,15 +3543,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="11">
         <f t="shared" si="4"/>
         <v>7.8667091836734704</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="11">
         <f t="shared" si="6"/>
         <v>16.75866367958966</v>
       </c>
-      <c r="G79" s="8">
+      <c r="G79" s="11">
         <v>3.3517327359179321</v>
       </c>
     </row>
@@ -3572,15 +3570,15 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="11">
         <f t="shared" si="4"/>
         <v>7.9559948979591839</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="11">
         <f t="shared" si="6"/>
         <v>16.862896863102925</v>
       </c>
-      <c r="G80" s="8">
+      <c r="G80" s="11">
         <v>3.372579372620585</v>
       </c>
     </row>
@@ -3599,15 +3597,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="11">
         <f t="shared" si="4"/>
         <v>8.0452806122448983</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="11">
         <f t="shared" si="6"/>
         <v>16.966610165238237</v>
       </c>
-      <c r="G81" s="8">
+      <c r="G81" s="11">
         <v>3.3933220330476472</v>
       </c>
     </row>
@@ -3626,15 +3624,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E82" s="5">
+      <c r="E82" s="11">
         <f t="shared" si="4"/>
         <v>8.1345663265306136</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="11">
         <f t="shared" si="6"/>
         <v>17.069812549906494</v>
       </c>
-      <c r="G82" s="8">
+      <c r="G82" s="11">
         <v>3.4139625099812987</v>
       </c>
     </row>
@@ -3653,15 +3651,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83" s="11">
         <f t="shared" si="4"/>
         <v>8.2238520408163254</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="11">
         <f t="shared" si="6"/>
         <v>17.172512719280761</v>
       </c>
-      <c r="G83" s="8">
+      <c r="G83" s="11">
         <v>3.4345025438561523</v>
       </c>
     </row>
@@ -3680,15 +3678,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84" s="11">
         <f t="shared" si="4"/>
         <v>8.3131377551020424</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="11">
         <f t="shared" si="6"/>
         <v>17.274719124493167</v>
       </c>
-      <c r="G84" s="8">
+      <c r="G84" s="11">
         <v>3.4549438248986335</v>
       </c>
     </row>
@@ -3707,15 +3705,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E85" s="5">
+      <c r="E85" s="11">
         <f t="shared" si="4"/>
         <v>8.402423469387756</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="11">
         <f t="shared" si="6"/>
         <v>17.376439975772879</v>
       </c>
-      <c r="G85" s="8">
+      <c r="G85" s="11">
         <v>3.4752879951545759</v>
       </c>
     </row>
@@ -3734,15 +3732,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E86" s="5">
+      <c r="E86" s="11">
         <f t="shared" si="4"/>
         <v>8.4917091836734695</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="11">
         <f t="shared" si="6"/>
         <v>17.477683252060292</v>
       </c>
-      <c r="G86" s="8">
+      <c r="G86" s="11">
         <v>3.4955366504120584</v>
       </c>
     </row>
@@ -3761,15 +3759,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E87" s="5">
+      <c r="E87" s="11">
         <f t="shared" si="4"/>
         <v>8.5809948979591848</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="11">
         <f t="shared" si="6"/>
         <v>17.578456710130649</v>
       </c>
-      <c r="G87" s="8">
+      <c r="G87" s="11">
         <v>3.5156913420261295</v>
       </c>
     </row>
@@ -3788,15 +3786,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E88" s="5">
+      <c r="E88" s="11">
         <f t="shared" si="4"/>
         <v>8.6702806122448965</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="11">
         <f t="shared" si="6"/>
         <v>17.678767893256996</v>
       </c>
-      <c r="G88" s="8">
+      <c r="G88" s="11">
         <v>3.5357535786513994</v>
       </c>
     </row>
@@ -3815,15 +3813,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E89" s="5">
+      <c r="E89" s="11">
         <f t="shared" ref="E89:E102" si="8">3.3+(A89-21)*0.1-E88*0.12</f>
         <v>8.7595663265306136</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="11">
         <f t="shared" si="6"/>
         <v>17.778624139441146</v>
       </c>
-      <c r="G89" s="8">
+      <c r="G89" s="11">
         <v>3.5557248278882292</v>
       </c>
     </row>
@@ -3842,15 +3840,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E90" s="5">
+      <c r="E90" s="11">
         <f t="shared" si="8"/>
         <v>8.8488520408163271</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="11">
         <f t="shared" si="6"/>
         <v>17.878032589238494</v>
       </c>
-      <c r="G90" s="8">
+      <c r="G90" s="11">
         <v>3.5756065178476986</v>
       </c>
     </row>
@@ -3869,15 +3867,15 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E91" s="5">
+      <c r="E91" s="11">
         <f t="shared" si="8"/>
         <v>8.9381377551020407</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="11">
         <f t="shared" si="6"/>
         <v>17.977000193201071</v>
       </c>
-      <c r="G91" s="8">
+      <c r="G91" s="11">
         <v>3.5954000386402143</v>
       </c>
     </row>
@@ -3896,15 +3894,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E92" s="5">
+      <c r="E92" s="11">
         <f t="shared" si="8"/>
         <v>9.027423469387756</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="11">
         <f t="shared" si="6"/>
         <v>18.075533718961573</v>
       </c>
-      <c r="G92" s="8">
+      <c r="G92" s="11">
         <v>3.6151067437923148</v>
       </c>
     </row>
@@ -3923,15 +3921,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E93" s="5">
+      <c r="E93" s="11">
         <f t="shared" si="8"/>
         <v>9.1167091836734677</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="11">
         <f t="shared" si="6"/>
         <v>18.173639757979167</v>
       </c>
-      <c r="G93" s="8">
+      <c r="G93" s="11">
         <v>3.6347279515958335</v>
       </c>
     </row>
@@ -3950,15 +3948,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E94" s="5">
+      <c r="E94" s="11">
         <f t="shared" si="8"/>
         <v>9.2059948979591848</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="11">
         <f t="shared" si="6"/>
         <v>18.271324731966914</v>
       </c>
-      <c r="G94" s="8">
+      <c r="G94" s="11">
         <v>3.6542649463933827</v>
       </c>
     </row>
@@ -3977,15 +3975,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E95" s="5">
+      <c r="E95" s="11">
         <f t="shared" si="8"/>
         <v>9.2952806122448983</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="11">
         <f t="shared" si="6"/>
         <v>18.368594899018895</v>
       </c>
-      <c r="G95" s="8">
+      <c r="G95" s="11">
         <v>3.673718979803779</v>
       </c>
     </row>
@@ -4004,15 +4002,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96" s="11">
         <f t="shared" si="8"/>
         <v>9.3845663265306118</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="11">
         <f t="shared" si="6"/>
         <v>18.465456359454102</v>
       </c>
-      <c r="G96" s="8">
+      <c r="G96" s="11">
         <v>3.6930912718908204</v>
       </c>
     </row>
@@ -4031,15 +4029,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E97" s="5">
+      <c r="E97" s="11">
         <f t="shared" si="8"/>
         <v>9.4738520408163289</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="11">
         <f t="shared" si="6"/>
         <v>18.561915061393066</v>
       </c>
-      <c r="G97" s="8">
+      <c r="G97" s="11">
         <v>3.7123830122786132</v>
       </c>
     </row>
@@ -4058,15 +4056,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E98" s="5">
+      <c r="E98" s="11">
         <f t="shared" si="8"/>
         <v>9.5631377551020407</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="11">
         <f t="shared" si="6"/>
         <v>18.657976806082026</v>
       </c>
-      <c r="G98" s="8">
+      <c r="G98" s="11">
         <v>3.7315953612164052</v>
       </c>
     </row>
@@ -4085,15 +4083,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E99" s="5">
+      <c r="E99" s="11">
         <f t="shared" si="8"/>
         <v>9.652423469387756</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="11">
         <f t="shared" si="6"/>
         <v>18.75364725297846</v>
       </c>
-      <c r="G99" s="8">
+      <c r="G99" s="11">
         <v>3.7507294505956921</v>
       </c>
     </row>
@@ -4112,15 +4110,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E100" s="5">
+      <c r="E100" s="11">
         <f t="shared" si="8"/>
         <v>9.7417091836734695</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="11">
         <f t="shared" si="6"/>
         <v>18.848931924611136</v>
       </c>
-      <c r="G100" s="8">
+      <c r="G100" s="11">
         <v>3.7697863849222273</v>
       </c>
     </row>
@@ -4139,15 +4137,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E101" s="11">
         <f t="shared" si="8"/>
         <v>9.830994897959183</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="11">
         <f t="shared" si="6"/>
         <v>18.9438362112266</v>
       </c>
-      <c r="G101" s="8">
+      <c r="G101" s="11">
         <v>3.7887672422453198</v>
       </c>
     </row>
@@ -4166,15 +4164,15 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E102" s="5">
+      <c r="E102" s="11">
         <f t="shared" si="8"/>
         <v>9.9202806122449001</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="11">
         <f t="shared" si="6"/>
         <v>19.038365375233763</v>
       </c>
-      <c r="G102" s="8">
+      <c r="G102" s="11">
         <v>3.8076730750467527</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a simple upgrade equip func
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelExp.xlsx
+++ b/ConfigData/Xlsx/LevelExp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>CardLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备升级经验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipExp</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -839,7 +851,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <b val="0"/>
@@ -938,6 +950,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1102,14 +1143,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G102" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A3:G102"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Id" dataDxfId="6"/>
-    <tableColumn id="2" name="Exp" dataDxfId="5"/>
-    <tableColumn id="3" name="CardExp" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H102" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A3:H102"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Id" dataDxfId="7"/>
+    <tableColumn id="2" name="Exp" dataDxfId="6"/>
+    <tableColumn id="3" name="CardExp" dataDxfId="5"/>
+    <tableColumn id="9" name="EquipExp" dataDxfId="4"/>
     <tableColumn id="4" name="TowerLevel" dataDxfId="3">
-      <calculatedColumnFormula>INT(E4)</calculatedColumnFormula>
+      <calculatedColumnFormula>INT(F4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="CardLevel" dataDxfId="2"/>
     <tableColumn id="6" name="GoldFactor" dataDxfId="1">
@@ -1442,20 +1484,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="7" width="6.875" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="7.125" customWidth="1"/>
+    <col min="6" max="8" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1466,19 +1509,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1489,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
@@ -1500,8 +1546,11 @@
       <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1512,19 +1561,22 @@
         <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1534,22 +1586,25 @@
       <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
-        <f>INT(E4)</f>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="5">
+        <f>INT(F4)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="11">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="11">
-        <f>POWER(A4+3,0.6)+3</f>
+      <c r="G4" s="11">
+        <f t="shared" ref="G4:G35" si="0">POWER(A4+3,0.6)+3</f>
         <v>5.2973967099940698</v>
       </c>
-      <c r="G4" s="11">
+      <c r="H4" s="11">
         <v>1.059479341998814</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -1559,22 +1614,25 @@
       <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="5">
-        <f t="shared" ref="D5:D68" si="0">INT(E5)</f>
+      <c r="D5" s="4">
+        <v>200</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" ref="E5:E68" si="1">INT(F5)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="F5" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:F68" si="1">POWER(A5+3,0.6)+3</f>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
         <v>5.626527804403767</v>
       </c>
-      <c r="G5" s="11">
+      <c r="H5" s="11">
         <v>1.1253055608807534</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -1584,22 +1642,25 @@
       <c r="C6" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
+        <v>500</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E6" s="11">
-        <v>1.2</v>
-      </c>
-      <c r="F6" s="11">
-        <f t="shared" si="1"/>
         <v>5.9301560515835217</v>
       </c>
-      <c r="G6" s="11">
+      <c r="H6" s="11">
         <v>1.1860312103167043</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -1610,22 +1671,25 @@
       <c r="C7" s="4">
         <v>20</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
+        <v>1500</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E7" s="11">
-        <v>1.3</v>
-      </c>
-      <c r="F7" s="11">
-        <f t="shared" si="1"/>
         <v>6.2140958497160383</v>
       </c>
-      <c r="G7" s="11">
+      <c r="H7" s="11">
         <v>1.2428191699432076</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -1636,22 +1700,25 @@
       <c r="C8" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
+        <v>5000</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="11">
-        <v>1.4</v>
-      </c>
-      <c r="F8" s="11">
-        <f t="shared" si="1"/>
         <v>6.4822022531844965</v>
       </c>
-      <c r="G8" s="11">
+      <c r="H8" s="11">
         <v>1.2964404506368994</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -1662,22 +1729,25 @@
       <c r="C9" s="4">
         <v>80</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E9" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="1"/>
         <v>6.7371928188465517</v>
       </c>
-      <c r="G9" s="11">
+      <c r="H9" s="11">
         <v>1.3474385637693103</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -1688,22 +1758,25 @@
       <c r="C10" s="4">
         <v>200</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
+        <v>20000</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E10" s="11">
-        <v>1.6</v>
-      </c>
-      <c r="F10" s="11">
-        <f t="shared" si="1"/>
         <v>6.9810717055349727</v>
       </c>
-      <c r="G10" s="11">
+      <c r="H10" s="11">
         <v>1.3962143411069945</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -1715,22 +1788,26 @@
         <f>C10+500</f>
         <v>700</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
+        <f>D10*2</f>
+        <v>40000</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="G11" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E11" s="11">
-        <v>1.7</v>
-      </c>
-      <c r="F11" s="11">
-        <f t="shared" si="1"/>
         <v>7.2153691330919001</v>
       </c>
-      <c r="G11" s="11">
+      <c r="H11" s="11">
         <v>1.44307382661838</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -1742,22 +1819,26 @@
         <f t="shared" ref="C12" si="3">C11+500</f>
         <v>1200</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
+        <f t="shared" ref="D12:D23" si="4">D11*2</f>
+        <v>80000</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="G12" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E12" s="11">
-        <v>1.8</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="1"/>
         <v>7.4412860698458401</v>
       </c>
-      <c r="G12" s="11">
+      <c r="H12" s="11">
         <v>1.4882572139691681</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -1768,22 +1849,26 @@
       <c r="C13" s="5">
         <v>999999</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
+        <f t="shared" si="4"/>
+        <v>160000</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="G13" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="11">
-        <v>1.9</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="1"/>
         <v>7.6597864200360659</v>
       </c>
-      <c r="G13" s="11">
+      <c r="H13" s="11">
         <v>1.5319572840072131</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -1794,22 +1879,26 @@
       <c r="C14" s="5">
         <v>999999</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
+        <f t="shared" si="4"/>
+        <v>320000</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="11">
+        <v>2</v>
+      </c>
+      <c r="G14" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E14" s="11">
-        <v>2</v>
-      </c>
-      <c r="F14" s="11">
-        <f t="shared" si="1"/>
         <v>7.8716583257669139</v>
       </c>
-      <c r="G14" s="11">
+      <c r="H14" s="11">
         <v>1.5743316651533827</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -1820,22 +1909,26 @@
       <c r="C15" s="5">
         <v>999999</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
+        <f t="shared" si="4"/>
+        <v>640000</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F15" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="G15" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E15" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="F15" s="11">
-        <f t="shared" si="1"/>
         <v>8.0775563919874074</v>
       </c>
-      <c r="G15" s="11">
+      <c r="H15" s="11">
         <v>1.6155112783974814</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -1846,22 +1939,26 @@
       <c r="C16" s="5">
         <v>999999</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
+        <f t="shared" si="4"/>
+        <v>1280000</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G16" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E16" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F16" s="11">
-        <f t="shared" si="1"/>
         <v>8.2780316430915768</v>
       </c>
-      <c r="G16" s="11">
+      <c r="H16" s="11">
         <v>1.6556063286183154</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -1872,22 +1969,26 @@
       <c r="C17" s="5">
         <v>999999</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
+        <f t="shared" si="4"/>
+        <v>2560000</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G17" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E17" s="11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
         <v>8.4735533169184887</v>
       </c>
-      <c r="G17" s="11">
+      <c r="H17" s="11">
         <v>1.6947106633836977</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -1898,22 +1999,26 @@
       <c r="C18" s="5">
         <v>999999</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
+        <f t="shared" si="4"/>
+        <v>5120000</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="11">
+        <v>2.4</v>
+      </c>
+      <c r="G18" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E18" s="11">
-        <v>2.4</v>
-      </c>
-      <c r="F18" s="11">
-        <f t="shared" si="1"/>
         <v>8.6645250677694108</v>
       </c>
-      <c r="G18" s="11">
+      <c r="H18" s="11">
         <v>1.7329050135538822</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="5">
         <v>16</v>
       </c>
@@ -1924,22 +2029,26 @@
       <c r="C19" s="5">
         <v>999999</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
+        <f t="shared" si="4"/>
+        <v>10240000</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E19" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="F19" s="11">
-        <f t="shared" si="1"/>
         <v>8.8512972424092151</v>
       </c>
-      <c r="G19" s="11">
+      <c r="H19" s="11">
         <v>1.770259448481843</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -1950,22 +2059,26 @@
       <c r="C20" s="5">
         <v>999999</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
+        <f t="shared" si="4"/>
+        <v>20480000</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>2.6</v>
+      </c>
+      <c r="G20" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E20" s="11">
-        <v>2.6</v>
-      </c>
-      <c r="F20" s="11">
-        <f t="shared" si="1"/>
         <v>9.0341763365451619</v>
       </c>
-      <c r="G20" s="11">
+      <c r="H20" s="11">
         <v>1.8068352673090324</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="5">
         <v>18</v>
       </c>
@@ -1976,22 +2089,26 @@
       <c r="C21" s="5">
         <v>999999</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
+        <f t="shared" si="4"/>
+        <v>40960000</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F21" s="11">
+        <v>2.7</v>
+      </c>
+      <c r="G21" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E21" s="11">
-        <v>2.7</v>
-      </c>
-      <c r="F21" s="11">
-        <f t="shared" si="1"/>
         <v>9.2134323873607435</v>
       </c>
-      <c r="G21" s="11">
+      <c r="H21" s="11">
         <v>1.8426864774721488</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -2002,22 +2119,26 @@
       <c r="C22" s="5">
         <v>999999</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
+        <f t="shared" si="4"/>
+        <v>81920000</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="G22" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E22" s="11">
-        <v>2.8</v>
-      </c>
-      <c r="F22" s="11">
-        <f t="shared" si="1"/>
         <v>9.3893048289839669</v>
       </c>
-      <c r="G22" s="11">
+      <c r="H22" s="11">
         <v>1.8778609657967933</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="5">
         <v>20</v>
       </c>
@@ -2028,22 +2149,26 @@
       <c r="C23" s="5">
         <v>999999</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
+        <f t="shared" si="4"/>
+        <v>163840000</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F23" s="11">
+        <v>2.9</v>
+      </c>
+      <c r="G23" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E23" s="11">
-        <v>2.9</v>
-      </c>
-      <c r="F23" s="11">
-        <f t="shared" si="1"/>
         <v>9.5620071855158546</v>
       </c>
-      <c r="G23" s="11">
+      <c r="H23" s="11">
         <v>1.912401437103171</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="5">
         <v>21</v>
       </c>
@@ -2055,22 +2180,25 @@
         <v>999999</v>
       </c>
       <c r="D24" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" ref="F24:F55" si="5">3.3+(A24-21)*0.1-F23*0.12</f>
+        <v>2.952</v>
+      </c>
+      <c r="G24" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E24" s="11">
-        <f>3.3+(A24-21)*0.1-E23*0.12</f>
-        <v>2.952</v>
-      </c>
-      <c r="F24" s="11">
-        <f t="shared" si="1"/>
         <v>9.7317308726771969</v>
       </c>
-      <c r="G24" s="11">
+      <c r="H24" s="11">
         <v>1.9463461745354393</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="5">
         <v>22</v>
       </c>
@@ -2082,22 +2210,25 @@
         <v>999999</v>
       </c>
       <c r="D25" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="5"/>
+        <v>3.04576</v>
+      </c>
+      <c r="G25" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E25" s="11">
-        <f t="shared" ref="E25:E88" si="4">3.3+(A25-21)*0.1-E24*0.12</f>
-        <v>3.04576</v>
-      </c>
-      <c r="F25" s="11">
-        <f t="shared" si="1"/>
         <v>9.8986483073060718</v>
       </c>
-      <c r="G25" s="11">
+      <c r="H25" s="11">
         <v>1.9797296614612143</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -2109,22 +2240,25 @@
         <v>999999</v>
       </c>
       <c r="D26" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" si="5"/>
+        <v>3.1345087999999999</v>
+      </c>
+      <c r="G26" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E26" s="11">
-        <f t="shared" si="4"/>
-        <v>3.1345087999999999</v>
-      </c>
-      <c r="F26" s="11">
-        <f t="shared" si="1"/>
         <v>10.062915473248847</v>
       </c>
-      <c r="G26" s="11">
+      <c r="H26" s="11">
         <v>2.0125830946497691</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="5">
         <v>24</v>
       </c>
@@ -2136,22 +2270,25 @@
         <v>999999</v>
       </c>
       <c r="D27" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="5"/>
+        <v>3.2238589439999998</v>
+      </c>
+      <c r="G27" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E27" s="11">
-        <f t="shared" si="4"/>
-        <v>3.2238589439999998</v>
-      </c>
-      <c r="F27" s="11">
-        <f t="shared" si="1"/>
         <v>10.224674055842076</v>
       </c>
-      <c r="G27" s="11">
+      <c r="H27" s="11">
         <v>2.0449348111684151</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="5">
         <v>25</v>
       </c>
@@ -2163,22 +2300,25 @@
         <v>999999</v>
       </c>
       <c r="D28" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" si="5"/>
+        <v>3.3131369267199999</v>
+      </c>
+      <c r="G28" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E28" s="11">
-        <f t="shared" si="4"/>
-        <v>3.3131369267199999</v>
-      </c>
-      <c r="F28" s="11">
-        <f t="shared" si="1"/>
         <v>10.38405323074322</v>
       </c>
-      <c r="G28" s="11">
+      <c r="H28" s="11">
         <v>2.076810646148644</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="5">
         <v>26</v>
       </c>
@@ -2190,22 +2330,25 @@
         <v>999999</v>
       </c>
       <c r="D29" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" si="5"/>
+        <v>3.4024235687936</v>
+      </c>
+      <c r="G29" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E29" s="11">
-        <f t="shared" si="4"/>
-        <v>3.4024235687936</v>
-      </c>
-      <c r="F29" s="11">
-        <f t="shared" si="1"/>
         <v>10.541171173377641</v>
       </c>
-      <c r="G29" s="11">
+      <c r="H29" s="11">
         <v>2.1082342346755283</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="5">
         <v>27</v>
       </c>
@@ -2217,22 +2360,25 @@
         <v>999999</v>
       </c>
       <c r="D30" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="5"/>
+        <v>3.4917091717447679</v>
+      </c>
+      <c r="G30" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E30" s="11">
-        <f t="shared" si="4"/>
-        <v>3.4917091717447679</v>
-      </c>
-      <c r="F30" s="11">
-        <f t="shared" si="1"/>
         <v>10.696136340726078</v>
       </c>
-      <c r="G30" s="11">
+      <c r="H30" s="11">
         <v>2.1392272681452154</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="5">
         <v>28</v>
       </c>
@@ -2244,22 +2390,25 @@
         <v>999999</v>
       </c>
       <c r="D31" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="5"/>
+        <v>3.5809948993906278</v>
+      </c>
+      <c r="G31" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E31" s="11">
-        <f t="shared" si="4"/>
-        <v>3.5809948993906278</v>
-      </c>
-      <c r="F31" s="11">
-        <f t="shared" si="1"/>
         <v>10.849048566202034</v>
       </c>
-      <c r="G31" s="11">
+      <c r="H31" s="11">
         <v>2.1698097132404071</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="5">
         <v>29</v>
       </c>
@@ -2271,22 +2420,25 @@
         <v>999999</v>
       </c>
       <c r="D32" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="5"/>
+        <v>3.6702806120731242</v>
+      </c>
+      <c r="G32" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E32" s="11">
-        <f t="shared" si="4"/>
-        <v>3.6702806120731242</v>
-      </c>
-      <c r="F32" s="11">
-        <f t="shared" si="1"/>
         <v>10.999999999999998</v>
       </c>
-      <c r="G32" s="11">
+      <c r="H32" s="11">
         <v>2.1999999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="5">
         <v>30</v>
       </c>
@@ -2298,22 +2450,25 @@
         <v>999999</v>
       </c>
       <c r="D33" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="5"/>
+        <v>3.7595663265512251</v>
+      </c>
+      <c r="G33" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E33" s="11">
-        <f t="shared" si="4"/>
-        <v>3.7595663265512251</v>
-      </c>
-      <c r="F33" s="11">
-        <f t="shared" si="1"/>
         <v>11.149075920852829</v>
       </c>
-      <c r="G33" s="11">
+      <c r="H33" s="11">
         <v>2.2298151841705658</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="5">
         <v>31</v>
       </c>
@@ -2325,22 +2480,25 @@
         <v>999999</v>
       </c>
       <c r="D34" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="5"/>
+        <v>3.8488520408138527</v>
+      </c>
+      <c r="G34" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E34" s="11">
-        <f t="shared" si="4"/>
-        <v>3.8488520408138527</v>
-      </c>
-      <c r="F34" s="11">
-        <f t="shared" si="1"/>
         <v>11.296355440131292</v>
       </c>
-      <c r="G34" s="11">
+      <c r="H34" s="11">
         <v>2.2592710880262583</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="5">
         <v>32</v>
       </c>
@@ -2352,22 +2510,25 @@
         <v>999999</v>
       </c>
       <c r="D35" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F35" s="11">
+        <f t="shared" si="5"/>
+        <v>3.9381377551023382</v>
+      </c>
+      <c r="G35" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E35" s="11">
-        <f t="shared" si="4"/>
-        <v>3.9381377551023382</v>
-      </c>
-      <c r="F35" s="11">
-        <f t="shared" si="1"/>
         <v>11.441912115297924</v>
       </c>
-      <c r="G35" s="11">
+      <c r="H35" s="11">
         <v>2.2883824230595851</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="5">
         <v>33</v>
       </c>
@@ -2379,22 +2540,25 @@
         <v>999999</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E36" s="11">
-        <f t="shared" si="4"/>
+      <c r="F36" s="11">
+        <f t="shared" si="5"/>
         <v>4.0274234693877196</v>
       </c>
-      <c r="F36" s="11">
-        <f t="shared" si="1"/>
+      <c r="G36" s="11">
+        <f t="shared" ref="G36:G67" si="6">POWER(A36+3,0.6)+3</f>
         <v>11.585814486631531</v>
       </c>
-      <c r="G36" s="11">
+      <c r="H36" s="11">
         <v>2.3171628973263063</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" s="5">
         <v>34</v>
       </c>
@@ -2406,22 +2570,25 @@
         <v>999999</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E37" s="11">
-        <f t="shared" si="4"/>
+      <c r="F37" s="11">
+        <f t="shared" si="5"/>
         <v>4.116709183673473</v>
       </c>
-      <c r="F37" s="11">
-        <f t="shared" si="1"/>
+      <c r="G37" s="11">
+        <f t="shared" si="6"/>
         <v>11.72812654867613</v>
       </c>
-      <c r="G37" s="11">
+      <c r="H37" s="11">
         <v>2.345625309735226</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="5">
         <v>35</v>
       </c>
@@ -2433,22 +2600,25 @@
         <v>999999</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E38" s="11">
-        <f t="shared" si="4"/>
+      <c r="F38" s="11">
+        <f t="shared" si="5"/>
         <v>4.205994897959183</v>
       </c>
-      <c r="F38" s="11">
-        <f t="shared" si="1"/>
+      <c r="G38" s="11">
+        <f t="shared" si="6"/>
         <v>11.868908165896258</v>
       </c>
-      <c r="G38" s="11">
+      <c r="H38" s="11">
         <v>2.3737816331792514</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" s="5">
         <v>36</v>
       </c>
@@ -2460,22 +2630,25 @@
         <v>999999</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E39" s="11">
-        <f t="shared" si="4"/>
+      <c r="F39" s="11">
+        <f t="shared" si="5"/>
         <v>4.2952806122448983</v>
       </c>
-      <c r="F39" s="11">
-        <f t="shared" si="1"/>
+      <c r="G39" s="11">
+        <f t="shared" si="6"/>
         <v>12.008215440430581</v>
       </c>
-      <c r="G39" s="11">
+      <c r="H39" s="11">
         <v>2.4016430880861162</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="5">
         <v>37</v>
       </c>
@@ -2487,22 +2660,25 @@
         <v>999999</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E40" s="11">
-        <f t="shared" si="4"/>
+      <c r="F40" s="11">
+        <f t="shared" si="5"/>
         <v>4.3845663265306127</v>
       </c>
-      <c r="F40" s="11">
-        <f t="shared" si="1"/>
+      <c r="G40" s="11">
+        <f t="shared" si="6"/>
         <v>12.146101038546524</v>
       </c>
-      <c r="G40" s="11">
+      <c r="H40" s="11">
         <v>2.4292202077093048</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="5">
         <v>38</v>
       </c>
@@ -2514,22 +2690,25 @@
         <v>999999</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E41" s="11">
-        <f t="shared" si="4"/>
+      <c r="F41" s="11">
+        <f t="shared" si="5"/>
         <v>4.4738520408163263</v>
       </c>
-      <c r="F41" s="11">
-        <f t="shared" si="1"/>
+      <c r="G41" s="11">
+        <f t="shared" si="6"/>
         <v>12.282614481346684</v>
       </c>
-      <c r="G41" s="11">
+      <c r="H41" s="11">
         <v>2.4565228962693366</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="5">
         <v>39</v>
       </c>
@@ -2541,22 +2720,25 @@
         <v>999999</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E42" s="11">
-        <f t="shared" si="4"/>
+      <c r="F42" s="11">
+        <f t="shared" si="5"/>
         <v>4.5631377551020407</v>
       </c>
-      <c r="F42" s="11">
-        <f t="shared" si="1"/>
+      <c r="G42" s="11">
+        <f t="shared" si="6"/>
         <v>12.41780240441493</v>
       </c>
-      <c r="G42" s="11">
+      <c r="H42" s="11">
         <v>2.4835604808829861</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="5">
         <v>40</v>
       </c>
@@ -2568,22 +2750,25 @@
         <v>999999</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E43" s="11">
-        <f t="shared" si="4"/>
+      <c r="F43" s="11">
+        <f t="shared" si="5"/>
         <v>4.6524234693877551</v>
       </c>
-      <c r="F43" s="11">
-        <f t="shared" si="1"/>
+      <c r="G43" s="11">
+        <f t="shared" si="6"/>
         <v>12.551708790378902</v>
       </c>
-      <c r="G43" s="11">
+      <c r="H43" s="11">
         <v>2.5103417580757803</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="5">
         <v>41</v>
       </c>
@@ -2595,22 +2780,25 @@
         <v>999999</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E44" s="11">
-        <f t="shared" si="4"/>
+      <c r="F44" s="11">
+        <f t="shared" si="5"/>
         <v>4.7417091836734695</v>
       </c>
-      <c r="F44" s="11">
-        <f t="shared" si="1"/>
+      <c r="G44" s="11">
+        <f t="shared" si="6"/>
         <v>12.684375177775884</v>
       </c>
-      <c r="G44" s="11">
+      <c r="H44" s="11">
         <v>2.5368750355551768</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="5">
         <v>42</v>
       </c>
@@ -2622,22 +2810,25 @@
         <v>999999</v>
       </c>
       <c r="D45" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E45" s="11">
-        <f t="shared" si="4"/>
+      <c r="F45" s="11">
+        <f t="shared" si="5"/>
         <v>4.8309948979591839</v>
       </c>
-      <c r="F45" s="11">
-        <f t="shared" si="1"/>
+      <c r="G45" s="11">
+        <f t="shared" si="6"/>
         <v>12.81584084911856</v>
       </c>
-      <c r="G45" s="11">
+      <c r="H45" s="11">
         <v>2.5631681698237121</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="5">
         <v>43</v>
       </c>
@@ -2649,22 +2840,25 @@
         <v>999999</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E46" s="11">
-        <f t="shared" si="4"/>
+      <c r="F46" s="11">
+        <f t="shared" si="5"/>
         <v>4.9202806122448983</v>
       </c>
-      <c r="F46" s="11">
-        <f t="shared" si="1"/>
+      <c r="G46" s="11">
+        <f t="shared" si="6"/>
         <v>12.946143000646654</v>
       </c>
-      <c r="G46" s="11">
+      <c r="H46" s="11">
         <v>2.5892286001293305</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="5">
         <v>44</v>
       </c>
@@ -2676,22 +2870,25 @@
         <v>999999</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E47" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E47" s="11">
-        <f t="shared" si="4"/>
+      <c r="F47" s="11">
+        <f t="shared" si="5"/>
         <v>5.0095663265306118</v>
       </c>
-      <c r="F47" s="11">
-        <f t="shared" si="1"/>
+      <c r="G47" s="11">
+        <f t="shared" si="6"/>
         <v>13.075316895906047</v>
       </c>
-      <c r="G47" s="11">
+      <c r="H47" s="11">
         <v>2.6150633791812092</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="5">
         <v>45</v>
       </c>
@@ -2703,22 +2900,25 @@
         <v>999999</v>
       </c>
       <c r="D48" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E48" s="11">
-        <f t="shared" si="4"/>
+      <c r="F48" s="11">
+        <f t="shared" si="5"/>
         <v>5.0988520408163271</v>
       </c>
-      <c r="F48" s="11">
-        <f t="shared" si="1"/>
+      <c r="G48" s="11">
+        <f t="shared" si="6"/>
         <v>13.203396005006329</v>
       </c>
-      <c r="G48" s="11">
+      <c r="H48" s="11">
         <v>2.6406792010012659</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" s="5">
         <v>46</v>
       </c>
@@ -2730,22 +2930,25 @@
         <v>999999</v>
       </c>
       <c r="D49" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E49" s="11">
-        <f t="shared" si="4"/>
+      <c r="F49" s="11">
+        <f t="shared" si="5"/>
         <v>5.1881377551020407</v>
       </c>
-      <c r="F49" s="11">
-        <f t="shared" si="1"/>
+      <c r="G49" s="11">
+        <f t="shared" si="6"/>
         <v>13.330412131161864</v>
       </c>
-      <c r="G49" s="11">
+      <c r="H49" s="11">
         <v>2.6660824262323728</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" s="5">
         <v>47</v>
       </c>
@@ -2757,22 +2960,25 @@
         <v>999999</v>
       </c>
       <c r="D50" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E50" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E50" s="11">
-        <f t="shared" si="4"/>
+      <c r="F50" s="11">
+        <f t="shared" si="5"/>
         <v>5.277423469387756</v>
       </c>
-      <c r="F50" s="11">
-        <f t="shared" si="1"/>
+      <c r="G50" s="11">
+        <f t="shared" si="6"/>
         <v>13.456395525912733</v>
       </c>
-      <c r="G50" s="11">
+      <c r="H50" s="11">
         <v>2.6912791051825464</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="5">
         <v>48</v>
       </c>
@@ -2784,22 +2990,25 @@
         <v>999999</v>
       </c>
       <c r="D51" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E51" s="11">
-        <f t="shared" si="4"/>
+      <c r="F51" s="11">
+        <f t="shared" si="5"/>
         <v>5.3667091836734695</v>
       </c>
-      <c r="F51" s="11">
-        <f t="shared" si="1"/>
+      <c r="G51" s="11">
+        <f t="shared" si="6"/>
         <v>13.581374994243514</v>
       </c>
-      <c r="G51" s="11">
+      <c r="H51" s="11">
         <v>2.7162749988487027</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="5">
         <v>49</v>
       </c>
@@ -2811,22 +3020,25 @@
         <v>999999</v>
       </c>
       <c r="D52" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E52" s="11">
-        <f t="shared" si="4"/>
+      <c r="F52" s="11">
+        <f t="shared" si="5"/>
         <v>5.455994897959183</v>
       </c>
-      <c r="F52" s="11">
-        <f t="shared" si="1"/>
+      <c r="G52" s="11">
+        <f t="shared" si="6"/>
         <v>13.705377990665905</v>
       </c>
-      <c r="G52" s="11">
+      <c r="H52" s="11">
         <v>2.7410755981331811</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="5">
         <v>50</v>
       </c>
@@ -2838,22 +3050,25 @@
         <v>999999</v>
       </c>
       <c r="D53" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E53" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E53" s="11">
-        <f t="shared" si="4"/>
+      <c r="F53" s="11">
+        <f t="shared" si="5"/>
         <v>5.5452806122448983</v>
       </c>
-      <c r="F53" s="11">
-        <f t="shared" si="1"/>
+      <c r="G53" s="11">
+        <f t="shared" si="6"/>
         <v>13.828430707200107</v>
       </c>
-      <c r="G53" s="11">
+      <c r="H53" s="11">
         <v>2.7656861414400216</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="5">
         <v>51</v>
       </c>
@@ -2865,22 +3080,25 @@
         <v>999999</v>
       </c>
       <c r="D54" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E54" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E54" s="11">
-        <f t="shared" si="4"/>
+      <c r="F54" s="11">
+        <f t="shared" si="5"/>
         <v>5.6345663265306118</v>
       </c>
-      <c r="F54" s="11">
-        <f t="shared" si="1"/>
+      <c r="G54" s="11">
+        <f t="shared" si="6"/>
         <v>13.950558154077704</v>
       </c>
-      <c r="G54" s="11">
+      <c r="H54" s="11">
         <v>2.7901116308155407</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="5">
         <v>52</v>
       </c>
@@ -2892,22 +3110,25 @@
         <v>999999</v>
       </c>
       <c r="D55" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E55" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E55" s="11">
-        <f t="shared" si="4"/>
+      <c r="F55" s="11">
+        <f t="shared" si="5"/>
         <v>5.7238520408163271</v>
       </c>
-      <c r="F55" s="11">
-        <f t="shared" si="1"/>
+      <c r="G55" s="11">
+        <f t="shared" si="6"/>
         <v>14.071784233891282</v>
       </c>
-      <c r="G55" s="11">
+      <c r="H55" s="11">
         <v>2.8143568467782565</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="5">
         <v>53</v>
       </c>
@@ -2919,22 +3140,25 @@
         <v>999999</v>
       </c>
       <c r="D56" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E56" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E56" s="11">
-        <f t="shared" si="4"/>
+      <c r="F56" s="11">
+        <f t="shared" ref="F56:F87" si="7">3.3+(A56-21)*0.1-F55*0.12</f>
         <v>5.8131377551020407</v>
       </c>
-      <c r="F56" s="11">
-        <f t="shared" si="1"/>
+      <c r="G56" s="11">
+        <f t="shared" si="6"/>
         <v>14.192131809832132</v>
       </c>
-      <c r="G56" s="11">
+      <c r="H56" s="11">
         <v>2.8384263619664263</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="5">
         <v>54</v>
       </c>
@@ -2946,22 +3170,25 @@
         <v>999999</v>
       </c>
       <c r="D57" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E57" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E57" s="11">
-        <f t="shared" si="4"/>
+      <c r="F57" s="11">
+        <f t="shared" si="7"/>
         <v>5.9024234693877551</v>
       </c>
-      <c r="F57" s="11">
-        <f t="shared" si="1"/>
+      <c r="G57" s="11">
+        <f t="shared" si="6"/>
         <v>14.311622768584231</v>
       </c>
-      <c r="G57" s="11">
+      <c r="H57" s="11">
         <v>2.8623245537168462</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="5">
         <v>55</v>
       </c>
@@ -2973,22 +3200,25 @@
         <v>999999</v>
       </c>
       <c r="D58" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E58" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E58" s="11">
-        <f t="shared" si="4"/>
+      <c r="F58" s="11">
+        <f t="shared" si="7"/>
         <v>5.9917091836734695</v>
       </c>
-      <c r="F58" s="11">
-        <f t="shared" si="1"/>
+      <c r="G58" s="11">
+        <f t="shared" si="6"/>
         <v>14.430278078379143</v>
       </c>
-      <c r="G58" s="11">
+      <c r="H58" s="11">
         <v>2.8860556156758284</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="5">
         <v>56</v>
       </c>
@@ -3000,22 +3230,25 @@
         <v>999999</v>
       </c>
       <c r="D59" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E59" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E59" s="11">
-        <f t="shared" si="4"/>
+      <c r="F59" s="11">
+        <f t="shared" si="7"/>
         <v>6.080994897959183</v>
       </c>
-      <c r="F59" s="11">
-        <f t="shared" si="1"/>
+      <c r="G59" s="11">
+        <f t="shared" si="6"/>
         <v>14.548117842660861</v>
       </c>
-      <c r="G59" s="11">
+      <c r="H59" s="11">
         <v>2.9096235685321723</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="5">
         <v>57</v>
       </c>
@@ -3027,22 +3260,25 @@
         <v>999999</v>
       </c>
       <c r="D60" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E60" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E60" s="11">
-        <f t="shared" si="4"/>
+      <c r="F60" s="11">
+        <f t="shared" si="7"/>
         <v>6.1702806122448983</v>
       </c>
-      <c r="F60" s="11">
-        <f t="shared" si="1"/>
+      <c r="G60" s="11">
+        <f t="shared" si="6"/>
         <v>14.665161349761227</v>
       </c>
-      <c r="G60" s="11">
+      <c r="H60" s="11">
         <v>2.9330322699522453</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A61" s="5">
         <v>58</v>
       </c>
@@ -3054,22 +3290,25 @@
         <v>999999</v>
       </c>
       <c r="D61" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E61" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E61" s="11">
-        <f t="shared" si="4"/>
+      <c r="F61" s="11">
+        <f t="shared" si="7"/>
         <v>6.2595663265306118</v>
       </c>
-      <c r="F61" s="11">
-        <f t="shared" si="1"/>
+      <c r="G61" s="11">
+        <f t="shared" si="6"/>
         <v>14.781427118943885</v>
       </c>
-      <c r="G61" s="11">
+      <c r="H61" s="11">
         <v>2.9562854237887768</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" s="5">
         <v>59</v>
       </c>
@@ -3081,22 +3320,25 @@
         <v>999999</v>
       </c>
       <c r="D62" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E62" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E62" s="11">
-        <f t="shared" si="4"/>
+      <c r="F62" s="11">
+        <f t="shared" si="7"/>
         <v>6.3488520408163263</v>
       </c>
-      <c r="F62" s="11">
-        <f t="shared" si="1"/>
+      <c r="G62" s="11">
+        <f t="shared" si="6"/>
         <v>14.896932943137111</v>
       </c>
-      <c r="G62" s="11">
+      <c r="H62" s="11">
         <v>2.9793865886274222</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A63" s="5">
         <v>60</v>
       </c>
@@ -3108,22 +3350,25 @@
         <v>999999</v>
       </c>
       <c r="D63" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E63" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E63" s="11">
-        <f t="shared" si="4"/>
+      <c r="F63" s="11">
+        <f t="shared" si="7"/>
         <v>6.4381377551020407</v>
       </c>
-      <c r="F63" s="11">
-        <f t="shared" si="1"/>
+      <c r="G63" s="11">
+        <f t="shared" si="6"/>
         <v>15.011695928643283</v>
       </c>
-      <c r="G63" s="11">
+      <c r="H63" s="11">
         <v>3.0023391857286565</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A64" s="5">
         <v>61</v>
       </c>
@@ -3135,22 +3380,25 @@
         <v>999999</v>
       </c>
       <c r="D64" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E64" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E64" s="11">
-        <f t="shared" si="4"/>
+      <c r="F64" s="11">
+        <f t="shared" si="7"/>
         <v>6.5274234693877551</v>
       </c>
-      <c r="F64" s="11">
-        <f t="shared" si="1"/>
+      <c r="G64" s="11">
+        <f t="shared" si="6"/>
         <v>15.125732532083184</v>
       </c>
-      <c r="G64" s="11">
+      <c r="H64" s="11">
         <v>3.025146506416637</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="5">
         <v>62</v>
       </c>
@@ -3162,22 +3410,25 @@
         <v>999999</v>
       </c>
       <c r="D65" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E65" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E65" s="11">
-        <f t="shared" si="4"/>
+      <c r="F65" s="11">
+        <f t="shared" si="7"/>
         <v>6.6167091836734695</v>
       </c>
-      <c r="F65" s="11">
-        <f t="shared" si="1"/>
+      <c r="G65" s="11">
+        <f t="shared" si="6"/>
         <v>15.239058594807814</v>
       </c>
-      <c r="G65" s="11">
+      <c r="H65" s="11">
         <v>3.0478117189615626</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="5">
         <v>63</v>
       </c>
@@ -3189,22 +3440,25 @@
         <v>999999</v>
       </c>
       <c r="D66" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E66" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E66" s="11">
-        <f t="shared" si="4"/>
+      <c r="F66" s="11">
+        <f t="shared" si="7"/>
         <v>6.7059948979591839</v>
       </c>
-      <c r="F66" s="11">
-        <f t="shared" si="1"/>
+      <c r="G66" s="11">
+        <f t="shared" si="6"/>
         <v>15.351689374987611</v>
       </c>
-      <c r="G66" s="11">
+      <c r="H66" s="11">
         <v>3.0703378749975223</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="5">
         <v>64</v>
       </c>
@@ -3216,22 +3470,25 @@
         <v>999999</v>
       </c>
       <c r="D67" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E67" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E67" s="11">
-        <f t="shared" si="4"/>
+      <c r="F67" s="11">
+        <f t="shared" si="7"/>
         <v>6.7952806122448974</v>
       </c>
-      <c r="F67" s="11">
-        <f t="shared" si="1"/>
+      <c r="G67" s="11">
+        <f t="shared" si="6"/>
         <v>15.463639577568394</v>
       </c>
-      <c r="G67" s="11">
+      <c r="H67" s="11">
         <v>3.0927279155136786</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" s="5">
         <v>65</v>
       </c>
@@ -3243,22 +3500,25 @@
         <v>999999</v>
       </c>
       <c r="D68" s="5">
-        <f t="shared" si="0"/>
+        <v>999999999</v>
+      </c>
+      <c r="E68" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E68" s="11">
-        <f t="shared" si="4"/>
+      <c r="F68" s="11">
+        <f t="shared" si="7"/>
         <v>6.8845663265306127</v>
       </c>
-      <c r="F68" s="11">
-        <f t="shared" si="1"/>
+      <c r="G68" s="11">
+        <f t="shared" ref="G68:G102" si="8">POWER(A68+3,0.6)+3</f>
         <v>15.574923382265665</v>
       </c>
-      <c r="G68" s="11">
+      <c r="H68" s="11">
         <v>3.1149846764531328</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" s="5">
         <v>66</v>
       </c>
@@ -3270,22 +3530,25 @@
         <v>999999</v>
       </c>
       <c r="D69" s="5">
-        <f t="shared" ref="D69:D102" si="5">INT(E69)</f>
+        <v>999999999</v>
+      </c>
+      <c r="E69" s="5">
+        <f t="shared" ref="E69:E102" si="9">INT(F69)</f>
         <v>6</v>
       </c>
-      <c r="E69" s="11">
-        <f t="shared" si="4"/>
+      <c r="F69" s="11">
+        <f t="shared" si="7"/>
         <v>6.9738520408163263</v>
       </c>
-      <c r="F69" s="11">
-        <f t="shared" ref="F69:F102" si="6">POWER(A69+3,0.6)+3</f>
+      <c r="G69" s="11">
+        <f t="shared" si="8"/>
         <v>15.685554469752462</v>
       </c>
-      <c r="G69" s="11">
+      <c r="H69" s="11">
         <v>3.1371108939504926</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="5">
         <v>67</v>
       </c>
@@ -3297,22 +3560,25 @@
         <v>999999</v>
       </c>
       <c r="D70" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E70" s="5">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="E70" s="11">
-        <f t="shared" si="4"/>
+      <c r="F70" s="11">
+        <f t="shared" si="7"/>
         <v>7.0631377551020416</v>
       </c>
-      <c r="F70" s="11">
-        <f t="shared" si="6"/>
+      <c r="G70" s="11">
+        <f t="shared" si="8"/>
         <v>15.79554604618191</v>
       </c>
-      <c r="G70" s="11">
+      <c r="H70" s="11">
         <v>3.1591092092363819</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="5">
         <v>68</v>
       </c>
@@ -3324,855 +3590,951 @@
         <v>999999</v>
       </c>
       <c r="D71" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E71" s="5">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="E71" s="11">
-        <f t="shared" si="4"/>
+      <c r="F71" s="11">
+        <f t="shared" si="7"/>
         <v>7.1524234693877551</v>
       </c>
-      <c r="F71" s="11">
-        <f t="shared" si="6"/>
+      <c r="G71" s="11">
+        <f t="shared" si="8"/>
         <v>15.904910866172429</v>
       </c>
-      <c r="G71" s="11">
+      <c r="H71" s="11">
         <v>3.1809821732344856</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" s="5">
         <v>69</v>
       </c>
       <c r="B72" s="4">
-        <f t="shared" ref="B72:B102" si="7">INT(B71*0.7+A72*10+A72*A72*3-30)</f>
+        <f t="shared" ref="B72:B102" si="10">INT(B71*0.7+A72*10+A72*A72*3-30)</f>
         <v>46643</v>
       </c>
       <c r="C72" s="5">
         <v>999999</v>
       </c>
       <c r="D72" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="E72" s="11">
-        <f t="shared" si="4"/>
+      <c r="F72" s="11">
+        <f t="shared" si="7"/>
         <v>7.2417091836734713</v>
       </c>
-      <c r="F72" s="11">
-        <f t="shared" si="6"/>
+      <c r="G72" s="11">
+        <f t="shared" si="8"/>
         <v>16.01366125437238</v>
       </c>
-      <c r="G72" s="11">
+      <c r="H72" s="11">
         <v>3.202732250874476</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" s="5">
         <v>70</v>
       </c>
       <c r="B73" s="4">
+        <f t="shared" si="10"/>
+        <v>48020</v>
+      </c>
+      <c r="C73" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D73" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F73" s="11">
         <f t="shared" si="7"/>
-        <v>48020</v>
-      </c>
-      <c r="C73" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D73" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E73" s="11">
-        <f t="shared" si="4"/>
         <v>7.330994897959183</v>
       </c>
-      <c r="F73" s="11">
-        <f t="shared" si="6"/>
+      <c r="G73" s="11">
+        <f t="shared" si="8"/>
         <v>16.121809125710286</v>
       </c>
-      <c r="G73" s="11">
+      <c r="H73" s="11">
         <v>3.2243618251420569</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="5">
         <v>71</v>
       </c>
       <c r="B74" s="4">
+        <f t="shared" si="10"/>
+        <v>49417</v>
+      </c>
+      <c r="C74" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D74" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F74" s="11">
         <f t="shared" si="7"/>
-        <v>49417</v>
-      </c>
-      <c r="C74" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D74" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E74" s="11">
-        <f t="shared" si="4"/>
         <v>7.4202806122448983</v>
       </c>
-      <c r="F74" s="11">
-        <f t="shared" si="6"/>
+      <c r="G74" s="11">
+        <f t="shared" si="8"/>
         <v>16.229366004427643</v>
       </c>
-      <c r="G74" s="11">
+      <c r="H74" s="11">
         <v>3.2458732008855287</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" s="5">
         <v>72</v>
       </c>
       <c r="B75" s="4">
+        <f t="shared" si="10"/>
+        <v>50833</v>
+      </c>
+      <c r="C75" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D75" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F75" s="11">
         <f t="shared" si="7"/>
-        <v>50833</v>
-      </c>
-      <c r="C75" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D75" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E75" s="11">
-        <f t="shared" si="4"/>
         <v>7.5095663265306127</v>
       </c>
-      <c r="F75" s="11">
-        <f t="shared" si="6"/>
+      <c r="G75" s="11">
+        <f t="shared" si="8"/>
         <v>16.336343041982992</v>
       </c>
-      <c r="G75" s="11">
+      <c r="H75" s="11">
         <v>3.2672686083965985</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A76" s="5">
         <v>73</v>
       </c>
       <c r="B76" s="4">
+        <f t="shared" si="10"/>
+        <v>52270</v>
+      </c>
+      <c r="C76" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D76" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F76" s="11">
         <f t="shared" si="7"/>
-        <v>52270</v>
-      </c>
-      <c r="C76" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D76" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E76" s="11">
-        <f t="shared" si="4"/>
         <v>7.5988520408163263</v>
       </c>
-      <c r="F76" s="11">
-        <f t="shared" si="6"/>
+      <c r="G76" s="11">
+        <f t="shared" si="8"/>
         <v>16.442751033908309</v>
       </c>
-      <c r="G76" s="11">
+      <c r="H76" s="11">
         <v>3.2885502067816619</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" s="5">
         <v>74</v>
       </c>
       <c r="B77" s="4">
+        <f t="shared" si="10"/>
+        <v>53727</v>
+      </c>
+      <c r="C77" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D77" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F77" s="11">
         <f t="shared" si="7"/>
-        <v>53727</v>
-      </c>
-      <c r="C77" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D77" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E77" s="11">
-        <f t="shared" si="4"/>
         <v>7.6881377551020424</v>
       </c>
-      <c r="F77" s="11">
-        <f t="shared" si="6"/>
+      <c r="G77" s="11">
+        <f t="shared" si="8"/>
         <v>16.548600435691771</v>
       </c>
-      <c r="G77" s="11">
+      <c r="H77" s="11">
         <v>3.3097200871383543</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="5">
         <v>75</v>
       </c>
       <c r="B78" s="4">
+        <f t="shared" si="10"/>
+        <v>55203</v>
+      </c>
+      <c r="C78" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D78" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E78" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F78" s="11">
         <f t="shared" si="7"/>
-        <v>55203</v>
-      </c>
-      <c r="C78" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D78" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E78" s="11">
-        <f t="shared" si="4"/>
         <v>7.7774234693877542</v>
       </c>
-      <c r="F78" s="11">
-        <f t="shared" si="6"/>
+      <c r="G78" s="11">
+        <f t="shared" si="8"/>
         <v>16.653901377755393</v>
       </c>
-      <c r="G78" s="11">
+      <c r="H78" s="11">
         <v>3.3307802755510787</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="5">
         <v>76</v>
       </c>
       <c r="B79" s="4">
+        <f t="shared" si="10"/>
+        <v>56700</v>
+      </c>
+      <c r="C79" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D79" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E79" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F79" s="11">
         <f t="shared" si="7"/>
-        <v>56700</v>
-      </c>
-      <c r="C79" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D79" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E79" s="11">
-        <f t="shared" si="4"/>
         <v>7.8667091836734704</v>
       </c>
-      <c r="F79" s="11">
-        <f t="shared" si="6"/>
+      <c r="G79" s="11">
+        <f t="shared" si="8"/>
         <v>16.75866367958966</v>
       </c>
-      <c r="G79" s="11">
+      <c r="H79" s="11">
         <v>3.3517327359179321</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" s="5">
         <v>77</v>
       </c>
       <c r="B80" s="4">
+        <f t="shared" si="10"/>
+        <v>58217</v>
+      </c>
+      <c r="C80" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D80" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E80" s="5">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F80" s="11">
         <f t="shared" si="7"/>
-        <v>58217</v>
-      </c>
-      <c r="C80" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D80" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="E80" s="11">
-        <f t="shared" si="4"/>
         <v>7.9559948979591839</v>
       </c>
-      <c r="F80" s="11">
-        <f t="shared" si="6"/>
+      <c r="G80" s="11">
+        <f t="shared" si="8"/>
         <v>16.862896863102925</v>
       </c>
-      <c r="G80" s="11">
+      <c r="H80" s="11">
         <v>3.372579372620585</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" s="5">
         <v>78</v>
       </c>
       <c r="B81" s="4">
+        <f t="shared" si="10"/>
+        <v>59753</v>
+      </c>
+      <c r="C81" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D81" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E81" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F81" s="11">
         <f t="shared" si="7"/>
-        <v>59753</v>
-      </c>
-      <c r="C81" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D81" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E81" s="11">
-        <f t="shared" si="4"/>
         <v>8.0452806122448983</v>
       </c>
-      <c r="F81" s="11">
-        <f t="shared" si="6"/>
+      <c r="G81" s="11">
+        <f t="shared" si="8"/>
         <v>16.966610165238237</v>
       </c>
-      <c r="G81" s="11">
+      <c r="H81" s="11">
         <v>3.3933220330476472</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A82" s="5">
         <v>79</v>
       </c>
       <c r="B82" s="4">
+        <f t="shared" si="10"/>
+        <v>61310</v>
+      </c>
+      <c r="C82" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D82" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E82" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F82" s="11">
         <f t="shared" si="7"/>
-        <v>61310</v>
-      </c>
-      <c r="C82" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D82" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E82" s="11">
-        <f t="shared" si="4"/>
         <v>8.1345663265306136</v>
       </c>
-      <c r="F82" s="11">
-        <f t="shared" si="6"/>
+      <c r="G82" s="11">
+        <f t="shared" si="8"/>
         <v>17.069812549906494</v>
       </c>
-      <c r="G82" s="11">
+      <c r="H82" s="11">
         <v>3.4139625099812987</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" s="5">
         <v>80</v>
       </c>
       <c r="B83" s="4">
+        <f t="shared" si="10"/>
+        <v>62887</v>
+      </c>
+      <c r="C83" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D83" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E83" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F83" s="11">
         <f t="shared" si="7"/>
-        <v>62887</v>
-      </c>
-      <c r="C83" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D83" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E83" s="11">
-        <f t="shared" si="4"/>
         <v>8.2238520408163254</v>
       </c>
-      <c r="F83" s="11">
-        <f t="shared" si="6"/>
+      <c r="G83" s="11">
+        <f t="shared" si="8"/>
         <v>17.172512719280761</v>
       </c>
-      <c r="G83" s="11">
+      <c r="H83" s="11">
         <v>3.4345025438561523</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A84" s="5">
         <v>81</v>
       </c>
       <c r="B84" s="4">
+        <f t="shared" si="10"/>
+        <v>64483</v>
+      </c>
+      <c r="C84" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D84" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E84" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F84" s="11">
         <f t="shared" si="7"/>
-        <v>64483</v>
-      </c>
-      <c r="C84" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D84" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E84" s="11">
-        <f t="shared" si="4"/>
         <v>8.3131377551020424</v>
       </c>
-      <c r="F84" s="11">
-        <f t="shared" si="6"/>
+      <c r="G84" s="11">
+        <f t="shared" si="8"/>
         <v>17.274719124493167</v>
       </c>
-      <c r="G84" s="11">
+      <c r="H84" s="11">
         <v>3.4549438248986335</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A85" s="5">
         <v>82</v>
       </c>
       <c r="B85" s="4">
+        <f t="shared" si="10"/>
+        <v>66100</v>
+      </c>
+      <c r="C85" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D85" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E85" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F85" s="11">
         <f t="shared" si="7"/>
-        <v>66100</v>
-      </c>
-      <c r="C85" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D85" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E85" s="11">
-        <f t="shared" si="4"/>
         <v>8.402423469387756</v>
       </c>
-      <c r="F85" s="11">
-        <f t="shared" si="6"/>
+      <c r="G85" s="11">
+        <f t="shared" si="8"/>
         <v>17.376439975772879</v>
       </c>
-      <c r="G85" s="11">
+      <c r="H85" s="11">
         <v>3.4752879951545759</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A86" s="5">
         <v>83</v>
       </c>
       <c r="B86" s="4">
+        <f t="shared" si="10"/>
+        <v>67737</v>
+      </c>
+      <c r="C86" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D86" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E86" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F86" s="11">
         <f t="shared" si="7"/>
-        <v>67737</v>
-      </c>
-      <c r="C86" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D86" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E86" s="11">
-        <f t="shared" si="4"/>
         <v>8.4917091836734695</v>
       </c>
-      <c r="F86" s="11">
-        <f t="shared" si="6"/>
+      <c r="G86" s="11">
+        <f t="shared" si="8"/>
         <v>17.477683252060292</v>
       </c>
-      <c r="G86" s="11">
+      <c r="H86" s="11">
         <v>3.4955366504120584</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A87" s="5">
         <v>84</v>
       </c>
       <c r="B87" s="4">
+        <f t="shared" si="10"/>
+        <v>69393</v>
+      </c>
+      <c r="C87" s="5">
+        <v>999999</v>
+      </c>
+      <c r="D87" s="5">
+        <v>999999999</v>
+      </c>
+      <c r="E87" s="5">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F87" s="11">
         <f t="shared" si="7"/>
-        <v>69393</v>
-      </c>
-      <c r="C87" s="5">
-        <v>999999</v>
-      </c>
-      <c r="D87" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E87" s="11">
-        <f t="shared" si="4"/>
         <v>8.5809948979591848</v>
       </c>
-      <c r="F87" s="11">
-        <f t="shared" si="6"/>
+      <c r="G87" s="11">
+        <f t="shared" si="8"/>
         <v>17.578456710130649</v>
       </c>
-      <c r="G87" s="11">
+      <c r="H87" s="11">
         <v>3.5156913420261295</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A88" s="5">
         <v>85</v>
       </c>
       <c r="B88" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>71070</v>
       </c>
       <c r="C88" s="5">
         <v>999999</v>
       </c>
       <c r="D88" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E88" s="5">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="E88" s="11">
-        <f t="shared" si="4"/>
+      <c r="F88" s="11">
+        <f t="shared" ref="F88:F102" si="11">3.3+(A88-21)*0.1-F87*0.12</f>
         <v>8.6702806122448965</v>
       </c>
-      <c r="F88" s="11">
-        <f t="shared" si="6"/>
+      <c r="G88" s="11">
+        <f t="shared" si="8"/>
         <v>17.678767893256996</v>
       </c>
-      <c r="G88" s="11">
+      <c r="H88" s="11">
         <v>3.5357535786513994</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" s="5">
         <v>86</v>
       </c>
       <c r="B89" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>72767</v>
       </c>
       <c r="C89" s="5">
         <v>999999</v>
       </c>
       <c r="D89" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E89" s="5">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="E89" s="11">
-        <f t="shared" ref="E89:E102" si="8">3.3+(A89-21)*0.1-E88*0.12</f>
+      <c r="F89" s="11">
+        <f t="shared" si="11"/>
         <v>8.7595663265306136</v>
       </c>
-      <c r="F89" s="11">
-        <f t="shared" si="6"/>
+      <c r="G89" s="11">
+        <f t="shared" si="8"/>
         <v>17.778624139441146</v>
       </c>
-      <c r="G89" s="11">
+      <c r="H89" s="11">
         <v>3.5557248278882292</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" s="5">
         <v>87</v>
       </c>
       <c r="B90" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>74483</v>
       </c>
       <c r="C90" s="5">
         <v>999999</v>
       </c>
       <c r="D90" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E90" s="5">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="E90" s="11">
+      <c r="F90" s="11">
+        <f t="shared" si="11"/>
+        <v>8.8488520408163271</v>
+      </c>
+      <c r="G90" s="11">
         <f t="shared" si="8"/>
-        <v>8.8488520408163271</v>
-      </c>
-      <c r="F90" s="11">
-        <f t="shared" si="6"/>
         <v>17.878032589238494</v>
       </c>
-      <c r="G90" s="11">
+      <c r="H90" s="11">
         <v>3.5756065178476986</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" s="5">
         <v>88</v>
       </c>
       <c r="B91" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>76220</v>
       </c>
       <c r="C91" s="5">
         <v>999999</v>
       </c>
       <c r="D91" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E91" s="5">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="E91" s="11">
+      <c r="F91" s="11">
+        <f t="shared" si="11"/>
+        <v>8.9381377551020407</v>
+      </c>
+      <c r="G91" s="11">
         <f t="shared" si="8"/>
-        <v>8.9381377551020407</v>
-      </c>
-      <c r="F91" s="11">
-        <f t="shared" si="6"/>
         <v>17.977000193201071</v>
       </c>
-      <c r="G91" s="11">
+      <c r="H91" s="11">
         <v>3.5954000386402143</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" s="5">
         <v>89</v>
       </c>
       <c r="B92" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>77977</v>
       </c>
       <c r="C92" s="5">
         <v>999999</v>
       </c>
       <c r="D92" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E92" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E92" s="11">
+      <c r="F92" s="11">
+        <f t="shared" si="11"/>
+        <v>9.027423469387756</v>
+      </c>
+      <c r="G92" s="11">
         <f t="shared" si="8"/>
-        <v>9.027423469387756</v>
-      </c>
-      <c r="F92" s="11">
-        <f t="shared" si="6"/>
         <v>18.075533718961573</v>
       </c>
-      <c r="G92" s="11">
+      <c r="H92" s="11">
         <v>3.6151067437923148</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" s="5">
         <v>90</v>
       </c>
       <c r="B93" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>79753</v>
       </c>
       <c r="C93" s="5">
         <v>999999</v>
       </c>
       <c r="D93" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E93" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E93" s="11">
+      <c r="F93" s="11">
+        <f t="shared" si="11"/>
+        <v>9.1167091836734677</v>
+      </c>
+      <c r="G93" s="11">
         <f t="shared" si="8"/>
-        <v>9.1167091836734677</v>
-      </c>
-      <c r="F93" s="11">
-        <f t="shared" si="6"/>
         <v>18.173639757979167</v>
       </c>
-      <c r="G93" s="11">
+      <c r="H93" s="11">
         <v>3.6347279515958335</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="5">
         <v>91</v>
       </c>
       <c r="B94" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>81550</v>
       </c>
       <c r="C94" s="5">
         <v>999999</v>
       </c>
       <c r="D94" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E94" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E94" s="11">
+      <c r="F94" s="11">
+        <f t="shared" si="11"/>
+        <v>9.2059948979591848</v>
+      </c>
+      <c r="G94" s="11">
         <f t="shared" si="8"/>
-        <v>9.2059948979591848</v>
-      </c>
-      <c r="F94" s="11">
-        <f t="shared" si="6"/>
         <v>18.271324731966914</v>
       </c>
-      <c r="G94" s="11">
+      <c r="H94" s="11">
         <v>3.6542649463933827</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A95" s="5">
         <v>92</v>
       </c>
       <c r="B95" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>83367</v>
       </c>
       <c r="C95" s="5">
         <v>999999</v>
       </c>
       <c r="D95" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E95" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E95" s="11">
+      <c r="F95" s="11">
+        <f t="shared" si="11"/>
+        <v>9.2952806122448983</v>
+      </c>
+      <c r="G95" s="11">
         <f t="shared" si="8"/>
-        <v>9.2952806122448983</v>
-      </c>
-      <c r="F95" s="11">
-        <f t="shared" si="6"/>
         <v>18.368594899018895</v>
       </c>
-      <c r="G95" s="11">
+      <c r="H95" s="11">
         <v>3.673718979803779</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A96" s="5">
         <v>93</v>
       </c>
       <c r="B96" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>85203</v>
       </c>
       <c r="C96" s="5">
         <v>999999</v>
       </c>
       <c r="D96" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E96" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E96" s="11">
+      <c r="F96" s="11">
+        <f t="shared" si="11"/>
+        <v>9.3845663265306118</v>
+      </c>
+      <c r="G96" s="11">
         <f t="shared" si="8"/>
-        <v>9.3845663265306118</v>
-      </c>
-      <c r="F96" s="11">
-        <f t="shared" si="6"/>
         <v>18.465456359454102</v>
       </c>
-      <c r="G96" s="11">
+      <c r="H96" s="11">
         <v>3.6930912718908204</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A97" s="5">
         <v>94</v>
       </c>
       <c r="B97" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>87060</v>
       </c>
       <c r="C97" s="5">
         <v>999999</v>
       </c>
       <c r="D97" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E97" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E97" s="11">
+      <c r="F97" s="11">
+        <f t="shared" si="11"/>
+        <v>9.4738520408163289</v>
+      </c>
+      <c r="G97" s="11">
         <f t="shared" si="8"/>
-        <v>9.4738520408163289</v>
-      </c>
-      <c r="F97" s="11">
-        <f t="shared" si="6"/>
         <v>18.561915061393066</v>
       </c>
-      <c r="G97" s="11">
+      <c r="H97" s="11">
         <v>3.7123830122786132</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A98" s="5">
         <v>95</v>
       </c>
       <c r="B98" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>88937</v>
       </c>
       <c r="C98" s="5">
         <v>999999</v>
       </c>
       <c r="D98" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E98" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E98" s="11">
+      <c r="F98" s="11">
+        <f t="shared" si="11"/>
+        <v>9.5631377551020407</v>
+      </c>
+      <c r="G98" s="11">
         <f t="shared" si="8"/>
-        <v>9.5631377551020407</v>
-      </c>
-      <c r="F98" s="11">
-        <f t="shared" si="6"/>
         <v>18.657976806082026</v>
       </c>
-      <c r="G98" s="11">
+      <c r="H98" s="11">
         <v>3.7315953612164052</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A99" s="5">
         <v>96</v>
       </c>
       <c r="B99" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>90833</v>
       </c>
       <c r="C99" s="5">
         <v>999999</v>
       </c>
       <c r="D99" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E99" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E99" s="11">
+      <c r="F99" s="11">
+        <f t="shared" si="11"/>
+        <v>9.652423469387756</v>
+      </c>
+      <c r="G99" s="11">
         <f t="shared" si="8"/>
-        <v>9.652423469387756</v>
-      </c>
-      <c r="F99" s="11">
-        <f t="shared" si="6"/>
         <v>18.75364725297846</v>
       </c>
-      <c r="G99" s="11">
+      <c r="H99" s="11">
         <v>3.7507294505956921</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="5">
         <v>97</v>
       </c>
       <c r="B100" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>92750</v>
       </c>
       <c r="C100" s="5">
         <v>999999</v>
       </c>
       <c r="D100" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E100" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E100" s="11">
+      <c r="F100" s="11">
+        <f t="shared" si="11"/>
+        <v>9.7417091836734695</v>
+      </c>
+      <c r="G100" s="11">
         <f t="shared" si="8"/>
-        <v>9.7417091836734695</v>
-      </c>
-      <c r="F100" s="11">
-        <f t="shared" si="6"/>
         <v>18.848931924611136</v>
       </c>
-      <c r="G100" s="11">
+      <c r="H100" s="11">
         <v>3.7697863849222273</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="5">
         <v>98</v>
       </c>
       <c r="B101" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>94687</v>
       </c>
       <c r="C101" s="5">
         <v>999999</v>
       </c>
       <c r="D101" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E101" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E101" s="11">
+      <c r="F101" s="11">
+        <f t="shared" si="11"/>
+        <v>9.830994897959183</v>
+      </c>
+      <c r="G101" s="11">
         <f t="shared" si="8"/>
-        <v>9.830994897959183</v>
-      </c>
-      <c r="F101" s="11">
-        <f t="shared" si="6"/>
         <v>18.9438362112266</v>
       </c>
-      <c r="G101" s="11">
+      <c r="H101" s="11">
         <v>3.7887672422453198</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A102" s="5">
         <v>99</v>
       </c>
       <c r="B102" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>96643</v>
       </c>
       <c r="C102" s="5">
         <v>999999</v>
       </c>
       <c r="D102" s="5">
-        <f t="shared" si="5"/>
+        <v>999999999</v>
+      </c>
+      <c r="E102" s="5">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="E102" s="11">
+      <c r="F102" s="11">
+        <f t="shared" si="11"/>
+        <v>9.9202806122449001</v>
+      </c>
+      <c r="G102" s="11">
         <f t="shared" si="8"/>
-        <v>9.9202806122449001</v>
-      </c>
-      <c r="F102" s="11">
-        <f t="shared" si="6"/>
         <v>19.038365375233763</v>
       </c>
-      <c r="G102" s="11">
+      <c r="H102" s="11">
         <v>3.8076730750467527</v>
       </c>
     </row>

</xml_diff>